<commit_message>
Improve OCR credentials handling and accumulation exports
</commit_message>
<xml_diff>
--- a/app/Data/accumulation/Aichi_Accumulated.xlsx
+++ b/app/Data/accumulation/Aichi_Accumulated.xlsx
@@ -1,105 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Business Office</t>
-  </si>
-  <si>
-    <t>Order Number</t>
-  </si>
-  <si>
-    <t>Invoice Number</t>
-  </si>
-  <si>
-    <t>Order Date</t>
-  </si>
-  <si>
-    <t>Client Name</t>
-  </si>
-  <si>
-    <t>Item Description</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Tax Category</t>
-  </si>
-  <si>
-    <t>Account Title</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>Tax Amount</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Responsible Person</t>
-  </si>
-  <si>
-    <t>Operator Full Name</t>
-  </si>
-  <si>
-    <t>Operator Email</t>
-  </si>
-  <si>
-    <t>Operator Employee ID</t>
-  </si>
-  <si>
-    <t>Processed Timestamp</t>
-  </si>
-  <si>
-    <t>Source File</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -114,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -430,76 +420,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Business Office</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Order Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Invoice Number</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Order Date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Store Name</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Item Description</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Tax Category</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Account Title</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Subtotal</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Tax Amount</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Responsible Person</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Operator Full Name</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Operator Email</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Operator Employee ID</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Processed Timestamp</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Source File</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Aichi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>T1010001112577</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>T1010001112577</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-12-02</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[証紙切手引受]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>標準税率</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>JPY</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>eshwarpotnuru35@gmail.com</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>eshwarpotnuru35@gmail.com</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>2025-11-18T04:01:18Z</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>720be3bc-4088-4acc-8c42-ca827e079cd9</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Big Update - 5.5
</commit_message>
<xml_diff>
--- a/app/Data/accumulation/Aichi_Accumulated.xlsx
+++ b/app/Data/accumulation/Aichi_Accumulated.xlsx
@@ -20,13 +20,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年12月" sheetId="15" state="visible" r:id="rId15"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="集計ﾃｰﾌﾞﾙ" sheetId="16" state="hidden" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024年11月" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年07月" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_4" localSheetId="3">'追加1'!$A$1:$H$39</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="0" r:id="rId18"/>
+    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="0" r:id="rId19"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -20692,51 +20693,3066 @@
       </c>
     </row>
     <row r="45" ht="18" customHeight="1" s="115">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="0" t="inlineStr">
         <is>
           <t>2024-11-20</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr">
+      <c r="B45" s="0" t="inlineStr"/>
+      <c r="C45" s="0" t="inlineStr">
         <is>
           <t>Final Test Store</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D45" s="0" t="inlineStr">
         <is>
           <t>Ethan Cole</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="n">
+      <c r="E45" s="0" t="inlineStr"/>
+      <c r="F45" s="0" t="n">
         <v>2500</v>
       </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr">
+      <c r="G45" s="0" t="inlineStr"/>
+      <c r="H45" s="0" t="inlineStr">
         <is>
           <t>FINAL-TEST-1763562003</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="n">
+      <c r="I45" s="0" t="inlineStr"/>
+      <c r="J45" s="0" t="inlineStr"/>
+      <c r="K45" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="L45" t="inlineStr"/>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="n">
+      <c r="L45" s="0" t="inlineStr"/>
+      <c r="M45" s="0" t="inlineStr"/>
+      <c r="N45" s="0" t="n">
         <v>2500</v>
       </c>
-      <c r="O45" t="inlineStr"/>
-      <c r="P45" t="n">
+      <c r="O45" s="0" t="inlineStr"/>
+      <c r="P45" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="n">
+      <c r="Q45" s="0" t="inlineStr"/>
+      <c r="R45" s="0" t="n">
         <v>250</v>
       </c>
     </row>
+    <row r="46" ht="18" customHeight="1" s="115"/>
+    <row r="47" ht="18" customHeight="1" s="115"/>
+    <row r="48" ht="18" customHeight="1" s="115"/>
+    <row r="49" ht="18" customHeight="1" s="115"/>
+    <row r="50" ht="18" customHeight="1" s="115"/>
+    <row r="51" ht="18" customHeight="1" s="115"/>
+    <row r="52" ht="18" customHeight="1" s="115"/>
+    <row r="53" ht="18" customHeight="1" s="115"/>
+    <row r="54" ht="18" customHeight="1" s="115"/>
+    <row r="55" ht="18" customHeight="1" s="115"/>
+    <row r="56" ht="18" customHeight="1" s="115"/>
+    <row r="57" ht="18" customHeight="1" s="115"/>
+    <row r="58" ht="18" customHeight="1" s="115"/>
+    <row r="59" ht="18" customHeight="1" s="115"/>
+    <row r="60" ht="18" customHeight="1" s="115"/>
+    <row r="61" ht="18" customHeight="1" s="115"/>
+    <row r="62" ht="18" customHeight="1" s="115"/>
+    <row r="63" ht="18" customHeight="1" s="115"/>
+    <row r="64" ht="18" customHeight="1" s="115"/>
+    <row r="65" ht="18" customHeight="1" s="115"/>
+    <row r="66" ht="18" customHeight="1" s="115"/>
+    <row r="67" ht="18" customHeight="1" s="115"/>
+    <row r="68" ht="18" customHeight="1" s="115"/>
+    <row r="69" ht="18" customHeight="1" s="115"/>
+    <row r="70" ht="18" customHeight="1" s="115"/>
+    <row r="71" ht="18" customHeight="1" s="115"/>
+    <row r="72" ht="18" customHeight="1" s="115"/>
+    <row r="73" ht="18" customHeight="1" s="115"/>
+    <row r="74" ht="18" customHeight="1" s="115"/>
+    <row r="75" ht="18" customHeight="1" s="115"/>
+    <row r="76" ht="18" customHeight="1" s="115"/>
+    <row r="77" ht="18" customHeight="1" s="115"/>
+    <row r="78" ht="18" customHeight="1" s="115"/>
+    <row r="79" ht="18" customHeight="1" s="115"/>
+    <row r="80" ht="18" customHeight="1" s="115"/>
+    <row r="81" ht="18" customHeight="1" s="115"/>
+    <row r="82" ht="18" customHeight="1" s="115"/>
+    <row r="83" ht="18" customHeight="1" s="115"/>
+    <row r="84" ht="18" customHeight="1" s="115"/>
+    <row r="85" ht="18" customHeight="1" s="115"/>
+    <row r="86" ht="18" customHeight="1" s="115"/>
+    <row r="87" ht="18" customHeight="1" s="115"/>
+    <row r="88" ht="18" customHeight="1" s="115"/>
+    <row r="89" ht="18" customHeight="1" s="115"/>
+    <row r="90" ht="18" customHeight="1" s="115"/>
+    <row r="91" ht="18" customHeight="1" s="115"/>
+    <row r="92" ht="18" customHeight="1" s="115"/>
+    <row r="93" ht="18" customHeight="1" s="115"/>
+    <row r="94" ht="18" customHeight="1" s="115"/>
+    <row r="95" ht="18" customHeight="1" s="115"/>
+    <row r="96" ht="18" customHeight="1" s="115"/>
+    <row r="97" ht="18" customHeight="1" s="115"/>
+    <row r="98" ht="18" customHeight="1" s="115"/>
+    <row r="99" ht="18" customHeight="1" s="115"/>
+    <row r="100" ht="18" customHeight="1" s="115"/>
+    <row r="101" ht="18" customHeight="1" s="115"/>
+    <row r="102" ht="18" customHeight="1" s="115"/>
+    <row r="103" ht="18" customHeight="1" s="115"/>
+    <row r="104" ht="18" customHeight="1" s="115"/>
+    <row r="105" ht="18" customHeight="1" s="115"/>
+    <row r="106" ht="18" customHeight="1" s="115"/>
+    <row r="107" ht="18" customHeight="1" s="115"/>
+    <row r="108" ht="18" customHeight="1" s="115"/>
+    <row r="109" ht="18" customHeight="1" s="115"/>
+    <row r="110" ht="18" customHeight="1" s="115"/>
+    <row r="111" ht="18" customHeight="1" s="115"/>
+    <row r="112" ht="18" customHeight="1" s="115"/>
+    <row r="113" ht="18" customHeight="1" s="115"/>
+    <row r="114" ht="18" customHeight="1" s="115"/>
+    <row r="115" ht="18" customHeight="1" s="115"/>
+    <row r="116" ht="18" customHeight="1" s="115"/>
+    <row r="117" ht="18" customHeight="1" s="115"/>
+    <row r="118" ht="18" customHeight="1" s="115"/>
+    <row r="119" ht="18" customHeight="1" s="115"/>
+    <row r="120" ht="18" customHeight="1" s="115"/>
+    <row r="121" ht="18" customHeight="1" s="115"/>
+    <row r="122" ht="18" customHeight="1" s="115"/>
+    <row r="123" ht="18" customHeight="1" s="115"/>
+    <row r="124" ht="18" customHeight="1" s="115"/>
+    <row r="125" ht="18" customHeight="1" s="115"/>
+    <row r="126" ht="18" customHeight="1" s="115"/>
+    <row r="127" ht="18" customHeight="1" s="115"/>
+    <row r="128" ht="18" customHeight="1" s="115"/>
+    <row r="129" ht="18" customHeight="1" s="115"/>
+    <row r="130" ht="18" customHeight="1" s="115"/>
+    <row r="131" ht="18" customHeight="1" s="115"/>
+    <row r="132" ht="18" customHeight="1" s="115"/>
+    <row r="133" ht="18" customHeight="1" s="115"/>
+    <row r="134" ht="18" customHeight="1" s="115"/>
+    <row r="135" ht="18" customHeight="1" s="115"/>
+    <row r="136" ht="18" customHeight="1" s="115"/>
+    <row r="137" ht="18" customHeight="1" s="115"/>
+    <row r="138" ht="18" customHeight="1" s="115"/>
+    <row r="139" ht="18" customHeight="1" s="115"/>
+    <row r="140" ht="18" customHeight="1" s="115"/>
+    <row r="141" ht="18" customHeight="1" s="115"/>
+    <row r="142" ht="18" customHeight="1" s="115"/>
+    <row r="143" ht="18" customHeight="1" s="115"/>
+    <row r="144" ht="18" customHeight="1" s="115"/>
+    <row r="145" ht="18" customHeight="1" s="115"/>
+    <row r="146" ht="18" customHeight="1" s="115"/>
+    <row r="147" ht="18" customHeight="1" s="115"/>
+    <row r="148" ht="18" customHeight="1" s="115"/>
+    <row r="149" ht="18" customHeight="1" s="115"/>
+    <row r="150" ht="18" customHeight="1" s="115"/>
+    <row r="151" ht="18" customHeight="1" s="115"/>
+    <row r="152" ht="18" customHeight="1" s="115"/>
+    <row r="153" ht="18" customHeight="1" s="115"/>
+    <row r="154" ht="18" customHeight="1" s="115"/>
+    <row r="155" ht="18" customHeight="1" s="115"/>
+    <row r="156" ht="18" customHeight="1" s="115"/>
+    <row r="157" ht="18" customHeight="1" s="115"/>
+    <row r="158" ht="18" customHeight="1" s="115"/>
+    <row r="159" ht="18" customHeight="1" s="115"/>
+    <row r="160" ht="18" customHeight="1" s="115"/>
+    <row r="161" ht="18" customHeight="1" s="115"/>
+    <row r="162" ht="18" customHeight="1" s="115"/>
+    <row r="163" ht="18" customHeight="1" s="115"/>
+    <row r="164" ht="18" customHeight="1" s="115"/>
+    <row r="165" ht="18" customHeight="1" s="115"/>
+    <row r="166" ht="18" customHeight="1" s="115"/>
+    <row r="167" ht="18" customHeight="1" s="115"/>
+    <row r="168" ht="18" customHeight="1" s="115"/>
+    <row r="169" ht="18" customHeight="1" s="115"/>
+    <row r="170" ht="18" customHeight="1" s="115"/>
+    <row r="171" ht="18" customHeight="1" s="115"/>
+    <row r="172" ht="18" customHeight="1" s="115"/>
+    <row r="173" ht="18" customHeight="1" s="115"/>
+    <row r="174" ht="18" customHeight="1" s="115"/>
+    <row r="175" ht="18" customHeight="1" s="115"/>
+    <row r="176" ht="18" customHeight="1" s="115"/>
+    <row r="177" ht="18" customHeight="1" s="115"/>
+    <row r="178" ht="18" customHeight="1" s="115"/>
+    <row r="179" ht="18" customHeight="1" s="115"/>
+    <row r="180" ht="18" customHeight="1" s="115"/>
+    <row r="181" ht="18" customHeight="1" s="115"/>
+    <row r="182" ht="18" customHeight="1" s="115"/>
+    <row r="183" ht="18" customHeight="1" s="115"/>
+    <row r="184" ht="18" customHeight="1" s="115"/>
+    <row r="185" ht="18" customHeight="1" s="115"/>
+    <row r="186" ht="18" customHeight="1" s="115"/>
+    <row r="187" ht="18" customHeight="1" s="115"/>
+    <row r="188" ht="18" customHeight="1" s="115"/>
+    <row r="189" ht="18" customHeight="1" s="115"/>
+    <row r="190" ht="18" customHeight="1" s="115"/>
+    <row r="191" ht="18" customHeight="1" s="115"/>
+    <row r="192" ht="18" customHeight="1" s="115"/>
+    <row r="193" ht="18" customHeight="1" s="115"/>
+    <row r="194" ht="18" customHeight="1" s="115"/>
+    <row r="195" ht="18" customHeight="1" s="115"/>
+    <row r="196" ht="18" customHeight="1" s="115"/>
+    <row r="197" ht="18" customHeight="1" s="115"/>
+    <row r="198" ht="18" customHeight="1" s="115"/>
+    <row r="199" ht="18" customHeight="1" s="115"/>
+    <row r="200" ht="18" customHeight="1" s="115"/>
+    <row r="201" ht="18" customHeight="1" s="115"/>
+    <row r="202" ht="18" customHeight="1" s="115"/>
+    <row r="203" ht="18" customHeight="1" s="115"/>
+    <row r="204" ht="18" customHeight="1" s="115"/>
+    <row r="205" ht="18" customHeight="1" s="115"/>
+    <row r="206" ht="18" customHeight="1" s="115"/>
+    <row r="207" ht="18" customHeight="1" s="115"/>
+    <row r="208" ht="18" customHeight="1" s="115"/>
+    <row r="209" ht="18" customHeight="1" s="115"/>
+    <row r="210" ht="18" customHeight="1" s="115"/>
+    <row r="211" ht="18" customHeight="1" s="115"/>
+    <row r="212" ht="18" customHeight="1" s="115"/>
+    <row r="213" ht="18" customHeight="1" s="115"/>
+    <row r="214" ht="18" customHeight="1" s="115"/>
+    <row r="215" ht="18" customHeight="1" s="115"/>
+    <row r="216" ht="18" customHeight="1" s="115"/>
+    <row r="217" ht="18" customHeight="1" s="115"/>
+    <row r="218" ht="18" customHeight="1" s="115"/>
+    <row r="219" ht="18" customHeight="1" s="115"/>
+    <row r="220" ht="18" customHeight="1" s="115"/>
+    <row r="221" ht="18" customHeight="1" s="115"/>
+    <row r="222" ht="18" customHeight="1" s="115"/>
+    <row r="223" ht="18" customHeight="1" s="115"/>
+    <row r="224" ht="18" customHeight="1" s="115"/>
+    <row r="225" ht="18" customHeight="1" s="115"/>
+    <row r="226" ht="18" customHeight="1" s="115"/>
+    <row r="227" ht="18" customHeight="1" s="115"/>
+    <row r="228" ht="18" customHeight="1" s="115"/>
+    <row r="229" ht="18" customHeight="1" s="115"/>
+    <row r="230" ht="18" customHeight="1" s="115"/>
+    <row r="231" ht="18" customHeight="1" s="115"/>
+    <row r="232" ht="18" customHeight="1" s="115"/>
+    <row r="233" ht="18" customHeight="1" s="115"/>
+    <row r="234" ht="18" customHeight="1" s="115"/>
+    <row r="235" ht="18" customHeight="1" s="115"/>
+    <row r="236" ht="18" customHeight="1" s="115"/>
+    <row r="237" ht="18" customHeight="1" s="115"/>
+    <row r="238" ht="18" customHeight="1" s="115"/>
+    <row r="239" ht="18" customHeight="1" s="115"/>
+    <row r="240" ht="18" customHeight="1" s="115"/>
+    <row r="241" ht="18" customHeight="1" s="115"/>
+    <row r="242" ht="18" customHeight="1" s="115"/>
+    <row r="243" ht="18" customHeight="1" s="115"/>
+    <row r="244" ht="18" customHeight="1" s="115"/>
+    <row r="245" ht="18" customHeight="1" s="115"/>
+    <row r="246" ht="18" customHeight="1" s="115"/>
+    <row r="247" ht="18" customHeight="1" s="115"/>
+    <row r="248" ht="18" customHeight="1" s="115"/>
+    <row r="249" ht="18" customHeight="1" s="115"/>
+    <row r="250" ht="18" customHeight="1" s="115"/>
+    <row r="251" ht="18" customHeight="1" s="115"/>
+    <row r="252" ht="18" customHeight="1" s="115"/>
+    <row r="253" ht="18" customHeight="1" s="115"/>
+    <row r="254" ht="18" customHeight="1" s="115"/>
+    <row r="255" ht="18" customHeight="1" s="115"/>
+    <row r="256" ht="18" customHeight="1" s="115"/>
+    <row r="257" ht="18" customHeight="1" s="115"/>
+    <row r="258" ht="18" customHeight="1" s="115"/>
+    <row r="259" ht="18" customHeight="1" s="115"/>
+    <row r="260" ht="18" customHeight="1" s="115"/>
+    <row r="261" ht="18" customHeight="1" s="115"/>
+    <row r="262" ht="18" customHeight="1" s="115"/>
+    <row r="263" ht="18" customHeight="1" s="115"/>
+    <row r="264" ht="18" customHeight="1" s="115"/>
+    <row r="265" ht="18" customHeight="1" s="115"/>
+    <row r="266" ht="18" customHeight="1" s="115"/>
+    <row r="267" ht="18" customHeight="1" s="115"/>
+    <row r="268" ht="18" customHeight="1" s="115"/>
+    <row r="269" ht="18" customHeight="1" s="115"/>
+    <row r="270" ht="18" customHeight="1" s="115"/>
+    <row r="271" ht="18" customHeight="1" s="115"/>
+    <row r="272" ht="18" customHeight="1" s="115"/>
+    <row r="273" ht="18" customHeight="1" s="115"/>
+    <row r="274" ht="18" customHeight="1" s="115"/>
+    <row r="275" ht="18" customHeight="1" s="115"/>
+    <row r="276" ht="18" customHeight="1" s="115"/>
+    <row r="277" ht="18" customHeight="1" s="115"/>
+    <row r="278" ht="18" customHeight="1" s="115"/>
+    <row r="279" ht="18" customHeight="1" s="115"/>
+    <row r="280" ht="18" customHeight="1" s="115"/>
+    <row r="281" ht="18" customHeight="1" s="115"/>
+    <row r="282" ht="18" customHeight="1" s="115"/>
+    <row r="283" ht="18" customHeight="1" s="115"/>
+    <row r="284" ht="18" customHeight="1" s="115"/>
+    <row r="285" ht="18" customHeight="1" s="115"/>
+    <row r="286" ht="18" customHeight="1" s="115"/>
+    <row r="287" ht="18" customHeight="1" s="115"/>
+    <row r="288" ht="18" customHeight="1" s="115"/>
+    <row r="289" ht="18" customHeight="1" s="115"/>
+    <row r="290" ht="18" customHeight="1" s="115"/>
+    <row r="291" ht="18" customHeight="1" s="115"/>
+    <row r="292" ht="18" customHeight="1" s="115"/>
+    <row r="293" ht="18" customHeight="1" s="115"/>
+    <row r="294" ht="18" customHeight="1" s="115"/>
+    <row r="295" ht="18" customHeight="1" s="115"/>
+    <row r="296" ht="18" customHeight="1" s="115"/>
+    <row r="297" ht="18" customHeight="1" s="115"/>
+    <row r="298" ht="18" customHeight="1" s="115"/>
+    <row r="299" ht="18" customHeight="1" s="115"/>
+    <row r="300" ht="18" customHeight="1" s="115"/>
+    <row r="301" ht="18" customHeight="1" s="115"/>
+    <row r="302" ht="18" customHeight="1" s="115"/>
+    <row r="303" ht="18" customHeight="1" s="115"/>
+    <row r="304" ht="18" customHeight="1" s="115"/>
+    <row r="305" ht="18" customHeight="1" s="115"/>
+    <row r="306" ht="18" customHeight="1" s="115"/>
+    <row r="307" ht="18" customHeight="1" s="115"/>
+    <row r="308" ht="18" customHeight="1" s="115"/>
+    <row r="309" ht="18" customHeight="1" s="115"/>
+    <row r="310" ht="18" customHeight="1" s="115"/>
+    <row r="311" ht="18" customHeight="1" s="115"/>
+    <row r="312" ht="18" customHeight="1" s="115"/>
+    <row r="313" ht="18" customHeight="1" s="115"/>
+    <row r="314" ht="18" customHeight="1" s="115"/>
+    <row r="315" ht="18" customHeight="1" s="115"/>
+    <row r="316" ht="18" customHeight="1" s="115"/>
+    <row r="317" ht="18" customHeight="1" s="115"/>
+    <row r="318" ht="18" customHeight="1" s="115"/>
+    <row r="319" ht="18" customHeight="1" s="115"/>
+    <row r="320" ht="18" customHeight="1" s="115"/>
+    <row r="321" ht="18" customHeight="1" s="115"/>
+    <row r="322" ht="18" customHeight="1" s="115"/>
+    <row r="323" ht="18" customHeight="1" s="115"/>
+    <row r="324" ht="18" customHeight="1" s="115"/>
+    <row r="325" ht="18" customHeight="1" s="115"/>
+    <row r="326" ht="18" customHeight="1" s="115"/>
+    <row r="327" ht="18" customHeight="1" s="115"/>
+    <row r="328" ht="18" customHeight="1" s="115"/>
+    <row r="329" ht="18" customHeight="1" s="115"/>
+    <row r="330" ht="18" customHeight="1" s="115"/>
+    <row r="331" ht="18" customHeight="1" s="115"/>
+    <row r="332" ht="18" customHeight="1" s="115"/>
+    <row r="333" ht="18" customHeight="1" s="115"/>
+    <row r="334" ht="18" customHeight="1" s="115"/>
+    <row r="335" ht="18" customHeight="1" s="115"/>
+    <row r="336" ht="18" customHeight="1" s="115"/>
+    <row r="337" ht="18" customHeight="1" s="115"/>
+    <row r="338" ht="18" customHeight="1" s="115"/>
+    <row r="339" ht="18" customHeight="1" s="115"/>
+    <row r="340" ht="18" customHeight="1" s="115"/>
+    <row r="341" ht="18" customHeight="1" s="115"/>
+    <row r="342" ht="18" customHeight="1" s="115"/>
+    <row r="343" ht="18" customHeight="1" s="115"/>
+    <row r="344" ht="18" customHeight="1" s="115"/>
+    <row r="345" ht="18" customHeight="1" s="115"/>
+    <row r="346" ht="18" customHeight="1" s="115"/>
+    <row r="347" ht="18" customHeight="1" s="115"/>
+    <row r="348" ht="18" customHeight="1" s="115"/>
+    <row r="349" ht="18" customHeight="1" s="115"/>
+    <row r="350" ht="18" customHeight="1" s="115"/>
+    <row r="351" ht="18" customHeight="1" s="115"/>
+    <row r="352" ht="18" customHeight="1" s="115"/>
+    <row r="353" ht="18" customHeight="1" s="115"/>
+    <row r="354" ht="18" customHeight="1" s="115"/>
+    <row r="355" ht="18" customHeight="1" s="115"/>
+    <row r="356" ht="18" customHeight="1" s="115"/>
+    <row r="357" ht="18" customHeight="1" s="115"/>
+    <row r="358" ht="18" customHeight="1" s="115"/>
+    <row r="359" ht="18" customHeight="1" s="115"/>
+    <row r="360" ht="18" customHeight="1" s="115"/>
+    <row r="361" ht="18" customHeight="1" s="115"/>
+    <row r="362" ht="18" customHeight="1" s="115"/>
+    <row r="363" ht="18" customHeight="1" s="115"/>
+    <row r="364" ht="18" customHeight="1" s="115"/>
+    <row r="365" ht="18" customHeight="1" s="115"/>
+    <row r="366" ht="18" customHeight="1" s="115"/>
+    <row r="367" ht="18" customHeight="1" s="115"/>
+    <row r="368" ht="18" customHeight="1" s="115"/>
+    <row r="369" ht="18" customHeight="1" s="115"/>
+    <row r="370" ht="18" customHeight="1" s="115"/>
+    <row r="371" ht="18" customHeight="1" s="115"/>
+    <row r="372" ht="18" customHeight="1" s="115"/>
+    <row r="373" ht="18" customHeight="1" s="115"/>
+    <row r="374" ht="18" customHeight="1" s="115"/>
+    <row r="375" ht="18" customHeight="1" s="115"/>
+    <row r="376" ht="18" customHeight="1" s="115"/>
+    <row r="377" ht="18" customHeight="1" s="115"/>
+    <row r="378" ht="18" customHeight="1" s="115"/>
+    <row r="379" ht="18" customHeight="1" s="115"/>
+    <row r="380" ht="18" customHeight="1" s="115"/>
+    <row r="381" ht="18" customHeight="1" s="115"/>
+    <row r="382" ht="18" customHeight="1" s="115"/>
+    <row r="383" ht="18" customHeight="1" s="115"/>
+    <row r="384" ht="18" customHeight="1" s="115"/>
+    <row r="385" ht="18" customHeight="1" s="115"/>
+    <row r="386" ht="18" customHeight="1" s="115"/>
+    <row r="387" ht="18" customHeight="1" s="115"/>
+    <row r="388" ht="18" customHeight="1" s="115"/>
+    <row r="389" ht="18" customHeight="1" s="115"/>
+    <row r="390" ht="18" customHeight="1" s="115"/>
+    <row r="391" ht="18" customHeight="1" s="115"/>
+    <row r="392" ht="18" customHeight="1" s="115"/>
+    <row r="393" ht="18" customHeight="1" s="115"/>
+    <row r="394" ht="18" customHeight="1" s="115"/>
+    <row r="395" ht="18" customHeight="1" s="115"/>
+    <row r="396" ht="18" customHeight="1" s="115"/>
+    <row r="397" ht="18" customHeight="1" s="115"/>
+    <row r="398" ht="18" customHeight="1" s="115"/>
+    <row r="399" ht="18" customHeight="1" s="115"/>
+    <row r="400" ht="18" customHeight="1" s="115"/>
+    <row r="401" ht="18" customHeight="1" s="115"/>
+    <row r="402" ht="18" customHeight="1" s="115"/>
+    <row r="403" ht="18" customHeight="1" s="115"/>
+    <row r="404" ht="18" customHeight="1" s="115"/>
+    <row r="405" ht="18" customHeight="1" s="115"/>
+    <row r="406" ht="18" customHeight="1" s="115"/>
+    <row r="407" ht="18" customHeight="1" s="115"/>
+    <row r="408" ht="18" customHeight="1" s="115"/>
+    <row r="409" ht="18" customHeight="1" s="115"/>
+    <row r="410" ht="18" customHeight="1" s="115"/>
+    <row r="411" ht="18" customHeight="1" s="115"/>
+    <row r="412" ht="18" customHeight="1" s="115"/>
+    <row r="413" ht="18" customHeight="1" s="115"/>
+    <row r="414" ht="18" customHeight="1" s="115"/>
+    <row r="415" ht="18" customHeight="1" s="115"/>
+    <row r="416" ht="18" customHeight="1" s="115"/>
+    <row r="417" ht="18" customHeight="1" s="115"/>
+    <row r="418" ht="18" customHeight="1" s="115"/>
+    <row r="419" ht="18" customHeight="1" s="115"/>
+    <row r="420" ht="18" customHeight="1" s="115"/>
+    <row r="421" ht="18" customHeight="1" s="115"/>
+    <row r="422" ht="18" customHeight="1" s="115"/>
+    <row r="423" ht="18" customHeight="1" s="115"/>
+    <row r="424" ht="18" customHeight="1" s="115"/>
+    <row r="425" ht="18" customHeight="1" s="115"/>
+    <row r="426" ht="18" customHeight="1" s="115"/>
+    <row r="427" ht="18" customHeight="1" s="115"/>
+    <row r="428" ht="18" customHeight="1" s="115"/>
+    <row r="429" ht="18" customHeight="1" s="115"/>
+    <row r="430" ht="18" customHeight="1" s="115"/>
+    <row r="431" ht="18" customHeight="1" s="115"/>
+    <row r="432" ht="18" customHeight="1" s="115"/>
+    <row r="433" ht="18" customHeight="1" s="115"/>
+    <row r="434" ht="18" customHeight="1" s="115"/>
+    <row r="435" ht="18" customHeight="1" s="115"/>
+    <row r="436" ht="18" customHeight="1" s="115"/>
+    <row r="437" ht="18" customHeight="1" s="115"/>
+    <row r="438" ht="18" customHeight="1" s="115"/>
+    <row r="439" ht="18" customHeight="1" s="115"/>
+    <row r="440" ht="18" customHeight="1" s="115"/>
+    <row r="441" ht="18" customHeight="1" s="115"/>
+    <row r="442" ht="18" customHeight="1" s="115"/>
+    <row r="443" ht="18" customHeight="1" s="115"/>
+    <row r="444" ht="18" customHeight="1" s="115"/>
+    <row r="445" ht="18" customHeight="1" s="115"/>
+    <row r="446" ht="18" customHeight="1" s="115"/>
+    <row r="447" ht="18" customHeight="1" s="115"/>
+    <row r="448" ht="18" customHeight="1" s="115"/>
+    <row r="449" ht="18" customHeight="1" s="115"/>
+    <row r="450" ht="18" customHeight="1" s="115"/>
+    <row r="451" ht="18" customHeight="1" s="115"/>
+    <row r="452" ht="18" customHeight="1" s="115"/>
+    <row r="453" ht="18" customHeight="1" s="115"/>
+    <row r="454" ht="18" customHeight="1" s="115"/>
+    <row r="455" ht="18" customHeight="1" s="115"/>
+    <row r="456" ht="18" customHeight="1" s="115"/>
+    <row r="457" ht="18" customHeight="1" s="115"/>
+    <row r="458" ht="18" customHeight="1" s="115"/>
+    <row r="459" ht="18" customHeight="1" s="115"/>
+    <row r="460" ht="18" customHeight="1" s="115"/>
+    <row r="461" ht="18" customHeight="1" s="115"/>
+    <row r="462" ht="18" customHeight="1" s="115"/>
+    <row r="463" ht="18" customHeight="1" s="115"/>
+    <row r="464" ht="18" customHeight="1" s="115"/>
+    <row r="465" ht="18" customHeight="1" s="115"/>
+    <row r="466" ht="18" customHeight="1" s="115"/>
+    <row r="467" ht="18" customHeight="1" s="115"/>
+    <row r="468" ht="18" customHeight="1" s="115"/>
+    <row r="469" ht="18" customHeight="1" s="115"/>
+    <row r="470" ht="18" customHeight="1" s="115"/>
+    <row r="471" ht="18" customHeight="1" s="115"/>
+    <row r="472" ht="18" customHeight="1" s="115"/>
+    <row r="473" ht="18" customHeight="1" s="115"/>
+    <row r="474" ht="18" customHeight="1" s="115"/>
+    <row r="475" ht="18" customHeight="1" s="115"/>
+    <row r="476" ht="18" customHeight="1" s="115"/>
+    <row r="477" ht="18" customHeight="1" s="115"/>
+    <row r="478" ht="18" customHeight="1" s="115"/>
+    <row r="479" ht="18" customHeight="1" s="115"/>
+    <row r="480" ht="18" customHeight="1" s="115"/>
+    <row r="481" ht="18" customHeight="1" s="115"/>
+    <row r="482" ht="18" customHeight="1" s="115"/>
+    <row r="483" ht="18" customHeight="1" s="115"/>
+    <row r="484" ht="18" customHeight="1" s="115"/>
+    <row r="485" ht="18" customHeight="1" s="115"/>
+    <row r="486" ht="18" customHeight="1" s="115"/>
+    <row r="487" ht="18" customHeight="1" s="115"/>
+    <row r="488" ht="18" customHeight="1" s="115"/>
+    <row r="489" ht="18" customHeight="1" s="115"/>
+    <row r="490" ht="18" customHeight="1" s="115"/>
+    <row r="491" ht="18" customHeight="1" s="115"/>
+    <row r="492" ht="18" customHeight="1" s="115"/>
+    <row r="493" ht="18" customHeight="1" s="115"/>
+    <row r="494" ht="18" customHeight="1" s="115"/>
+    <row r="495" ht="18" customHeight="1" s="115"/>
+    <row r="496" ht="18" customHeight="1" s="115"/>
+    <row r="497" ht="18" customHeight="1" s="115"/>
+    <row r="498" ht="18" customHeight="1" s="115"/>
+    <row r="499" ht="18" customHeight="1" s="115"/>
+    <row r="500" ht="18" customHeight="1" s="115"/>
+    <row r="501" ht="18" customHeight="1" s="115"/>
+    <row r="502" ht="18" customHeight="1" s="115"/>
+    <row r="503" ht="18" customHeight="1" s="115"/>
+    <row r="504" ht="18" customHeight="1" s="115"/>
+    <row r="505" ht="18" customHeight="1" s="115"/>
+    <row r="506" ht="18" customHeight="1" s="115"/>
+    <row r="507" ht="18" customHeight="1" s="115"/>
+    <row r="508" ht="18" customHeight="1" s="115"/>
+    <row r="509" ht="18" customHeight="1" s="115"/>
+    <row r="510" ht="18" customHeight="1" s="115"/>
+    <row r="511" ht="18" customHeight="1" s="115"/>
+    <row r="512" ht="18" customHeight="1" s="115"/>
+    <row r="513" ht="18" customHeight="1" s="115"/>
+    <row r="514" ht="18" customHeight="1" s="115"/>
+    <row r="515" ht="18" customHeight="1" s="115"/>
+    <row r="516" ht="18" customHeight="1" s="115"/>
+    <row r="517" ht="18" customHeight="1" s="115"/>
+    <row r="518" ht="18" customHeight="1" s="115"/>
+    <row r="519" ht="18" customHeight="1" s="115"/>
+    <row r="520" ht="18" customHeight="1" s="115"/>
+    <row r="521" ht="18" customHeight="1" s="115"/>
+    <row r="522" ht="18" customHeight="1" s="115"/>
+    <row r="523" ht="18" customHeight="1" s="115"/>
+    <row r="524" ht="18" customHeight="1" s="115"/>
+    <row r="525" ht="18" customHeight="1" s="115"/>
+    <row r="526" ht="18" customHeight="1" s="115"/>
+    <row r="527" ht="18" customHeight="1" s="115"/>
+    <row r="528" ht="18" customHeight="1" s="115"/>
+    <row r="529" ht="18" customHeight="1" s="115"/>
+    <row r="530" ht="18" customHeight="1" s="115"/>
+    <row r="531" ht="18" customHeight="1" s="115"/>
+    <row r="532" ht="18" customHeight="1" s="115"/>
+    <row r="533" ht="18" customHeight="1" s="115"/>
+    <row r="534" ht="18" customHeight="1" s="115"/>
+    <row r="535" ht="18" customHeight="1" s="115"/>
+    <row r="536" ht="18" customHeight="1" s="115"/>
+    <row r="537" ht="18" customHeight="1" s="115"/>
+    <row r="538" ht="18" customHeight="1" s="115"/>
+    <row r="539" ht="18" customHeight="1" s="115"/>
+    <row r="540" ht="18" customHeight="1" s="115"/>
+    <row r="541" ht="18" customHeight="1" s="115"/>
+    <row r="542" ht="18" customHeight="1" s="115"/>
+    <row r="543" ht="18" customHeight="1" s="115"/>
+    <row r="544" ht="18" customHeight="1" s="115"/>
+    <row r="545" ht="18" customHeight="1" s="115"/>
+    <row r="546" ht="18" customHeight="1" s="115"/>
+    <row r="547" ht="18" customHeight="1" s="115"/>
+    <row r="548" ht="18" customHeight="1" s="115"/>
+    <row r="549" ht="18" customHeight="1" s="115"/>
+    <row r="550" ht="18" customHeight="1" s="115"/>
+    <row r="551" ht="18" customHeight="1" s="115"/>
+    <row r="552" ht="18" customHeight="1" s="115"/>
+    <row r="553" ht="18" customHeight="1" s="115"/>
+    <row r="554" ht="18" customHeight="1" s="115"/>
+    <row r="555" ht="18" customHeight="1" s="115"/>
+    <row r="556" ht="18" customHeight="1" s="115"/>
+    <row r="557" ht="18" customHeight="1" s="115"/>
+    <row r="558" ht="18" customHeight="1" s="115"/>
+    <row r="559" ht="18" customHeight="1" s="115"/>
+    <row r="560" ht="18" customHeight="1" s="115"/>
+    <row r="561" ht="18" customHeight="1" s="115"/>
+    <row r="562" ht="18" customHeight="1" s="115"/>
+    <row r="563" ht="18" customHeight="1" s="115"/>
+    <row r="564" ht="18" customHeight="1" s="115"/>
+    <row r="565" ht="18" customHeight="1" s="115"/>
+    <row r="566" ht="18" customHeight="1" s="115"/>
+    <row r="567" ht="18" customHeight="1" s="115"/>
+    <row r="568" ht="18" customHeight="1" s="115"/>
+    <row r="569" ht="18" customHeight="1" s="115"/>
+    <row r="570" ht="18" customHeight="1" s="115"/>
+    <row r="571" ht="18" customHeight="1" s="115"/>
+    <row r="572" ht="18" customHeight="1" s="115"/>
+    <row r="573" ht="18" customHeight="1" s="115"/>
+    <row r="574" ht="18" customHeight="1" s="115"/>
+    <row r="575" ht="18" customHeight="1" s="115"/>
+    <row r="576" ht="18" customHeight="1" s="115"/>
+    <row r="577" ht="18" customHeight="1" s="115"/>
+    <row r="578" ht="18" customHeight="1" s="115"/>
+    <row r="579" ht="18" customHeight="1" s="115"/>
+    <row r="580" ht="18" customHeight="1" s="115"/>
+    <row r="581" ht="18" customHeight="1" s="115"/>
+    <row r="582" ht="18" customHeight="1" s="115"/>
+    <row r="583" ht="18" customHeight="1" s="115"/>
+    <row r="584" ht="18" customHeight="1" s="115"/>
+    <row r="585" ht="18" customHeight="1" s="115"/>
+    <row r="586" ht="18" customHeight="1" s="115"/>
+    <row r="587" ht="18" customHeight="1" s="115"/>
+    <row r="588" ht="18" customHeight="1" s="115"/>
+    <row r="589" ht="18" customHeight="1" s="115"/>
+    <row r="590" ht="18" customHeight="1" s="115"/>
+    <row r="591" ht="18" customHeight="1" s="115"/>
+    <row r="592" ht="18" customHeight="1" s="115"/>
+    <row r="593" ht="18" customHeight="1" s="115"/>
+    <row r="594" ht="18" customHeight="1" s="115"/>
+    <row r="595" ht="18" customHeight="1" s="115"/>
+    <row r="596" ht="18" customHeight="1" s="115"/>
+    <row r="597" ht="18" customHeight="1" s="115"/>
+    <row r="598" ht="18" customHeight="1" s="115"/>
+    <row r="599" ht="18" customHeight="1" s="115"/>
+    <row r="600" ht="18" customHeight="1" s="115"/>
+    <row r="601" ht="18" customHeight="1" s="115"/>
+    <row r="602" ht="18" customHeight="1" s="115"/>
+    <row r="603" ht="18" customHeight="1" s="115"/>
+    <row r="604" ht="18" customHeight="1" s="115"/>
+    <row r="605" ht="18" customHeight="1" s="115"/>
+    <row r="606" ht="18" customHeight="1" s="115"/>
+    <row r="607" ht="18" customHeight="1" s="115"/>
+    <row r="608" ht="18" customHeight="1" s="115"/>
+    <row r="609" ht="18" customHeight="1" s="115"/>
+    <row r="610" ht="18" customHeight="1" s="115"/>
+    <row r="611" ht="18" customHeight="1" s="115"/>
+    <row r="612" ht="18" customHeight="1" s="115"/>
+    <row r="613" ht="18" customHeight="1" s="115"/>
+    <row r="614" ht="18" customHeight="1" s="115"/>
+    <row r="615" ht="18" customHeight="1" s="115"/>
+    <row r="616" ht="18" customHeight="1" s="115"/>
+    <row r="617" ht="18" customHeight="1" s="115"/>
+    <row r="618" ht="18" customHeight="1" s="115"/>
+    <row r="619" ht="18" customHeight="1" s="115"/>
+    <row r="620" ht="18" customHeight="1" s="115"/>
+    <row r="621" ht="18" customHeight="1" s="115"/>
+    <row r="622" ht="18" customHeight="1" s="115"/>
+    <row r="623" ht="18" customHeight="1" s="115"/>
+    <row r="624" ht="18" customHeight="1" s="115"/>
+    <row r="625" ht="18" customHeight="1" s="115"/>
+    <row r="626" ht="18" customHeight="1" s="115"/>
+    <row r="627" ht="18" customHeight="1" s="115"/>
+    <row r="628" ht="18" customHeight="1" s="115"/>
+    <row r="629" ht="18" customHeight="1" s="115"/>
+    <row r="630" ht="18" customHeight="1" s="115"/>
+    <row r="631" ht="18" customHeight="1" s="115"/>
+    <row r="632" ht="18" customHeight="1" s="115"/>
+    <row r="633" ht="18" customHeight="1" s="115"/>
+    <row r="634" ht="18" customHeight="1" s="115"/>
+    <row r="635" ht="18" customHeight="1" s="115"/>
+    <row r="636" ht="18" customHeight="1" s="115"/>
+    <row r="637" ht="18" customHeight="1" s="115"/>
+    <row r="638" ht="18" customHeight="1" s="115"/>
+    <row r="639" ht="18" customHeight="1" s="115"/>
+    <row r="640" ht="18" customHeight="1" s="115"/>
+    <row r="641" ht="18" customHeight="1" s="115"/>
+    <row r="642" ht="18" customHeight="1" s="115"/>
+    <row r="643" ht="18" customHeight="1" s="115"/>
+    <row r="644" ht="18" customHeight="1" s="115"/>
+    <row r="645" ht="18" customHeight="1" s="115"/>
+    <row r="646" ht="18" customHeight="1" s="115"/>
+    <row r="647" ht="18" customHeight="1" s="115"/>
+    <row r="648" ht="18" customHeight="1" s="115"/>
+    <row r="649" ht="18" customHeight="1" s="115"/>
+    <row r="650" ht="18" customHeight="1" s="115"/>
+    <row r="651" ht="18" customHeight="1" s="115"/>
+    <row r="652" ht="18" customHeight="1" s="115"/>
+    <row r="653" ht="18" customHeight="1" s="115"/>
+    <row r="654" ht="18" customHeight="1" s="115"/>
+    <row r="655" ht="18" customHeight="1" s="115"/>
+    <row r="656" ht="18" customHeight="1" s="115"/>
+    <row r="657" ht="18" customHeight="1" s="115"/>
+    <row r="658" ht="18" customHeight="1" s="115"/>
+    <row r="659" ht="18" customHeight="1" s="115"/>
+    <row r="660" ht="18" customHeight="1" s="115"/>
+    <row r="661" ht="18" customHeight="1" s="115"/>
+    <row r="662" ht="18" customHeight="1" s="115"/>
+    <row r="663" ht="18" customHeight="1" s="115"/>
+    <row r="664" ht="18" customHeight="1" s="115"/>
+    <row r="665" ht="18" customHeight="1" s="115"/>
+    <row r="666" ht="18" customHeight="1" s="115"/>
+    <row r="667" ht="18" customHeight="1" s="115"/>
+    <row r="668" ht="18" customHeight="1" s="115"/>
+    <row r="669" ht="18" customHeight="1" s="115"/>
+    <row r="670" ht="18" customHeight="1" s="115"/>
+    <row r="671" ht="18" customHeight="1" s="115"/>
+    <row r="672" ht="18" customHeight="1" s="115"/>
+    <row r="673" ht="18" customHeight="1" s="115"/>
+    <row r="674" ht="18" customHeight="1" s="115"/>
+    <row r="675" ht="18" customHeight="1" s="115"/>
+    <row r="676" ht="18" customHeight="1" s="115"/>
+    <row r="677" ht="18" customHeight="1" s="115"/>
+    <row r="678" ht="18" customHeight="1" s="115"/>
+    <row r="679" ht="18" customHeight="1" s="115"/>
+    <row r="680" ht="18" customHeight="1" s="115"/>
+    <row r="681" ht="18" customHeight="1" s="115"/>
+    <row r="682" ht="18" customHeight="1" s="115"/>
+    <row r="683" ht="18" customHeight="1" s="115"/>
+    <row r="684" ht="18" customHeight="1" s="115"/>
+    <row r="685" ht="18" customHeight="1" s="115"/>
+    <row r="686" ht="18" customHeight="1" s="115"/>
+    <row r="687" ht="18" customHeight="1" s="115"/>
+    <row r="688" ht="18" customHeight="1" s="115"/>
+    <row r="689" ht="18" customHeight="1" s="115"/>
+    <row r="690" ht="18" customHeight="1" s="115"/>
+    <row r="691" ht="18" customHeight="1" s="115"/>
+    <row r="692" ht="18" customHeight="1" s="115"/>
+    <row r="693" ht="18" customHeight="1" s="115"/>
+    <row r="694" ht="18" customHeight="1" s="115"/>
+    <row r="695" ht="18" customHeight="1" s="115"/>
+    <row r="696" ht="18" customHeight="1" s="115"/>
+    <row r="697" ht="18" customHeight="1" s="115"/>
+    <row r="698" ht="18" customHeight="1" s="115"/>
+    <row r="699" ht="18" customHeight="1" s="115"/>
+    <row r="700" ht="18" customHeight="1" s="115"/>
+    <row r="701" ht="18" customHeight="1" s="115"/>
+    <row r="702" ht="18" customHeight="1" s="115"/>
+    <row r="703" ht="18" customHeight="1" s="115"/>
+    <row r="704" ht="18" customHeight="1" s="115"/>
+    <row r="705" ht="18" customHeight="1" s="115"/>
+    <row r="706" ht="18" customHeight="1" s="115"/>
+    <row r="707" ht="18" customHeight="1" s="115"/>
+    <row r="708" ht="18" customHeight="1" s="115"/>
+    <row r="709" ht="18" customHeight="1" s="115"/>
+    <row r="710" ht="18" customHeight="1" s="115"/>
+    <row r="711" ht="18" customHeight="1" s="115"/>
+    <row r="712" ht="18" customHeight="1" s="115"/>
+    <row r="713" ht="18" customHeight="1" s="115"/>
+    <row r="714" ht="18" customHeight="1" s="115"/>
+    <row r="715" ht="18" customHeight="1" s="115"/>
+    <row r="716" ht="18" customHeight="1" s="115"/>
+    <row r="717" ht="18" customHeight="1" s="115"/>
+    <row r="718" ht="18" customHeight="1" s="115"/>
+    <row r="719" ht="18" customHeight="1" s="115"/>
+    <row r="720" ht="18" customHeight="1" s="115"/>
+    <row r="721" ht="18" customHeight="1" s="115"/>
+    <row r="722" ht="18" customHeight="1" s="115"/>
+    <row r="723" ht="18" customHeight="1" s="115"/>
+    <row r="724" ht="18" customHeight="1" s="115"/>
+    <row r="725" ht="18" customHeight="1" s="115"/>
+    <row r="726" ht="18" customHeight="1" s="115"/>
+    <row r="727" ht="18" customHeight="1" s="115"/>
+    <row r="728" ht="18" customHeight="1" s="115"/>
+    <row r="729" ht="18" customHeight="1" s="115"/>
+    <row r="730" ht="18" customHeight="1" s="115"/>
+    <row r="731" ht="18" customHeight="1" s="115"/>
+    <row r="732" ht="18" customHeight="1" s="115"/>
+    <row r="733" ht="18" customHeight="1" s="115"/>
+    <row r="734" ht="18" customHeight="1" s="115"/>
+    <row r="735" ht="18" customHeight="1" s="115"/>
+    <row r="736" ht="18" customHeight="1" s="115"/>
+    <row r="737" ht="18" customHeight="1" s="115"/>
+    <row r="738" ht="18" customHeight="1" s="115"/>
+    <row r="739" ht="18" customHeight="1" s="115"/>
+    <row r="740" ht="18" customHeight="1" s="115"/>
+    <row r="741" ht="18" customHeight="1" s="115"/>
+    <row r="742" ht="18" customHeight="1" s="115"/>
+    <row r="743" ht="18" customHeight="1" s="115"/>
+    <row r="744" ht="18" customHeight="1" s="115"/>
+    <row r="745" ht="18" customHeight="1" s="115"/>
+    <row r="746" ht="18" customHeight="1" s="115"/>
+    <row r="747" ht="18" customHeight="1" s="115"/>
+    <row r="748" ht="18" customHeight="1" s="115"/>
+    <row r="749" ht="18" customHeight="1" s="115"/>
+    <row r="750" ht="18" customHeight="1" s="115"/>
+    <row r="751" ht="18" customHeight="1" s="115"/>
+    <row r="752" ht="18" customHeight="1" s="115"/>
+    <row r="753" ht="18" customHeight="1" s="115"/>
+    <row r="754" ht="18" customHeight="1" s="115"/>
+    <row r="755" ht="18" customHeight="1" s="115"/>
+    <row r="756" ht="18" customHeight="1" s="115"/>
+    <row r="757" ht="18" customHeight="1" s="115"/>
+    <row r="758" ht="18" customHeight="1" s="115"/>
+    <row r="759" ht="18" customHeight="1" s="115"/>
+    <row r="760" ht="18" customHeight="1" s="115"/>
+    <row r="761" ht="18" customHeight="1" s="115"/>
+    <row r="762" ht="18" customHeight="1" s="115"/>
+    <row r="763" ht="18" customHeight="1" s="115"/>
+    <row r="764" ht="18" customHeight="1" s="115"/>
+    <row r="765" ht="18" customHeight="1" s="115"/>
+    <row r="766" ht="18" customHeight="1" s="115"/>
+    <row r="767" ht="18" customHeight="1" s="115"/>
+    <row r="768" ht="18" customHeight="1" s="115"/>
+    <row r="769" ht="18" customHeight="1" s="115"/>
+    <row r="770" ht="18" customHeight="1" s="115"/>
+    <row r="771" ht="18" customHeight="1" s="115"/>
+    <row r="772" ht="18" customHeight="1" s="115"/>
+    <row r="773" ht="18" customHeight="1" s="115"/>
+    <row r="774" ht="18" customHeight="1" s="115"/>
+    <row r="775" ht="18" customHeight="1" s="115"/>
+    <row r="776" ht="18" customHeight="1" s="115"/>
+    <row r="777" ht="18" customHeight="1" s="115"/>
+    <row r="778" ht="18" customHeight="1" s="115"/>
+    <row r="779" ht="18" customHeight="1" s="115"/>
+    <row r="780" ht="18" customHeight="1" s="115"/>
+    <row r="781" ht="18" customHeight="1" s="115"/>
+    <row r="782" ht="18" customHeight="1" s="115"/>
+    <row r="783" ht="18" customHeight="1" s="115"/>
+    <row r="784" ht="18" customHeight="1" s="115"/>
+    <row r="785" ht="18" customHeight="1" s="115"/>
+    <row r="786" ht="18" customHeight="1" s="115"/>
+    <row r="787" ht="18" customHeight="1" s="115"/>
+    <row r="788" ht="18" customHeight="1" s="115"/>
+    <row r="789" ht="18" customHeight="1" s="115"/>
+    <row r="790" ht="18" customHeight="1" s="115"/>
+    <row r="791" ht="18" customHeight="1" s="115"/>
+    <row r="792" ht="18" customHeight="1" s="115"/>
+    <row r="793" ht="18" customHeight="1" s="115"/>
+    <row r="794" ht="18" customHeight="1" s="115"/>
+    <row r="795" ht="18" customHeight="1" s="115"/>
+    <row r="796" ht="18" customHeight="1" s="115"/>
+    <row r="797" ht="18" customHeight="1" s="115"/>
+    <row r="798" ht="18" customHeight="1" s="115"/>
+    <row r="799" ht="18" customHeight="1" s="115"/>
+    <row r="800" ht="18" customHeight="1" s="115"/>
+    <row r="801" ht="18" customHeight="1" s="115"/>
+    <row r="802" ht="18" customHeight="1" s="115"/>
+    <row r="803" ht="18" customHeight="1" s="115"/>
+    <row r="804" ht="18" customHeight="1" s="115"/>
+    <row r="805" ht="18" customHeight="1" s="115"/>
+    <row r="806" ht="18" customHeight="1" s="115"/>
+    <row r="807" ht="18" customHeight="1" s="115"/>
+    <row r="808" ht="18" customHeight="1" s="115"/>
+    <row r="809" ht="18" customHeight="1" s="115"/>
+    <row r="810" ht="18" customHeight="1" s="115"/>
+    <row r="811" ht="18" customHeight="1" s="115"/>
+    <row r="812" ht="18" customHeight="1" s="115"/>
+    <row r="813" ht="18" customHeight="1" s="115"/>
+    <row r="814" ht="18" customHeight="1" s="115"/>
+    <row r="815" ht="18" customHeight="1" s="115"/>
+    <row r="816" ht="18" customHeight="1" s="115"/>
+    <row r="817" ht="18" customHeight="1" s="115"/>
+    <row r="818" ht="18" customHeight="1" s="115"/>
+    <row r="819" ht="18" customHeight="1" s="115"/>
+    <row r="820" ht="18" customHeight="1" s="115"/>
+    <row r="821" ht="18" customHeight="1" s="115"/>
+    <row r="822" ht="18" customHeight="1" s="115"/>
+    <row r="823" ht="18" customHeight="1" s="115"/>
+    <row r="824" ht="18" customHeight="1" s="115"/>
+    <row r="825" ht="18" customHeight="1" s="115"/>
+    <row r="826" ht="18" customHeight="1" s="115"/>
+    <row r="827" ht="18" customHeight="1" s="115"/>
+    <row r="828" ht="18" customHeight="1" s="115"/>
+    <row r="829" ht="18" customHeight="1" s="115"/>
+    <row r="830" ht="18" customHeight="1" s="115"/>
+    <row r="831" ht="18" customHeight="1" s="115"/>
+    <row r="832" ht="18" customHeight="1" s="115"/>
+    <row r="833" ht="18" customHeight="1" s="115"/>
+    <row r="834" ht="18" customHeight="1" s="115"/>
+    <row r="835" ht="18" customHeight="1" s="115"/>
+    <row r="836" ht="18" customHeight="1" s="115"/>
+    <row r="837" ht="18" customHeight="1" s="115"/>
+    <row r="838" ht="18" customHeight="1" s="115"/>
+    <row r="839" ht="18" customHeight="1" s="115"/>
+    <row r="840" ht="18" customHeight="1" s="115"/>
+    <row r="841" ht="18" customHeight="1" s="115"/>
+    <row r="842" ht="18" customHeight="1" s="115"/>
+    <row r="843" ht="18" customHeight="1" s="115"/>
+    <row r="844" ht="18" customHeight="1" s="115"/>
+    <row r="845" ht="18" customHeight="1" s="115"/>
+    <row r="846" ht="18" customHeight="1" s="115"/>
+    <row r="847" ht="18" customHeight="1" s="115"/>
+    <row r="848" ht="18" customHeight="1" s="115"/>
+    <row r="849" ht="18" customHeight="1" s="115"/>
+    <row r="850" ht="18" customHeight="1" s="115"/>
+    <row r="851" ht="18" customHeight="1" s="115"/>
+    <row r="852" ht="18" customHeight="1" s="115"/>
+    <row r="853" ht="18" customHeight="1" s="115"/>
+    <row r="854" ht="18" customHeight="1" s="115"/>
+    <row r="855" ht="18" customHeight="1" s="115"/>
+    <row r="856" ht="18" customHeight="1" s="115"/>
+    <row r="857" ht="18" customHeight="1" s="115"/>
+    <row r="858" ht="18" customHeight="1" s="115"/>
+    <row r="859" ht="18" customHeight="1" s="115"/>
+    <row r="860" ht="18" customHeight="1" s="115"/>
+    <row r="861" ht="18" customHeight="1" s="115"/>
+    <row r="862" ht="18" customHeight="1" s="115"/>
+    <row r="863" ht="18" customHeight="1" s="115"/>
+    <row r="864" ht="18" customHeight="1" s="115"/>
+    <row r="865" ht="18" customHeight="1" s="115"/>
+    <row r="866" ht="18" customHeight="1" s="115"/>
+    <row r="867" ht="18" customHeight="1" s="115"/>
+    <row r="868" ht="18" customHeight="1" s="115"/>
+    <row r="869" ht="18" customHeight="1" s="115"/>
+    <row r="870" ht="18" customHeight="1" s="115"/>
+    <row r="871" ht="18" customHeight="1" s="115"/>
+    <row r="872" ht="18" customHeight="1" s="115"/>
+    <row r="873" ht="18" customHeight="1" s="115"/>
+    <row r="874" ht="18" customHeight="1" s="115"/>
+    <row r="875" ht="18" customHeight="1" s="115"/>
+    <row r="876" ht="18" customHeight="1" s="115"/>
+    <row r="877" ht="18" customHeight="1" s="115"/>
+    <row r="878" ht="18" customHeight="1" s="115"/>
+    <row r="879" ht="18" customHeight="1" s="115"/>
+    <row r="880" ht="18" customHeight="1" s="115"/>
+    <row r="881" ht="18" customHeight="1" s="115"/>
+    <row r="882" ht="18" customHeight="1" s="115"/>
+    <row r="883" ht="18" customHeight="1" s="115"/>
+    <row r="884" ht="18" customHeight="1" s="115"/>
+    <row r="885" ht="18" customHeight="1" s="115"/>
+    <row r="886" ht="18" customHeight="1" s="115"/>
+    <row r="887" ht="18" customHeight="1" s="115"/>
+    <row r="888" ht="18" customHeight="1" s="115"/>
+    <row r="889" ht="18" customHeight="1" s="115"/>
+    <row r="890" ht="18" customHeight="1" s="115"/>
+    <row r="891" ht="18" customHeight="1" s="115"/>
+    <row r="892" ht="18" customHeight="1" s="115"/>
+    <row r="893" ht="18" customHeight="1" s="115"/>
+    <row r="894" ht="18" customHeight="1" s="115"/>
+    <row r="895" ht="18" customHeight="1" s="115"/>
+    <row r="896" ht="18" customHeight="1" s="115"/>
+    <row r="897" ht="18" customHeight="1" s="115"/>
+    <row r="898" ht="18" customHeight="1" s="115"/>
+    <row r="899" ht="18" customHeight="1" s="115"/>
+    <row r="900" ht="18" customHeight="1" s="115"/>
+    <row r="901" ht="18" customHeight="1" s="115"/>
+    <row r="902" ht="18" customHeight="1" s="115"/>
+    <row r="903" ht="18" customHeight="1" s="115"/>
+    <row r="904" ht="18" customHeight="1" s="115"/>
+    <row r="905" ht="18" customHeight="1" s="115"/>
+    <row r="906" ht="18" customHeight="1" s="115"/>
+    <row r="907" ht="18" customHeight="1" s="115"/>
+    <row r="908" ht="18" customHeight="1" s="115"/>
+    <row r="909" ht="18" customHeight="1" s="115"/>
+    <row r="910" ht="18" customHeight="1" s="115"/>
+    <row r="911" ht="18" customHeight="1" s="115"/>
+    <row r="912" ht="18" customHeight="1" s="115"/>
+    <row r="913" ht="18" customHeight="1" s="115"/>
+    <row r="914" ht="18" customHeight="1" s="115"/>
+    <row r="915" ht="18" customHeight="1" s="115"/>
+    <row r="916" ht="18" customHeight="1" s="115"/>
+    <row r="917" ht="18" customHeight="1" s="115"/>
+    <row r="918" ht="18" customHeight="1" s="115"/>
+    <row r="919" ht="18" customHeight="1" s="115"/>
+    <row r="920" ht="18" customHeight="1" s="115"/>
+    <row r="921" ht="18" customHeight="1" s="115"/>
+    <row r="922" ht="18" customHeight="1" s="115"/>
+    <row r="923" ht="18" customHeight="1" s="115"/>
+    <row r="924" ht="18" customHeight="1" s="115"/>
+    <row r="925" ht="18" customHeight="1" s="115"/>
+    <row r="926" ht="18" customHeight="1" s="115"/>
+    <row r="927" ht="18" customHeight="1" s="115"/>
+    <row r="928" ht="18" customHeight="1" s="115"/>
+    <row r="929" ht="18" customHeight="1" s="115"/>
+    <row r="930" ht="18" customHeight="1" s="115"/>
+    <row r="931" ht="18" customHeight="1" s="115"/>
+    <row r="932" ht="18" customHeight="1" s="115"/>
+    <row r="933" ht="18" customHeight="1" s="115"/>
+    <row r="934" ht="18" customHeight="1" s="115"/>
+    <row r="935" ht="18" customHeight="1" s="115"/>
+    <row r="936" ht="18" customHeight="1" s="115"/>
+    <row r="937" ht="18" customHeight="1" s="115"/>
+    <row r="938" ht="18" customHeight="1" s="115"/>
+    <row r="939" ht="18" customHeight="1" s="115"/>
+    <row r="940" ht="18" customHeight="1" s="115"/>
+    <row r="941" ht="18" customHeight="1" s="115"/>
+    <row r="942" ht="18" customHeight="1" s="115"/>
+    <row r="943" ht="18" customHeight="1" s="115"/>
+    <row r="944" ht="18" customHeight="1" s="115"/>
+    <row r="945" ht="18" customHeight="1" s="115"/>
+    <row r="946" ht="18" customHeight="1" s="115"/>
+    <row r="947" ht="18" customHeight="1" s="115"/>
+    <row r="948" ht="18" customHeight="1" s="115"/>
+    <row r="949" ht="18" customHeight="1" s="115"/>
+    <row r="950" ht="18" customHeight="1" s="115"/>
+    <row r="951" ht="18" customHeight="1" s="115"/>
+    <row r="952" ht="18" customHeight="1" s="115"/>
+    <row r="953" ht="18" customHeight="1" s="115"/>
+    <row r="954" ht="18" customHeight="1" s="115"/>
+    <row r="955" ht="18" customHeight="1" s="115"/>
+    <row r="956" ht="18" customHeight="1" s="115"/>
+    <row r="957" ht="18" customHeight="1" s="115"/>
+    <row r="958" ht="18" customHeight="1" s="115"/>
+    <row r="959" ht="18" customHeight="1" s="115"/>
+    <row r="960" ht="18" customHeight="1" s="115"/>
+    <row r="961" ht="18" customHeight="1" s="115"/>
+    <row r="962" ht="18" customHeight="1" s="115"/>
+    <row r="963" ht="18" customHeight="1" s="115"/>
+    <row r="964" ht="18" customHeight="1" s="115"/>
+    <row r="965" ht="18" customHeight="1" s="115"/>
+    <row r="966" ht="18" customHeight="1" s="115"/>
+    <row r="967" ht="18" customHeight="1" s="115"/>
+    <row r="968" ht="18" customHeight="1" s="115"/>
+    <row r="969" ht="18" customHeight="1" s="115"/>
+    <row r="970" ht="18" customHeight="1" s="115"/>
+    <row r="971" ht="18" customHeight="1" s="115"/>
+    <row r="972" ht="18" customHeight="1" s="115"/>
+    <row r="973" ht="18" customHeight="1" s="115"/>
+    <row r="974" ht="18" customHeight="1" s="115"/>
+    <row r="975" ht="18" customHeight="1" s="115"/>
+    <row r="976" ht="18" customHeight="1" s="115"/>
+    <row r="977" ht="18" customHeight="1" s="115"/>
+    <row r="978" ht="18" customHeight="1" s="115"/>
+    <row r="979" ht="18" customHeight="1" s="115"/>
+    <row r="980" ht="18" customHeight="1" s="115"/>
+    <row r="981" ht="18" customHeight="1" s="115"/>
+    <row r="982" ht="18" customHeight="1" s="115"/>
+    <row r="983" ht="18" customHeight="1" s="115"/>
+    <row r="984" ht="18" customHeight="1" s="115"/>
+    <row r="985" ht="18" customHeight="1" s="115"/>
+    <row r="986" ht="18" customHeight="1" s="115"/>
+    <row r="987" ht="18" customHeight="1" s="115"/>
+    <row r="988" ht="18" customHeight="1" s="115"/>
+    <row r="989" ht="18" customHeight="1" s="115"/>
+    <row r="990" ht="18" customHeight="1" s="115"/>
+    <row r="991" ht="18" customHeight="1" s="115"/>
+    <row r="992" ht="18" customHeight="1" s="115"/>
+    <row r="993" ht="18" customHeight="1" s="115"/>
+    <row r="994" ht="18" customHeight="1" s="115"/>
+    <row r="995" ht="18" customHeight="1" s="115"/>
+    <row r="996" ht="18" customHeight="1" s="115"/>
+    <row r="997" ht="18" customHeight="1" s="115"/>
+    <row r="998" ht="18" customHeight="1" s="115"/>
+    <row r="999" ht="18" customHeight="1" s="115"/>
+    <row r="1000" ht="18" customHeight="1" s="115"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.5118110236220472" right="0.1181102362204725" top="2.362204724409449" bottom="0.7480314960629921" header="0" footer="0"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col width="9" customWidth="1" style="115" min="1" max="1"/>
+    <col width="8.140000000000001" customWidth="1" style="115" min="2" max="2"/>
+    <col width="44.14" customWidth="1" style="115" min="3" max="3"/>
+    <col width="6.43" customWidth="1" style="115" min="4" max="4"/>
+    <col width="8.710000000000001" customWidth="1" style="115" min="5" max="6"/>
+    <col width="1.43" customWidth="1" style="115" min="7" max="7"/>
+    <col hidden="1" outlineLevel="1" width="7.14" customWidth="1" style="115" min="8" max="8"/>
+    <col hidden="1" outlineLevel="1" width="11.71" customWidth="1" style="115" min="9" max="9"/>
+    <col hidden="1" outlineLevel="1" width="0.86" customWidth="1" style="115" min="10" max="10"/>
+    <col hidden="1" outlineLevel="1" width="9.140000000000001" customWidth="1" style="115" min="11" max="13"/>
+    <col hidden="1" outlineLevel="1" width="10.14" customWidth="1" style="115" min="14" max="14"/>
+    <col hidden="1" outlineLevel="1" width="1.14" customWidth="1" style="115" min="15" max="15"/>
+    <col hidden="1" outlineLevel="1" width="9.140000000000001" customWidth="1" style="115" min="16" max="17"/>
+    <col hidden="1" outlineLevel="1" width="10.14" customWidth="1" style="115" min="18" max="18"/>
+    <col width="9" customWidth="1" style="115" min="19" max="19"/>
+    <col width="14.29" customWidth="1" style="115" min="20" max="20"/>
+    <col width="11.71" customWidth="1" style="115" min="21" max="24"/>
+    <col width="8.710000000000001" customWidth="1" style="115" min="25" max="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" s="115">
+      <c r="A1" s="116" t="inlineStr">
+        <is>
+          <t>2025年</t>
+        </is>
+      </c>
+      <c r="B1" s="117" t="inlineStr">
+        <is>
+          <t>1月度</t>
+        </is>
+      </c>
+      <c r="C1" s="118" t="inlineStr">
+        <is>
+          <t>経費仮払金精算</t>
+        </is>
+      </c>
+      <c r="D1" s="119" t="n"/>
+      <c r="E1" s="120" t="inlineStr">
+        <is>
+          <t>硝子設備・
+プラントプロジェクト部</t>
+        </is>
+      </c>
+      <c r="F1" s="121" t="n"/>
+      <c r="I1" s="7" t="n"/>
+      <c r="K1" s="7" t="n"/>
+      <c r="L1" s="7" t="n"/>
+      <c r="M1" s="7" t="n"/>
+      <c r="N1" s="7" t="n"/>
+      <c r="O1" s="7" t="n"/>
+      <c r="P1" s="7" t="n"/>
+      <c r="Q1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" s="115">
+      <c r="A2" s="122" t="n"/>
+      <c r="B2" s="123" t="n"/>
+      <c r="C2" s="124" t="n"/>
+      <c r="D2" s="119" t="n"/>
+      <c r="E2" s="125" t="n"/>
+      <c r="F2" s="126" t="n"/>
+      <c r="I2" s="7" t="n"/>
+      <c r="K2" s="7" t="n"/>
+      <c r="L2" s="7" t="n"/>
+      <c r="M2" s="7" t="n"/>
+      <c r="N2" s="7" t="n"/>
+      <c r="O2" s="7" t="n"/>
+      <c r="P2" s="7" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="4.5" customHeight="1" s="115">
+      <c r="B3" s="13" t="n"/>
+      <c r="D3" s="14" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="F3" s="15" t="n"/>
+      <c r="I3" s="7" t="n"/>
+      <c r="K3" s="7" t="n"/>
+      <c r="L3" s="7" t="n"/>
+      <c r="M3" s="7" t="n"/>
+      <c r="N3" s="7" t="n"/>
+      <c r="O3" s="7" t="n"/>
+      <c r="P3" s="7" t="n"/>
+      <c r="Q3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="18" customHeight="1" s="115">
+      <c r="A4" s="90" t="inlineStr">
+        <is>
+          <t>支払日</t>
+        </is>
+      </c>
+      <c r="B4" s="91" t="inlineStr">
+        <is>
+          <t>工番</t>
+        </is>
+      </c>
+      <c r="C4" s="92" t="inlineStr">
+        <is>
+          <t>摘　　要</t>
+        </is>
+      </c>
+      <c r="D4" s="93" t="inlineStr">
+        <is>
+          <t>担当者</t>
+        </is>
+      </c>
+      <c r="E4" s="94" t="inlineStr">
+        <is>
+          <t>収入</t>
+        </is>
+      </c>
+      <c r="F4" s="95" t="inlineStr">
+        <is>
+          <t>支出</t>
+        </is>
+      </c>
+      <c r="G4" s="22" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H4" s="23" t="inlineStr">
+        <is>
+          <t>インボイス</t>
+        </is>
+      </c>
+      <c r="I4" s="24" t="inlineStr">
+        <is>
+          <t>勘定科目</t>
+        </is>
+      </c>
+      <c r="J4" s="25" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K4" s="26" t="inlineStr">
+        <is>
+          <t>10％税込額</t>
+        </is>
+      </c>
+      <c r="L4" s="27" t="inlineStr">
+        <is>
+          <t>8％税込額</t>
+        </is>
+      </c>
+      <c r="M4" s="28" t="inlineStr">
+        <is>
+          <t>非課税額</t>
+        </is>
+      </c>
+      <c r="N4" s="29" t="inlineStr">
+        <is>
+          <t>税込合計</t>
+        </is>
+      </c>
+      <c r="O4" s="30" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="P4" s="31" t="inlineStr">
+        <is>
+          <t>消費税10</t>
+        </is>
+      </c>
+      <c r="Q4" s="32" t="inlineStr">
+        <is>
+          <t>消費税8</t>
+        </is>
+      </c>
+      <c r="R4" s="24" t="inlineStr">
+        <is>
+          <t>消費税計</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1" s="115">
+      <c r="A5" s="33" t="n"/>
+      <c r="B5" s="34" t="n"/>
+      <c r="C5" s="96" t="inlineStr">
+        <is>
+          <t>前月より繰越</t>
+        </is>
+      </c>
+      <c r="D5" s="36" t="n"/>
+      <c r="E5" s="37" t="n">
+        <v>624668</v>
+      </c>
+      <c r="F5" s="38" t="n"/>
+      <c r="H5" s="39" t="n"/>
+      <c r="I5" s="40" t="n"/>
+      <c r="K5" s="41" t="n"/>
+      <c r="L5" s="42" t="n"/>
+      <c r="M5" s="43" t="n"/>
+      <c r="N5" s="44" t="n"/>
+      <c r="O5" s="45" t="n"/>
+      <c r="P5" s="41" t="n"/>
+      <c r="Q5" s="43" t="n"/>
+      <c r="R5" s="44" t="n"/>
+      <c r="T5" s="100" t="inlineStr">
+        <is>
+          <t>GPP</t>
+        </is>
+      </c>
+      <c r="U5" s="100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="18" customHeight="1" s="115">
+      <c r="A6" s="97" t="n">
+        <v>45664</v>
+      </c>
+      <c r="B6" s="47" t="n"/>
+      <c r="C6" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  ご祈祷 玉串代</t>
+        </is>
+      </c>
+      <c r="D6" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E6" s="50" t="n"/>
+      <c r="F6" s="99" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G6" s="51" t="n"/>
+      <c r="H6" s="52" t="inlineStr">
+        <is>
+          <t>不要</t>
+        </is>
+      </c>
+      <c r="I6" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J6" s="51" t="n"/>
+      <c r="K6" s="54" t="n"/>
+      <c r="L6" s="55" t="n"/>
+      <c r="M6" s="56" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N6" s="57">
+        <f>IF(K6+L6+M6=0,"",K6+L6+M6)</f>
+        <v/>
+      </c>
+      <c r="O6" s="58" t="n"/>
+      <c r="P6" s="59">
+        <f>ROUNDDOWN($K6/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q6" s="60">
+        <f>ROUNDDOWN($L6/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R6" s="57">
+        <f>P6+Q6</f>
+        <v/>
+      </c>
+      <c r="T6" s="100" t="inlineStr">
+        <is>
+          <t>科目</t>
+        </is>
+      </c>
+      <c r="U6" s="109" t="inlineStr">
+        <is>
+          <t>10％税込額</t>
+        </is>
+      </c>
+      <c r="V6" s="109" t="inlineStr">
+        <is>
+          <t>8％税込額</t>
+        </is>
+      </c>
+      <c r="W6" s="109" t="inlineStr">
+        <is>
+          <t>非課税額</t>
+        </is>
+      </c>
+      <c r="X6" s="109" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1" s="115">
+      <c r="A7" s="97" t="n">
+        <v>45665</v>
+      </c>
+      <c r="B7" s="47" t="n"/>
+      <c r="C7" s="98" t="inlineStr">
+        <is>
+          <t>水道光熱費・租税公課  水道料金・印紙</t>
+        </is>
+      </c>
+      <c r="D7" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E7" s="55" t="n"/>
+      <c r="F7" s="99" t="n">
+        <v>7571</v>
+      </c>
+      <c r="H7" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I7" s="53" t="inlineStr">
+        <is>
+          <t>水道光熱費</t>
+        </is>
+      </c>
+      <c r="J7" s="51" t="n"/>
+      <c r="K7" s="54" t="n">
+        <v>5571</v>
+      </c>
+      <c r="L7" s="55" t="n"/>
+      <c r="M7" s="56" t="n"/>
+      <c r="N7" s="57">
+        <f>IF(K7+L7+M7=0,"",K7+L7+M7)</f>
+        <v/>
+      </c>
+      <c r="O7" s="58" t="n"/>
+      <c r="P7" s="59">
+        <f>ROUNDDOWN($K7/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q7" s="60">
+        <f>ROUNDDOWN($L7/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R7" s="57">
+        <f>P7+Q7</f>
+        <v/>
+      </c>
+      <c r="T7" s="102" t="inlineStr">
+        <is>
+          <t>交際費</t>
+        </is>
+      </c>
+      <c r="U7" s="111" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V7" s="111" t="n"/>
+      <c r="W7" s="111" t="n"/>
+      <c r="X7" s="111" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" ht="18" customHeight="1" s="115">
+      <c r="A8" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B8" s="47" t="n"/>
+      <c r="C8" s="98" t="inlineStr">
+        <is>
+          <t>💰💰💰入金💰💰💰</t>
+        </is>
+      </c>
+      <c r="D8" s="99" t="inlineStr">
+        <is>
+          <t>田代</t>
+        </is>
+      </c>
+      <c r="E8" s="55" t="n">
+        <v>300000</v>
+      </c>
+      <c r="F8" s="99" t="n"/>
+      <c r="H8" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I8" s="53" t="inlineStr">
+        <is>
+          <t>租税公課</t>
+        </is>
+      </c>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="54" t="n"/>
+      <c r="L8" s="55" t="n"/>
+      <c r="M8" s="56" t="n">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="57">
+        <f>IF(K8+L8+M8=0,"",K8+L8+M8)</f>
+        <v/>
+      </c>
+      <c r="O8" s="58" t="n"/>
+      <c r="P8" s="59">
+        <f>ROUNDDOWN($K8/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q8" s="60">
+        <f>ROUNDDOWN($L8/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R8" s="57">
+        <f>P8+Q8</f>
+        <v/>
+      </c>
+      <c r="T8" s="102" t="inlineStr">
+        <is>
+          <t>仕入材料</t>
+        </is>
+      </c>
+      <c r="U8" s="111" t="n">
+        <v>4176</v>
+      </c>
+      <c r="V8" s="111" t="n"/>
+      <c r="W8" s="111" t="n"/>
+      <c r="X8" s="111" t="n">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1" s="115">
+      <c r="A9" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B9" s="47" t="n"/>
+      <c r="C9" s="98" t="inlineStr">
+        <is>
+          <t>交際費・旅費交通費  協創会忘年会・駐車場代・PCデータ抜出</t>
+        </is>
+      </c>
+      <c r="D9" s="99" t="inlineStr">
+        <is>
+          <t>田代</t>
+        </is>
+      </c>
+      <c r="E9" s="55" t="n"/>
+      <c r="F9" s="99" t="n">
+        <v>50100</v>
+      </c>
+      <c r="H9" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I9" s="53" t="inlineStr">
+        <is>
+          <t>交際費</t>
+        </is>
+      </c>
+      <c r="J9" s="51" t="n"/>
+      <c r="K9" s="54" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L9" s="55" t="n"/>
+      <c r="M9" s="56" t="n"/>
+      <c r="N9" s="57">
+        <f>IF(K9+L9+M9=0,"",K9+L9+M9)</f>
+        <v/>
+      </c>
+      <c r="O9" s="58" t="n"/>
+      <c r="P9" s="59">
+        <f>ROUNDDOWN($K9/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q9" s="60">
+        <f>ROUNDDOWN($L9/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R9" s="57">
+        <f>P9+Q9</f>
+        <v/>
+      </c>
+      <c r="T9" s="102" t="inlineStr">
+        <is>
+          <t>事務消耗品費</t>
+        </is>
+      </c>
+      <c r="U9" s="111" t="n">
+        <v>3300</v>
+      </c>
+      <c r="V9" s="111" t="n"/>
+      <c r="W9" s="111" t="n"/>
+      <c r="X9" s="111" t="n">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="115">
+      <c r="A10" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B10" s="47" t="n"/>
+      <c r="C10" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費・仕入材料  出張経費11/28～12/27【詳細別紙】</t>
+        </is>
+      </c>
+      <c r="D10" s="99" t="inlineStr">
+        <is>
+          <t>佐藤</t>
+        </is>
+      </c>
+      <c r="E10" s="55" t="n"/>
+      <c r="F10" s="99" t="n">
+        <v>77293</v>
+      </c>
+      <c r="H10" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I10" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J10" s="51" t="n"/>
+      <c r="K10" s="54" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L10" s="55" t="n"/>
+      <c r="M10" s="56" t="n"/>
+      <c r="N10" s="57">
+        <f>IF(K10+L10+M10=0,"",K10+L10+M10)</f>
+        <v/>
+      </c>
+      <c r="O10" s="58" t="n"/>
+      <c r="P10" s="59">
+        <f>ROUNDDOWN($K10/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q10" s="60">
+        <f>ROUNDDOWN($L10/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R10" s="57">
+        <f>P10+Q10</f>
+        <v/>
+      </c>
+      <c r="T10" s="102" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="U10" s="111" t="n">
+        <v>86634</v>
+      </c>
+      <c r="V10" s="111" t="n"/>
+      <c r="W10" s="111" t="n">
+        <v>30000</v>
+      </c>
+      <c r="X10" s="111" t="n">
+        <v>116634</v>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1" s="115">
+      <c r="A11" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B11" s="47" t="n"/>
+      <c r="C11" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費・仕入材料  出張経費1/6～1/9【詳細別紙】</t>
+        </is>
+      </c>
+      <c r="D11" s="99" t="inlineStr">
+        <is>
+          <t>佐藤</t>
+        </is>
+      </c>
+      <c r="E11" s="55" t="n"/>
+      <c r="F11" s="99" t="n">
+        <v>14856</v>
+      </c>
+      <c r="H11" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I11" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J11" s="51" t="n"/>
+      <c r="K11" s="54" t="n">
+        <v>41800</v>
+      </c>
+      <c r="L11" s="55" t="n"/>
+      <c r="M11" s="56" t="n"/>
+      <c r="N11" s="57">
+        <f>IF(K11+L11+M11=0,"",K11+L11+M11)</f>
+        <v/>
+      </c>
+      <c r="O11" s="58" t="n"/>
+      <c r="P11" s="59">
+        <f>ROUNDDOWN($K11/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q11" s="60">
+        <f>ROUNDDOWN($L11/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R11" s="57">
+        <f>P11+Q11</f>
+        <v/>
+      </c>
+      <c r="T11" s="102" t="inlineStr">
+        <is>
+          <t>水道光熱費</t>
+        </is>
+      </c>
+      <c r="U11" s="111" t="n">
+        <v>5571</v>
+      </c>
+      <c r="V11" s="111" t="n"/>
+      <c r="W11" s="111" t="n"/>
+      <c r="X11" s="111" t="n">
+        <v>5571</v>
+      </c>
+    </row>
+    <row r="12" ht="18" customHeight="1" s="115">
+      <c r="A12" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B12" s="47" t="n"/>
+      <c r="C12" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  ETC代</t>
+        </is>
+      </c>
+      <c r="D12" s="99" t="inlineStr">
+        <is>
+          <t>佐藤</t>
+        </is>
+      </c>
+      <c r="E12" s="55" t="n"/>
+      <c r="F12" s="99" t="n">
+        <v>14530</v>
+      </c>
+      <c r="H12" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I12" s="53" t="inlineStr">
+        <is>
+          <t>事務消耗品費</t>
+        </is>
+      </c>
+      <c r="J12" s="51" t="n"/>
+      <c r="K12" s="54" t="n">
+        <v>3300</v>
+      </c>
+      <c r="L12" s="55" t="n"/>
+      <c r="M12" s="56" t="n"/>
+      <c r="N12" s="57">
+        <f>IF(K12+L12+M12=0,"",K12+L12+M12)</f>
+        <v/>
+      </c>
+      <c r="O12" s="58" t="n"/>
+      <c r="P12" s="59">
+        <f>ROUNDDOWN($K12/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q12" s="60">
+        <f>ROUNDDOWN($L12/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R12" s="57">
+        <f>P12+Q12</f>
+        <v/>
+      </c>
+      <c r="T12" s="102" t="inlineStr">
+        <is>
+          <t>租税公課</t>
+        </is>
+      </c>
+      <c r="U12" s="111" t="n"/>
+      <c r="V12" s="111" t="n"/>
+      <c r="W12" s="111" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X12" s="111" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="115">
+      <c r="A13" s="97" t="n">
+        <v>45671</v>
+      </c>
+      <c r="B13" s="47" t="n"/>
+      <c r="C13" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  日本認証講習会交通費 横浜駅～浜松町駅(JR)往復x2日</t>
+        </is>
+      </c>
+      <c r="D13" s="99" t="inlineStr">
+        <is>
+          <t>小仁所</t>
+        </is>
+      </c>
+      <c r="E13" s="55" t="n"/>
+      <c r="F13" s="99" t="n">
+        <v>1932</v>
+      </c>
+      <c r="H13" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I13" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J13" s="51" t="n"/>
+      <c r="K13" s="54" t="n">
+        <v>14530</v>
+      </c>
+      <c r="L13" s="55" t="n"/>
+      <c r="M13" s="56" t="n"/>
+      <c r="N13" s="57">
+        <f>IF(K13+L13+M13=0,"",K13+L13+M13)</f>
+        <v/>
+      </c>
+      <c r="O13" s="58" t="n"/>
+      <c r="P13" s="59">
+        <f>ROUNDDOWN($K13/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q13" s="60">
+        <f>ROUNDDOWN($L13/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R13" s="57">
+        <f>P13+Q13</f>
+        <v/>
+      </c>
+      <c r="T13" s="102" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="U13" s="111" t="n">
+        <v>5210</v>
+      </c>
+      <c r="V13" s="111" t="n"/>
+      <c r="W13" s="111" t="n"/>
+      <c r="X13" s="111" t="n">
+        <v>5210</v>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="115">
+      <c r="A14" s="97" t="n">
+        <v>45671</v>
+      </c>
+      <c r="B14" s="47" t="n"/>
+      <c r="C14" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  榊代</t>
+        </is>
+      </c>
+      <c r="D14" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E14" s="55" t="n"/>
+      <c r="F14" s="99" t="n">
+        <v>600</v>
+      </c>
+      <c r="H14" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I14" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J14" s="51" t="n"/>
+      <c r="K14" s="54" t="n">
+        <v>1932</v>
+      </c>
+      <c r="L14" s="55" t="n"/>
+      <c r="M14" s="56" t="n"/>
+      <c r="N14" s="57">
+        <f>IF(K14+L14+M14=0,"",K14+L14+M14)</f>
+        <v/>
+      </c>
+      <c r="O14" s="58" t="n"/>
+      <c r="P14" s="59">
+        <f>ROUNDDOWN($K14/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q14" s="60">
+        <f>ROUNDDOWN($L14/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R14" s="57">
+        <f>P14+Q14</f>
+        <v/>
+      </c>
+      <c r="T14" s="102" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="U14" s="111" t="n">
+        <v>158438</v>
+      </c>
+      <c r="V14" s="111" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W14" s="111" t="n"/>
+      <c r="X14" s="111" t="n">
+        <v>162447</v>
+      </c>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="115">
+      <c r="A15" s="97" t="n">
+        <v>45672</v>
+      </c>
+      <c r="B15" s="47" t="n"/>
+      <c r="C15" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  奉献酒</t>
+        </is>
+      </c>
+      <c r="D15" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E15" s="55" t="n"/>
+      <c r="F15" s="99" t="n">
+        <v>4100</v>
+      </c>
+      <c r="H15" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I15" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J15" s="51" t="n"/>
+      <c r="K15" s="54" t="n">
+        <v>600</v>
+      </c>
+      <c r="L15" s="55" t="n"/>
+      <c r="M15" s="56" t="n"/>
+      <c r="N15" s="57">
+        <f>IF(K15+L15+M15=0,"",K15+L15+M15)</f>
+        <v/>
+      </c>
+      <c r="O15" s="58" t="n"/>
+      <c r="P15" s="59">
+        <f>ROUNDDOWN($K15/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q15" s="60">
+        <f>ROUNDDOWN($L15/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R15" s="57">
+        <f>P15+Q15</f>
+        <v/>
+      </c>
+      <c r="T15" s="102" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+      <c r="U15" s="111" t="n">
+        <v>266329</v>
+      </c>
+      <c r="V15" s="111" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W15" s="111" t="n">
+        <v>32000</v>
+      </c>
+      <c r="X15" s="111" t="n">
+        <v>302338</v>
+      </c>
+    </row>
+    <row r="16" ht="18" customHeight="1" s="115">
+      <c r="A16" s="97" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B16" s="47" t="n"/>
+      <c r="C16" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  AGC鏡開き物品代</t>
+        </is>
+      </c>
+      <c r="D16" s="99" t="inlineStr">
+        <is>
+          <t>小仁所</t>
+        </is>
+      </c>
+      <c r="E16" s="55" t="n"/>
+      <c r="F16" s="99" t="n">
+        <v>6534</v>
+      </c>
+      <c r="H16" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I16" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J16" s="51" t="n"/>
+      <c r="K16" s="54" t="n">
+        <v>4100</v>
+      </c>
+      <c r="L16" s="55" t="n"/>
+      <c r="M16" s="56" t="n"/>
+      <c r="N16" s="57">
+        <f>IF(K16+L16+M16=0,"",K16+L16+M16)</f>
+        <v/>
+      </c>
+      <c r="O16" s="58" t="n"/>
+      <c r="P16" s="59">
+        <f>ROUNDDOWN($K16/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q16" s="60">
+        <f>ROUNDDOWN($L16/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R16" s="57">
+        <f>P16+Q16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="115">
+      <c r="A17" s="97" t="n">
+        <v>45677</v>
+      </c>
+      <c r="B17" s="47" t="n"/>
+      <c r="C17" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  宿泊費</t>
+        </is>
+      </c>
+      <c r="D17" s="99" t="inlineStr">
+        <is>
+          <t>尾川</t>
+        </is>
+      </c>
+      <c r="E17" s="55" t="n"/>
+      <c r="F17" s="99" t="n">
+        <v>54600</v>
+      </c>
+      <c r="H17" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I17" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J17" s="51" t="n"/>
+      <c r="K17" s="54" t="n">
+        <v>6534</v>
+      </c>
+      <c r="L17" s="55" t="n"/>
+      <c r="M17" s="56" t="n"/>
+      <c r="N17" s="57">
+        <f>IF(K17+L17+M17=0,"",K17+L17+M17)</f>
+        <v/>
+      </c>
+      <c r="O17" s="58" t="n"/>
+      <c r="P17" s="59">
+        <f>ROUNDDOWN($K17/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q17" s="60">
+        <f>ROUNDDOWN($L17/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R17" s="57">
+        <f>P17+Q17</f>
+        <v/>
+      </c>
+      <c r="T17" s="104" t="inlineStr">
+        <is>
+          <t>GPP</t>
+        </is>
+      </c>
+      <c r="U17" s="104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V17" s="104" t="n"/>
+      <c r="W17" s="104" t="n"/>
+      <c r="X17" s="104" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="115">
+      <c r="A18" s="97" t="n">
+        <v>45680</v>
+      </c>
+      <c r="B18" s="47" t="n"/>
+      <c r="C18" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  指定ゴミ袋</t>
+        </is>
+      </c>
+      <c r="D18" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E18" s="55" t="n"/>
+      <c r="F18" s="99" t="n">
+        <v>33000</v>
+      </c>
+      <c r="H18" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I18" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J18" s="51" t="n"/>
+      <c r="K18" s="54" t="n">
+        <v>54600</v>
+      </c>
+      <c r="L18" s="55" t="n"/>
+      <c r="M18" s="56" t="n"/>
+      <c r="N18" s="57">
+        <f>IF(K18+L18+M18=0,"",K18+L18+M18)</f>
+        <v/>
+      </c>
+      <c r="O18" s="58" t="n"/>
+      <c r="P18" s="59">
+        <f>ROUNDDOWN($K18/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q18" s="60">
+        <f>ROUNDDOWN($L18/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R18" s="57">
+        <f>P18+Q18</f>
+        <v/>
+      </c>
+      <c r="T18" s="105" t="inlineStr">
+        <is>
+          <t>科目</t>
+        </is>
+      </c>
+      <c r="U18" s="106" t="inlineStr">
+        <is>
+          <t>10％税込額</t>
+        </is>
+      </c>
+      <c r="V18" s="106" t="inlineStr">
+        <is>
+          <t>8％税込額</t>
+        </is>
+      </c>
+      <c r="W18" s="106" t="inlineStr">
+        <is>
+          <t>非課税額</t>
+        </is>
+      </c>
+      <c r="X18" s="106" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="115">
+      <c r="A19" s="97" t="n">
+        <v>45684</v>
+      </c>
+      <c r="B19" s="47" t="n"/>
+      <c r="C19" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  日本認証試験交通費 鶴見駅～テレコムセンター(JR・ゆりかもめ)往復</t>
+        </is>
+      </c>
+      <c r="D19" s="99" t="inlineStr">
+        <is>
+          <t>小仁所</t>
+        </is>
+      </c>
+      <c r="E19" s="55" t="n"/>
+      <c r="F19" s="99" t="n">
+        <v>1412</v>
+      </c>
+      <c r="H19" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I19" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J19" s="51" t="n"/>
+      <c r="K19" s="54" t="n">
+        <v>33000</v>
+      </c>
+      <c r="L19" s="55" t="n"/>
+      <c r="M19" s="56" t="n"/>
+      <c r="N19" s="57">
+        <f>IF(K19+L19+M19=0,"",K19+L19+M19)</f>
+        <v/>
+      </c>
+      <c r="O19" s="58" t="n"/>
+      <c r="P19" s="59">
+        <f>ROUNDDOWN($K19/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q19" s="60">
+        <f>ROUNDDOWN($L19/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R19" s="57">
+        <f>P19+Q19</f>
+        <v/>
+      </c>
+      <c r="T19" s="102" t="inlineStr">
+        <is>
+          <t>交際費</t>
+        </is>
+      </c>
+      <c r="U19" s="111" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V19" s="111" t="n"/>
+      <c r="W19" s="111" t="n"/>
+      <c r="X19" s="111" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="115">
+      <c r="A20" s="97" t="n">
+        <v>45685</v>
+      </c>
+      <c r="B20" s="47" t="n"/>
+      <c r="C20" s="98" t="inlineStr">
+        <is>
+          <t>通信費・租税公課  工事依頼書郵送代・印紙</t>
+        </is>
+      </c>
+      <c r="D20" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E20" s="55" t="n"/>
+      <c r="F20" s="99" t="n">
+        <v>5210</v>
+      </c>
+      <c r="H20" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I20" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J20" s="51" t="n"/>
+      <c r="K20" s="54" t="n">
+        <v>1412</v>
+      </c>
+      <c r="L20" s="55" t="n"/>
+      <c r="M20" s="56" t="n"/>
+      <c r="N20" s="57">
+        <f>IF(K20+L20+M20=0,"",K20+L20+M20)</f>
+        <v/>
+      </c>
+      <c r="O20" s="58" t="n"/>
+      <c r="P20" s="59">
+        <f>ROUNDDOWN($K20/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q20" s="60">
+        <f>ROUNDDOWN($L20/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R20" s="57">
+        <f>P20+Q20</f>
+        <v/>
+      </c>
+      <c r="T20" s="102" t="inlineStr">
+        <is>
+          <t>仕入材料</t>
+        </is>
+      </c>
+      <c r="U20" s="111" t="n">
+        <v>4176</v>
+      </c>
+      <c r="V20" s="111" t="n"/>
+      <c r="W20" s="111" t="n"/>
+      <c r="X20" s="111" t="n">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="115">
+      <c r="A21" s="97" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B21" s="47" t="n"/>
+      <c r="C21" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  榊代</t>
+        </is>
+      </c>
+      <c r="D21" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E21" s="55" t="n"/>
+      <c r="F21" s="99" t="n">
+        <v>600</v>
+      </c>
+      <c r="H21" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I21" s="53" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="J21" s="51" t="n"/>
+      <c r="K21" s="54" t="n">
+        <v>5210</v>
+      </c>
+      <c r="L21" s="55" t="n"/>
+      <c r="M21" s="56" t="n"/>
+      <c r="N21" s="57">
+        <f>IF(K21+L21+M21=0,"",K21+L21+M21)</f>
+        <v/>
+      </c>
+      <c r="O21" s="58" t="n"/>
+      <c r="P21" s="59">
+        <f>ROUNDDOWN($K21/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q21" s="60">
+        <f>ROUNDDOWN($L21/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R21" s="57">
+        <f>P21+Q21</f>
+        <v/>
+      </c>
+      <c r="T21" s="102" t="inlineStr">
+        <is>
+          <t>事務消耗品費</t>
+        </is>
+      </c>
+      <c r="U21" s="111" t="n">
+        <v>3300</v>
+      </c>
+      <c r="V21" s="111" t="n"/>
+      <c r="W21" s="111" t="n"/>
+      <c r="X21" s="111" t="n">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="22" ht="18" customHeight="1" s="115">
+      <c r="A22" s="97" t="n"/>
+      <c r="B22" s="47" t="n"/>
+      <c r="C22" s="98" t="n"/>
+      <c r="D22" s="99" t="n"/>
+      <c r="E22" s="55" t="n"/>
+      <c r="F22" s="99" t="n"/>
+      <c r="H22" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I22" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J22" s="51" t="n"/>
+      <c r="K22" s="54" t="n">
+        <v>600</v>
+      </c>
+      <c r="L22" s="55" t="n"/>
+      <c r="M22" s="56" t="n"/>
+      <c r="N22" s="57">
+        <f>IF(K22+L22+M22=0,"",K22+L22+M22)</f>
+        <v/>
+      </c>
+      <c r="O22" s="58" t="n"/>
+      <c r="P22" s="59">
+        <f>ROUNDDOWN($K22/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q22" s="60">
+        <f>ROUNDDOWN($L22/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R22" s="57">
+        <f>P22+Q22</f>
+        <v/>
+      </c>
+      <c r="T22" s="102" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="U22" s="111" t="n">
+        <v>86634</v>
+      </c>
+      <c r="V22" s="111" t="n"/>
+      <c r="W22" s="111" t="n">
+        <v>30000</v>
+      </c>
+      <c r="X22" s="111" t="n">
+        <v>116634</v>
+      </c>
+    </row>
+    <row r="23" ht="18" customHeight="1" s="115">
+      <c r="A23" s="97" t="n"/>
+      <c r="B23" s="47" t="n"/>
+      <c r="C23" s="98" t="n"/>
+      <c r="D23" s="99" t="n"/>
+      <c r="E23" s="55" t="n"/>
+      <c r="F23" s="99" t="n"/>
+      <c r="H23" s="52" t="n"/>
+      <c r="I23" s="53" t="n"/>
+      <c r="J23" s="51" t="n"/>
+      <c r="K23" s="54" t="n"/>
+      <c r="L23" s="55" t="n"/>
+      <c r="M23" s="56" t="n"/>
+      <c r="N23" s="57">
+        <f>IF(K23+L23+M23=0,"",K23+L23+M23)</f>
+        <v/>
+      </c>
+      <c r="O23" s="58" t="n"/>
+      <c r="P23" s="59">
+        <f>ROUNDDOWN($K23/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q23" s="60">
+        <f>ROUNDDOWN($L23/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R23" s="57">
+        <f>P23+Q23</f>
+        <v/>
+      </c>
+      <c r="T23" s="102" t="inlineStr">
+        <is>
+          <t>水道光熱費</t>
+        </is>
+      </c>
+      <c r="U23" s="111" t="n">
+        <v>5571</v>
+      </c>
+      <c r="V23" s="111" t="n"/>
+      <c r="W23" s="111" t="n"/>
+      <c r="X23" s="111" t="n">
+        <v>5571</v>
+      </c>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="115">
+      <c r="A24" s="97" t="n"/>
+      <c r="B24" s="47" t="n"/>
+      <c r="C24" s="98" t="n"/>
+      <c r="D24" s="99" t="n"/>
+      <c r="E24" s="55" t="n"/>
+      <c r="F24" s="99" t="n"/>
+      <c r="H24" s="52" t="n"/>
+      <c r="I24" s="53" t="n"/>
+      <c r="J24" s="51" t="n"/>
+      <c r="K24" s="54" t="n"/>
+      <c r="L24" s="55" t="n"/>
+      <c r="M24" s="56" t="n"/>
+      <c r="N24" s="57">
+        <f>IF(K24+L24+M24=0,"",K24+L24+M24)</f>
+        <v/>
+      </c>
+      <c r="O24" s="58" t="n"/>
+      <c r="P24" s="59">
+        <f>ROUNDDOWN($K24/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q24" s="60">
+        <f>ROUNDDOWN($L24/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R24" s="57">
+        <f>P24+Q24</f>
+        <v/>
+      </c>
+      <c r="T24" s="102" t="inlineStr">
+        <is>
+          <t>租税公課</t>
+        </is>
+      </c>
+      <c r="U24" s="111" t="n"/>
+      <c r="V24" s="111" t="n"/>
+      <c r="W24" s="111" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X24" s="111" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="115">
+      <c r="A25" s="97" t="n"/>
+      <c r="B25" s="47" t="n"/>
+      <c r="C25" s="98" t="n"/>
+      <c r="D25" s="99" t="n"/>
+      <c r="E25" s="55" t="n"/>
+      <c r="F25" s="99" t="n"/>
+      <c r="H25" s="52" t="n"/>
+      <c r="I25" s="53" t="n"/>
+      <c r="J25" s="51" t="n"/>
+      <c r="K25" s="54" t="n"/>
+      <c r="L25" s="55" t="n"/>
+      <c r="M25" s="56" t="n"/>
+      <c r="N25" s="57">
+        <f>IF(K25+L25+M25=0,"",K25+L25+M25)</f>
+        <v/>
+      </c>
+      <c r="O25" s="58" t="n"/>
+      <c r="P25" s="59">
+        <f>ROUNDDOWN($K25/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q25" s="60">
+        <f>ROUNDDOWN($L25/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R25" s="57">
+        <f>P25+Q25</f>
+        <v/>
+      </c>
+      <c r="T25" s="102" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="U25" s="111" t="n">
+        <v>5210</v>
+      </c>
+      <c r="V25" s="111" t="n"/>
+      <c r="W25" s="111" t="n"/>
+      <c r="X25" s="111" t="n">
+        <v>5210</v>
+      </c>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="115">
+      <c r="A26" s="97" t="n"/>
+      <c r="B26" s="47" t="n"/>
+      <c r="C26" s="98" t="n"/>
+      <c r="D26" s="99" t="n"/>
+      <c r="E26" s="55" t="n"/>
+      <c r="F26" s="99" t="n"/>
+      <c r="H26" s="52" t="n"/>
+      <c r="I26" s="53" t="n"/>
+      <c r="J26" s="51" t="n"/>
+      <c r="K26" s="54" t="n"/>
+      <c r="L26" s="55" t="n"/>
+      <c r="M26" s="56" t="n"/>
+      <c r="N26" s="57">
+        <f>IF(K26+L26+M26=0,"",K26+L26+M26)</f>
+        <v/>
+      </c>
+      <c r="O26" s="58" t="n"/>
+      <c r="P26" s="59">
+        <f>ROUNDDOWN($K26/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q26" s="60">
+        <f>ROUNDDOWN($L26/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R26" s="57">
+        <f>P26+Q26</f>
+        <v/>
+      </c>
+      <c r="T26" s="102" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="U26" s="111" t="n">
+        <v>158438</v>
+      </c>
+      <c r="V26" s="111" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W26" s="111" t="n"/>
+      <c r="X26" s="111" t="n">
+        <v>162447</v>
+      </c>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="115">
+      <c r="A27" s="97" t="n"/>
+      <c r="B27" s="47" t="n"/>
+      <c r="C27" s="98" t="n"/>
+      <c r="D27" s="99" t="n"/>
+      <c r="E27" s="55" t="n"/>
+      <c r="F27" s="99" t="n"/>
+      <c r="H27" s="52" t="n"/>
+      <c r="I27" s="53" t="n"/>
+      <c r="J27" s="51" t="n"/>
+      <c r="K27" s="54" t="n"/>
+      <c r="L27" s="55" t="n"/>
+      <c r="M27" s="56" t="n"/>
+      <c r="N27" s="57">
+        <f>IF(K27+L27+M27=0,"",K27+L27+M27)</f>
+        <v/>
+      </c>
+      <c r="O27" s="58" t="n"/>
+      <c r="P27" s="59">
+        <f>ROUNDDOWN($K27/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q27" s="60">
+        <f>ROUNDDOWN($L27/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R27" s="57">
+        <f>P27+Q27</f>
+        <v/>
+      </c>
+      <c r="T27" s="107" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+      <c r="U27" s="108" t="n">
+        <v>266329</v>
+      </c>
+      <c r="V27" s="108" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W27" s="108" t="n">
+        <v>32000</v>
+      </c>
+      <c r="X27" s="108" t="n">
+        <v>302338</v>
+      </c>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="115">
+      <c r="A28" s="97" t="n"/>
+      <c r="B28" s="47" t="n"/>
+      <c r="C28" s="98" t="n"/>
+      <c r="D28" s="99" t="n"/>
+      <c r="E28" s="55" t="n"/>
+      <c r="F28" s="99" t="n"/>
+      <c r="H28" s="52" t="n"/>
+      <c r="I28" s="53" t="n"/>
+      <c r="J28" s="51" t="n"/>
+      <c r="K28" s="54" t="n"/>
+      <c r="L28" s="55" t="n"/>
+      <c r="M28" s="56" t="n"/>
+      <c r="N28" s="57">
+        <f>IF(K28+L28+M28=0,"",K28+L28+M28)</f>
+        <v/>
+      </c>
+      <c r="O28" s="58" t="n"/>
+      <c r="P28" s="59">
+        <f>ROUNDDOWN($K28/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q28" s="60">
+        <f>ROUNDDOWN($L28/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R28" s="57">
+        <f>P28+Q28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="115">
+      <c r="A29" s="97" t="n"/>
+      <c r="B29" s="47" t="n"/>
+      <c r="C29" s="98" t="n"/>
+      <c r="D29" s="99" t="n"/>
+      <c r="E29" s="55" t="n"/>
+      <c r="F29" s="99" t="n"/>
+      <c r="H29" s="52" t="n"/>
+      <c r="I29" s="53" t="n"/>
+      <c r="J29" s="51" t="n"/>
+      <c r="K29" s="54" t="n"/>
+      <c r="L29" s="55" t="n"/>
+      <c r="M29" s="56" t="n"/>
+      <c r="N29" s="57">
+        <f>IF(K29+L29+M29=0,"",K29+L29+M29)</f>
+        <v/>
+      </c>
+      <c r="O29" s="58" t="n"/>
+      <c r="P29" s="59">
+        <f>ROUNDDOWN($K29/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q29" s="60">
+        <f>ROUNDDOWN($L29/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R29" s="57">
+        <f>P29+Q29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="115">
+      <c r="A30" s="97" t="n"/>
+      <c r="B30" s="47" t="n"/>
+      <c r="C30" s="98" t="n"/>
+      <c r="D30" s="99" t="n"/>
+      <c r="E30" s="55" t="n"/>
+      <c r="F30" s="99" t="n"/>
+      <c r="H30" s="52" t="n"/>
+      <c r="I30" s="53" t="n"/>
+      <c r="J30" s="51" t="n"/>
+      <c r="K30" s="54" t="n"/>
+      <c r="L30" s="55" t="n"/>
+      <c r="M30" s="56" t="n"/>
+      <c r="N30" s="57">
+        <f>IF(K30+L30+M30=0,"",K30+L30+M30)</f>
+        <v/>
+      </c>
+      <c r="O30" s="58" t="n"/>
+      <c r="P30" s="59">
+        <f>ROUNDDOWN($K30/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q30" s="60">
+        <f>ROUNDDOWN($L30/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R30" s="57">
+        <f>P30+Q30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" ht="18" customHeight="1" s="115">
+      <c r="A31" s="97" t="n"/>
+      <c r="B31" s="47" t="n"/>
+      <c r="C31" s="98" t="n"/>
+      <c r="D31" s="99" t="n"/>
+      <c r="E31" s="55" t="n"/>
+      <c r="F31" s="99" t="n"/>
+      <c r="H31" s="52" t="n"/>
+      <c r="I31" s="53" t="n"/>
+      <c r="J31" s="51" t="n"/>
+      <c r="K31" s="54" t="n"/>
+      <c r="L31" s="55" t="n"/>
+      <c r="M31" s="56" t="n"/>
+      <c r="N31" s="57">
+        <f>IF(K31+L31+M31=0,"",K31+L31+M31)</f>
+        <v/>
+      </c>
+      <c r="O31" s="58" t="n"/>
+      <c r="P31" s="59">
+        <f>ROUNDDOWN($K31/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q31" s="60">
+        <f>ROUNDDOWN($L31/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R31" s="57">
+        <f>P31+Q31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" ht="18" customHeight="1" s="115">
+      <c r="A32" s="97" t="n"/>
+      <c r="B32" s="47" t="n"/>
+      <c r="C32" s="98" t="n"/>
+      <c r="D32" s="99" t="n"/>
+      <c r="E32" s="55" t="n"/>
+      <c r="F32" s="99" t="n"/>
+      <c r="H32" s="52" t="n"/>
+      <c r="I32" s="53" t="n"/>
+      <c r="J32" s="51" t="n"/>
+      <c r="K32" s="54" t="n"/>
+      <c r="L32" s="55" t="n"/>
+      <c r="M32" s="56" t="n"/>
+      <c r="N32" s="57">
+        <f>IF(K32+L32+M32=0,"",K32+L32+M32)</f>
+        <v/>
+      </c>
+      <c r="O32" s="58" t="n"/>
+      <c r="P32" s="59">
+        <f>ROUNDDOWN($K32/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q32" s="60">
+        <f>ROUNDDOWN($L32/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R32" s="57">
+        <f>P32+Q32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" ht="18" customHeight="1" s="115">
+      <c r="A33" s="97" t="n"/>
+      <c r="B33" s="47" t="n"/>
+      <c r="C33" s="98" t="n"/>
+      <c r="D33" s="99" t="n"/>
+      <c r="E33" s="55" t="n"/>
+      <c r="F33" s="99" t="n"/>
+      <c r="H33" s="52" t="n"/>
+      <c r="I33" s="53" t="n"/>
+      <c r="J33" s="51" t="n"/>
+      <c r="K33" s="54" t="n"/>
+      <c r="L33" s="55" t="n"/>
+      <c r="M33" s="56" t="n"/>
+      <c r="N33" s="57">
+        <f>IF(K33+L33+M33=0,"",K33+L33+M33)</f>
+        <v/>
+      </c>
+      <c r="O33" s="58" t="n"/>
+      <c r="P33" s="59">
+        <f>ROUNDDOWN($K33/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q33" s="60">
+        <f>ROUNDDOWN($L33/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R33" s="57">
+        <f>P33+Q33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" ht="18" customHeight="1" s="115">
+      <c r="A34" s="97" t="n"/>
+      <c r="B34" s="47" t="n"/>
+      <c r="C34" s="98" t="n"/>
+      <c r="D34" s="99" t="n"/>
+      <c r="E34" s="55" t="n"/>
+      <c r="F34" s="99" t="n"/>
+      <c r="H34" s="52" t="n"/>
+      <c r="I34" s="53" t="n"/>
+      <c r="J34" s="51" t="n"/>
+      <c r="K34" s="54" t="n"/>
+      <c r="L34" s="55" t="n"/>
+      <c r="M34" s="56" t="n"/>
+      <c r="N34" s="57">
+        <f>IF(K34+L34+M34=0,"",K34+L34+M34)</f>
+        <v/>
+      </c>
+      <c r="O34" s="58" t="n"/>
+      <c r="P34" s="59">
+        <f>ROUNDDOWN($K34/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q34" s="60">
+        <f>ROUNDDOWN($L34/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R34" s="57">
+        <f>P34+Q34</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="115">
+      <c r="A35" s="97" t="n"/>
+      <c r="B35" s="47" t="n"/>
+      <c r="C35" s="98" t="n"/>
+      <c r="D35" s="99" t="n"/>
+      <c r="E35" s="55" t="n"/>
+      <c r="F35" s="99" t="n"/>
+      <c r="H35" s="52" t="n"/>
+      <c r="I35" s="53" t="n"/>
+      <c r="J35" s="51" t="n"/>
+      <c r="K35" s="54" t="n"/>
+      <c r="L35" s="55" t="n"/>
+      <c r="M35" s="56" t="n"/>
+      <c r="N35" s="57">
+        <f>IF(K35+L35+M35=0,"",K35+L35+M35)</f>
+        <v/>
+      </c>
+      <c r="O35" s="58" t="n"/>
+      <c r="P35" s="59">
+        <f>ROUNDDOWN($K35/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q35" s="60">
+        <f>ROUNDDOWN($L35/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R35" s="57">
+        <f>P35+Q35</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" ht="18" customHeight="1" s="115">
+      <c r="A36" s="97" t="n"/>
+      <c r="B36" s="47" t="n"/>
+      <c r="C36" s="98" t="n"/>
+      <c r="D36" s="99" t="n"/>
+      <c r="E36" s="55" t="n"/>
+      <c r="F36" s="99" t="n"/>
+      <c r="H36" s="52" t="n"/>
+      <c r="I36" s="53" t="n"/>
+      <c r="J36" s="51" t="n"/>
+      <c r="K36" s="54" t="n"/>
+      <c r="L36" s="55" t="n"/>
+      <c r="M36" s="56" t="n"/>
+      <c r="N36" s="57">
+        <f>IF(K36+L36+M36=0,"",K36+L36+M36)</f>
+        <v/>
+      </c>
+      <c r="O36" s="58" t="n"/>
+      <c r="P36" s="59">
+        <f>ROUNDDOWN($K36/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q36" s="60">
+        <f>ROUNDDOWN($L36/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R36" s="57">
+        <f>P36+Q36</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" ht="18" customHeight="1" s="115">
+      <c r="A37" s="97" t="n"/>
+      <c r="B37" s="47" t="n"/>
+      <c r="C37" s="98" t="n"/>
+      <c r="D37" s="99" t="n"/>
+      <c r="E37" s="55" t="n"/>
+      <c r="F37" s="99" t="n"/>
+      <c r="H37" s="52" t="n"/>
+      <c r="I37" s="53" t="n"/>
+      <c r="J37" s="51" t="n"/>
+      <c r="K37" s="54" t="n"/>
+      <c r="L37" s="55" t="n"/>
+      <c r="M37" s="56" t="n"/>
+      <c r="N37" s="57">
+        <f>IF(K37+L37+M37=0,"",K37+L37+M37)</f>
+        <v/>
+      </c>
+      <c r="O37" s="58" t="n"/>
+      <c r="P37" s="59">
+        <f>ROUNDDOWN($K37/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q37" s="60">
+        <f>ROUNDDOWN($L37/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R37" s="57">
+        <f>P37+Q37</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" ht="18" customHeight="1" s="115">
+      <c r="A38" s="61" t="n"/>
+      <c r="B38" s="62" t="n"/>
+      <c r="C38" s="63" t="n"/>
+      <c r="D38" s="64" t="n"/>
+      <c r="E38" s="65" t="n"/>
+      <c r="F38" s="64" t="n"/>
+      <c r="H38" s="66" t="n"/>
+      <c r="I38" s="67" t="n"/>
+      <c r="J38" s="51" t="n"/>
+      <c r="K38" s="68" t="n"/>
+      <c r="L38" s="65" t="n"/>
+      <c r="M38" s="69" t="n"/>
+      <c r="N38" s="70">
+        <f>IF(K38+L38+M38=0,"",K38+L38+M38)</f>
+        <v/>
+      </c>
+      <c r="O38" s="58" t="n"/>
+      <c r="P38" s="71">
+        <f>ROUNDDOWN($K38/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q38" s="72">
+        <f>ROUNDDOWN($L38/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R38" s="70">
+        <f>P38+Q38</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="115">
+      <c r="A39" s="73" t="n"/>
+      <c r="B39" s="73" t="n"/>
+      <c r="C39" s="74" t="n"/>
+      <c r="D39" s="75" t="inlineStr">
+        <is>
+          <t>合計</t>
+        </is>
+      </c>
+      <c r="E39" s="76">
+        <f>SUM(E5:E38)</f>
+        <v/>
+      </c>
+      <c r="F39" s="77">
+        <f>SUM(F6:F38)</f>
+        <v/>
+      </c>
+      <c r="H39" s="73" t="n"/>
+      <c r="I39" s="73" t="n"/>
+      <c r="K39" s="78">
+        <f>SUM(K6:K38)</f>
+        <v/>
+      </c>
+      <c r="L39" s="79">
+        <f>SUM(L6:L38)</f>
+        <v/>
+      </c>
+      <c r="M39" s="80">
+        <f>SUM(M6:M38)</f>
+        <v/>
+      </c>
+      <c r="N39" s="81">
+        <f>SUM(N6:N38)</f>
+        <v/>
+      </c>
+      <c r="O39" s="58" t="n"/>
+      <c r="P39" s="82">
+        <f>SUM(P6:P38)</f>
+        <v/>
+      </c>
+      <c r="Q39" s="83">
+        <f>SUM(Q6:Q38)</f>
+        <v/>
+      </c>
+      <c r="R39" s="81">
+        <f>SUM(R6:R38)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" ht="18" customHeight="1" s="115">
+      <c r="C40" s="84" t="n"/>
+      <c r="D40" s="85" t="inlineStr">
+        <is>
+          <t>残高</t>
+        </is>
+      </c>
+      <c r="E40" s="127">
+        <f>E39-F39</f>
+        <v/>
+      </c>
+      <c r="F40" s="128" t="n"/>
+      <c r="K40" s="45" t="n"/>
+      <c r="L40" s="45" t="n"/>
+      <c r="M40" s="45" t="n"/>
+      <c r="N40" s="45" t="n"/>
+      <c r="O40" s="45" t="n"/>
+      <c r="P40" s="45" t="n"/>
+      <c r="Q40" s="45" t="n"/>
+      <c r="R40" s="45" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" s="115">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>郡山桑野食堂</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Ava Thompson</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>2848</v>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>6543456543</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>24</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>2848</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" ht="18" customHeight="1" s="115"/>
+    <row r="43" ht="18" customHeight="1" s="115"/>
+    <row r="44" ht="18" customHeight="1" s="115"/>
+    <row r="45" ht="18" customHeight="1" s="115"/>
     <row r="46" ht="18" customHeight="1" s="115"/>
     <row r="47" ht="18" customHeight="1" s="115"/>
     <row r="48" ht="18" customHeight="1" s="115"/>

</xml_diff>

<commit_message>
Big Update - Full deployment Phase 2E
</commit_message>
<xml_diff>
--- a/app/Data/accumulation/Aichi_Accumulated.xlsx
+++ b/app/Data/accumulation/Aichi_Accumulated.xlsx
@@ -21,13 +21,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="集計ﾃｰﾌﾞﾙ" sheetId="16" state="hidden" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024年11月" sheetId="17" state="visible" r:id="rId17"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年07月" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024年12月" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_4" localSheetId="3">'追加1'!$A$1:$H$39</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="0" r:id="rId19"/>
+    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="0" r:id="rId20"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -23700,53 +23701,3068 @@
       <c r="R40" s="45" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1" s="115">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>2025-07-02</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr"/>
+      <c r="C41" s="0" t="inlineStr">
+        <is>
+          <t>郡山桑野食堂</t>
+        </is>
+      </c>
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>Ava Thompson</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr"/>
+      <c r="F41" s="0" t="n">
+        <v>2848</v>
+      </c>
+      <c r="G41" s="0" t="inlineStr"/>
+      <c r="H41" s="0" t="inlineStr">
+        <is>
+          <t>6543456543</t>
+        </is>
+      </c>
+      <c r="I41" s="0" t="inlineStr"/>
+      <c r="J41" s="0" t="inlineStr"/>
+      <c r="K41" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="0" t="inlineStr"/>
+      <c r="N41" s="0" t="n">
+        <v>2848</v>
+      </c>
+      <c r="O41" s="0" t="inlineStr"/>
+      <c r="P41" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" ht="18" customHeight="1" s="115"/>
+    <row r="43" ht="18" customHeight="1" s="115"/>
+    <row r="44" ht="18" customHeight="1" s="115"/>
+    <row r="45" ht="18" customHeight="1" s="115"/>
+    <row r="46" ht="18" customHeight="1" s="115"/>
+    <row r="47" ht="18" customHeight="1" s="115"/>
+    <row r="48" ht="18" customHeight="1" s="115"/>
+    <row r="49" ht="18" customHeight="1" s="115"/>
+    <row r="50" ht="18" customHeight="1" s="115"/>
+    <row r="51" ht="18" customHeight="1" s="115"/>
+    <row r="52" ht="18" customHeight="1" s="115"/>
+    <row r="53" ht="18" customHeight="1" s="115"/>
+    <row r="54" ht="18" customHeight="1" s="115"/>
+    <row r="55" ht="18" customHeight="1" s="115"/>
+    <row r="56" ht="18" customHeight="1" s="115"/>
+    <row r="57" ht="18" customHeight="1" s="115"/>
+    <row r="58" ht="18" customHeight="1" s="115"/>
+    <row r="59" ht="18" customHeight="1" s="115"/>
+    <row r="60" ht="18" customHeight="1" s="115"/>
+    <row r="61" ht="18" customHeight="1" s="115"/>
+    <row r="62" ht="18" customHeight="1" s="115"/>
+    <row r="63" ht="18" customHeight="1" s="115"/>
+    <row r="64" ht="18" customHeight="1" s="115"/>
+    <row r="65" ht="18" customHeight="1" s="115"/>
+    <row r="66" ht="18" customHeight="1" s="115"/>
+    <row r="67" ht="18" customHeight="1" s="115"/>
+    <row r="68" ht="18" customHeight="1" s="115"/>
+    <row r="69" ht="18" customHeight="1" s="115"/>
+    <row r="70" ht="18" customHeight="1" s="115"/>
+    <row r="71" ht="18" customHeight="1" s="115"/>
+    <row r="72" ht="18" customHeight="1" s="115"/>
+    <row r="73" ht="18" customHeight="1" s="115"/>
+    <row r="74" ht="18" customHeight="1" s="115"/>
+    <row r="75" ht="18" customHeight="1" s="115"/>
+    <row r="76" ht="18" customHeight="1" s="115"/>
+    <row r="77" ht="18" customHeight="1" s="115"/>
+    <row r="78" ht="18" customHeight="1" s="115"/>
+    <row r="79" ht="18" customHeight="1" s="115"/>
+    <row r="80" ht="18" customHeight="1" s="115"/>
+    <row r="81" ht="18" customHeight="1" s="115"/>
+    <row r="82" ht="18" customHeight="1" s="115"/>
+    <row r="83" ht="18" customHeight="1" s="115"/>
+    <row r="84" ht="18" customHeight="1" s="115"/>
+    <row r="85" ht="18" customHeight="1" s="115"/>
+    <row r="86" ht="18" customHeight="1" s="115"/>
+    <row r="87" ht="18" customHeight="1" s="115"/>
+    <row r="88" ht="18" customHeight="1" s="115"/>
+    <row r="89" ht="18" customHeight="1" s="115"/>
+    <row r="90" ht="18" customHeight="1" s="115"/>
+    <row r="91" ht="18" customHeight="1" s="115"/>
+    <row r="92" ht="18" customHeight="1" s="115"/>
+    <row r="93" ht="18" customHeight="1" s="115"/>
+    <row r="94" ht="18" customHeight="1" s="115"/>
+    <row r="95" ht="18" customHeight="1" s="115"/>
+    <row r="96" ht="18" customHeight="1" s="115"/>
+    <row r="97" ht="18" customHeight="1" s="115"/>
+    <row r="98" ht="18" customHeight="1" s="115"/>
+    <row r="99" ht="18" customHeight="1" s="115"/>
+    <row r="100" ht="18" customHeight="1" s="115"/>
+    <row r="101" ht="18" customHeight="1" s="115"/>
+    <row r="102" ht="18" customHeight="1" s="115"/>
+    <row r="103" ht="18" customHeight="1" s="115"/>
+    <row r="104" ht="18" customHeight="1" s="115"/>
+    <row r="105" ht="18" customHeight="1" s="115"/>
+    <row r="106" ht="18" customHeight="1" s="115"/>
+    <row r="107" ht="18" customHeight="1" s="115"/>
+    <row r="108" ht="18" customHeight="1" s="115"/>
+    <row r="109" ht="18" customHeight="1" s="115"/>
+    <row r="110" ht="18" customHeight="1" s="115"/>
+    <row r="111" ht="18" customHeight="1" s="115"/>
+    <row r="112" ht="18" customHeight="1" s="115"/>
+    <row r="113" ht="18" customHeight="1" s="115"/>
+    <row r="114" ht="18" customHeight="1" s="115"/>
+    <row r="115" ht="18" customHeight="1" s="115"/>
+    <row r="116" ht="18" customHeight="1" s="115"/>
+    <row r="117" ht="18" customHeight="1" s="115"/>
+    <row r="118" ht="18" customHeight="1" s="115"/>
+    <row r="119" ht="18" customHeight="1" s="115"/>
+    <row r="120" ht="18" customHeight="1" s="115"/>
+    <row r="121" ht="18" customHeight="1" s="115"/>
+    <row r="122" ht="18" customHeight="1" s="115"/>
+    <row r="123" ht="18" customHeight="1" s="115"/>
+    <row r="124" ht="18" customHeight="1" s="115"/>
+    <row r="125" ht="18" customHeight="1" s="115"/>
+    <row r="126" ht="18" customHeight="1" s="115"/>
+    <row r="127" ht="18" customHeight="1" s="115"/>
+    <row r="128" ht="18" customHeight="1" s="115"/>
+    <row r="129" ht="18" customHeight="1" s="115"/>
+    <row r="130" ht="18" customHeight="1" s="115"/>
+    <row r="131" ht="18" customHeight="1" s="115"/>
+    <row r="132" ht="18" customHeight="1" s="115"/>
+    <row r="133" ht="18" customHeight="1" s="115"/>
+    <row r="134" ht="18" customHeight="1" s="115"/>
+    <row r="135" ht="18" customHeight="1" s="115"/>
+    <row r="136" ht="18" customHeight="1" s="115"/>
+    <row r="137" ht="18" customHeight="1" s="115"/>
+    <row r="138" ht="18" customHeight="1" s="115"/>
+    <row r="139" ht="18" customHeight="1" s="115"/>
+    <row r="140" ht="18" customHeight="1" s="115"/>
+    <row r="141" ht="18" customHeight="1" s="115"/>
+    <row r="142" ht="18" customHeight="1" s="115"/>
+    <row r="143" ht="18" customHeight="1" s="115"/>
+    <row r="144" ht="18" customHeight="1" s="115"/>
+    <row r="145" ht="18" customHeight="1" s="115"/>
+    <row r="146" ht="18" customHeight="1" s="115"/>
+    <row r="147" ht="18" customHeight="1" s="115"/>
+    <row r="148" ht="18" customHeight="1" s="115"/>
+    <row r="149" ht="18" customHeight="1" s="115"/>
+    <row r="150" ht="18" customHeight="1" s="115"/>
+    <row r="151" ht="18" customHeight="1" s="115"/>
+    <row r="152" ht="18" customHeight="1" s="115"/>
+    <row r="153" ht="18" customHeight="1" s="115"/>
+    <row r="154" ht="18" customHeight="1" s="115"/>
+    <row r="155" ht="18" customHeight="1" s="115"/>
+    <row r="156" ht="18" customHeight="1" s="115"/>
+    <row r="157" ht="18" customHeight="1" s="115"/>
+    <row r="158" ht="18" customHeight="1" s="115"/>
+    <row r="159" ht="18" customHeight="1" s="115"/>
+    <row r="160" ht="18" customHeight="1" s="115"/>
+    <row r="161" ht="18" customHeight="1" s="115"/>
+    <row r="162" ht="18" customHeight="1" s="115"/>
+    <row r="163" ht="18" customHeight="1" s="115"/>
+    <row r="164" ht="18" customHeight="1" s="115"/>
+    <row r="165" ht="18" customHeight="1" s="115"/>
+    <row r="166" ht="18" customHeight="1" s="115"/>
+    <row r="167" ht="18" customHeight="1" s="115"/>
+    <row r="168" ht="18" customHeight="1" s="115"/>
+    <row r="169" ht="18" customHeight="1" s="115"/>
+    <row r="170" ht="18" customHeight="1" s="115"/>
+    <row r="171" ht="18" customHeight="1" s="115"/>
+    <row r="172" ht="18" customHeight="1" s="115"/>
+    <row r="173" ht="18" customHeight="1" s="115"/>
+    <row r="174" ht="18" customHeight="1" s="115"/>
+    <row r="175" ht="18" customHeight="1" s="115"/>
+    <row r="176" ht="18" customHeight="1" s="115"/>
+    <row r="177" ht="18" customHeight="1" s="115"/>
+    <row r="178" ht="18" customHeight="1" s="115"/>
+    <row r="179" ht="18" customHeight="1" s="115"/>
+    <row r="180" ht="18" customHeight="1" s="115"/>
+    <row r="181" ht="18" customHeight="1" s="115"/>
+    <row r="182" ht="18" customHeight="1" s="115"/>
+    <row r="183" ht="18" customHeight="1" s="115"/>
+    <row r="184" ht="18" customHeight="1" s="115"/>
+    <row r="185" ht="18" customHeight="1" s="115"/>
+    <row r="186" ht="18" customHeight="1" s="115"/>
+    <row r="187" ht="18" customHeight="1" s="115"/>
+    <row r="188" ht="18" customHeight="1" s="115"/>
+    <row r="189" ht="18" customHeight="1" s="115"/>
+    <row r="190" ht="18" customHeight="1" s="115"/>
+    <row r="191" ht="18" customHeight="1" s="115"/>
+    <row r="192" ht="18" customHeight="1" s="115"/>
+    <row r="193" ht="18" customHeight="1" s="115"/>
+    <row r="194" ht="18" customHeight="1" s="115"/>
+    <row r="195" ht="18" customHeight="1" s="115"/>
+    <row r="196" ht="18" customHeight="1" s="115"/>
+    <row r="197" ht="18" customHeight="1" s="115"/>
+    <row r="198" ht="18" customHeight="1" s="115"/>
+    <row r="199" ht="18" customHeight="1" s="115"/>
+    <row r="200" ht="18" customHeight="1" s="115"/>
+    <row r="201" ht="18" customHeight="1" s="115"/>
+    <row r="202" ht="18" customHeight="1" s="115"/>
+    <row r="203" ht="18" customHeight="1" s="115"/>
+    <row r="204" ht="18" customHeight="1" s="115"/>
+    <row r="205" ht="18" customHeight="1" s="115"/>
+    <row r="206" ht="18" customHeight="1" s="115"/>
+    <row r="207" ht="18" customHeight="1" s="115"/>
+    <row r="208" ht="18" customHeight="1" s="115"/>
+    <row r="209" ht="18" customHeight="1" s="115"/>
+    <row r="210" ht="18" customHeight="1" s="115"/>
+    <row r="211" ht="18" customHeight="1" s="115"/>
+    <row r="212" ht="18" customHeight="1" s="115"/>
+    <row r="213" ht="18" customHeight="1" s="115"/>
+    <row r="214" ht="18" customHeight="1" s="115"/>
+    <row r="215" ht="18" customHeight="1" s="115"/>
+    <row r="216" ht="18" customHeight="1" s="115"/>
+    <row r="217" ht="18" customHeight="1" s="115"/>
+    <row r="218" ht="18" customHeight="1" s="115"/>
+    <row r="219" ht="18" customHeight="1" s="115"/>
+    <row r="220" ht="18" customHeight="1" s="115"/>
+    <row r="221" ht="18" customHeight="1" s="115"/>
+    <row r="222" ht="18" customHeight="1" s="115"/>
+    <row r="223" ht="18" customHeight="1" s="115"/>
+    <row r="224" ht="18" customHeight="1" s="115"/>
+    <row r="225" ht="18" customHeight="1" s="115"/>
+    <row r="226" ht="18" customHeight="1" s="115"/>
+    <row r="227" ht="18" customHeight="1" s="115"/>
+    <row r="228" ht="18" customHeight="1" s="115"/>
+    <row r="229" ht="18" customHeight="1" s="115"/>
+    <row r="230" ht="18" customHeight="1" s="115"/>
+    <row r="231" ht="18" customHeight="1" s="115"/>
+    <row r="232" ht="18" customHeight="1" s="115"/>
+    <row r="233" ht="18" customHeight="1" s="115"/>
+    <row r="234" ht="18" customHeight="1" s="115"/>
+    <row r="235" ht="18" customHeight="1" s="115"/>
+    <row r="236" ht="18" customHeight="1" s="115"/>
+    <row r="237" ht="18" customHeight="1" s="115"/>
+    <row r="238" ht="18" customHeight="1" s="115"/>
+    <row r="239" ht="18" customHeight="1" s="115"/>
+    <row r="240" ht="18" customHeight="1" s="115"/>
+    <row r="241" ht="18" customHeight="1" s="115"/>
+    <row r="242" ht="18" customHeight="1" s="115"/>
+    <row r="243" ht="18" customHeight="1" s="115"/>
+    <row r="244" ht="18" customHeight="1" s="115"/>
+    <row r="245" ht="18" customHeight="1" s="115"/>
+    <row r="246" ht="18" customHeight="1" s="115"/>
+    <row r="247" ht="18" customHeight="1" s="115"/>
+    <row r="248" ht="18" customHeight="1" s="115"/>
+    <row r="249" ht="18" customHeight="1" s="115"/>
+    <row r="250" ht="18" customHeight="1" s="115"/>
+    <row r="251" ht="18" customHeight="1" s="115"/>
+    <row r="252" ht="18" customHeight="1" s="115"/>
+    <row r="253" ht="18" customHeight="1" s="115"/>
+    <row r="254" ht="18" customHeight="1" s="115"/>
+    <row r="255" ht="18" customHeight="1" s="115"/>
+    <row r="256" ht="18" customHeight="1" s="115"/>
+    <row r="257" ht="18" customHeight="1" s="115"/>
+    <row r="258" ht="18" customHeight="1" s="115"/>
+    <row r="259" ht="18" customHeight="1" s="115"/>
+    <row r="260" ht="18" customHeight="1" s="115"/>
+    <row r="261" ht="18" customHeight="1" s="115"/>
+    <row r="262" ht="18" customHeight="1" s="115"/>
+    <row r="263" ht="18" customHeight="1" s="115"/>
+    <row r="264" ht="18" customHeight="1" s="115"/>
+    <row r="265" ht="18" customHeight="1" s="115"/>
+    <row r="266" ht="18" customHeight="1" s="115"/>
+    <row r="267" ht="18" customHeight="1" s="115"/>
+    <row r="268" ht="18" customHeight="1" s="115"/>
+    <row r="269" ht="18" customHeight="1" s="115"/>
+    <row r="270" ht="18" customHeight="1" s="115"/>
+    <row r="271" ht="18" customHeight="1" s="115"/>
+    <row r="272" ht="18" customHeight="1" s="115"/>
+    <row r="273" ht="18" customHeight="1" s="115"/>
+    <row r="274" ht="18" customHeight="1" s="115"/>
+    <row r="275" ht="18" customHeight="1" s="115"/>
+    <row r="276" ht="18" customHeight="1" s="115"/>
+    <row r="277" ht="18" customHeight="1" s="115"/>
+    <row r="278" ht="18" customHeight="1" s="115"/>
+    <row r="279" ht="18" customHeight="1" s="115"/>
+    <row r="280" ht="18" customHeight="1" s="115"/>
+    <row r="281" ht="18" customHeight="1" s="115"/>
+    <row r="282" ht="18" customHeight="1" s="115"/>
+    <row r="283" ht="18" customHeight="1" s="115"/>
+    <row r="284" ht="18" customHeight="1" s="115"/>
+    <row r="285" ht="18" customHeight="1" s="115"/>
+    <row r="286" ht="18" customHeight="1" s="115"/>
+    <row r="287" ht="18" customHeight="1" s="115"/>
+    <row r="288" ht="18" customHeight="1" s="115"/>
+    <row r="289" ht="18" customHeight="1" s="115"/>
+    <row r="290" ht="18" customHeight="1" s="115"/>
+    <row r="291" ht="18" customHeight="1" s="115"/>
+    <row r="292" ht="18" customHeight="1" s="115"/>
+    <row r="293" ht="18" customHeight="1" s="115"/>
+    <row r="294" ht="18" customHeight="1" s="115"/>
+    <row r="295" ht="18" customHeight="1" s="115"/>
+    <row r="296" ht="18" customHeight="1" s="115"/>
+    <row r="297" ht="18" customHeight="1" s="115"/>
+    <row r="298" ht="18" customHeight="1" s="115"/>
+    <row r="299" ht="18" customHeight="1" s="115"/>
+    <row r="300" ht="18" customHeight="1" s="115"/>
+    <row r="301" ht="18" customHeight="1" s="115"/>
+    <row r="302" ht="18" customHeight="1" s="115"/>
+    <row r="303" ht="18" customHeight="1" s="115"/>
+    <row r="304" ht="18" customHeight="1" s="115"/>
+    <row r="305" ht="18" customHeight="1" s="115"/>
+    <row r="306" ht="18" customHeight="1" s="115"/>
+    <row r="307" ht="18" customHeight="1" s="115"/>
+    <row r="308" ht="18" customHeight="1" s="115"/>
+    <row r="309" ht="18" customHeight="1" s="115"/>
+    <row r="310" ht="18" customHeight="1" s="115"/>
+    <row r="311" ht="18" customHeight="1" s="115"/>
+    <row r="312" ht="18" customHeight="1" s="115"/>
+    <row r="313" ht="18" customHeight="1" s="115"/>
+    <row r="314" ht="18" customHeight="1" s="115"/>
+    <row r="315" ht="18" customHeight="1" s="115"/>
+    <row r="316" ht="18" customHeight="1" s="115"/>
+    <row r="317" ht="18" customHeight="1" s="115"/>
+    <row r="318" ht="18" customHeight="1" s="115"/>
+    <row r="319" ht="18" customHeight="1" s="115"/>
+    <row r="320" ht="18" customHeight="1" s="115"/>
+    <row r="321" ht="18" customHeight="1" s="115"/>
+    <row r="322" ht="18" customHeight="1" s="115"/>
+    <row r="323" ht="18" customHeight="1" s="115"/>
+    <row r="324" ht="18" customHeight="1" s="115"/>
+    <row r="325" ht="18" customHeight="1" s="115"/>
+    <row r="326" ht="18" customHeight="1" s="115"/>
+    <row r="327" ht="18" customHeight="1" s="115"/>
+    <row r="328" ht="18" customHeight="1" s="115"/>
+    <row r="329" ht="18" customHeight="1" s="115"/>
+    <row r="330" ht="18" customHeight="1" s="115"/>
+    <row r="331" ht="18" customHeight="1" s="115"/>
+    <row r="332" ht="18" customHeight="1" s="115"/>
+    <row r="333" ht="18" customHeight="1" s="115"/>
+    <row r="334" ht="18" customHeight="1" s="115"/>
+    <row r="335" ht="18" customHeight="1" s="115"/>
+    <row r="336" ht="18" customHeight="1" s="115"/>
+    <row r="337" ht="18" customHeight="1" s="115"/>
+    <row r="338" ht="18" customHeight="1" s="115"/>
+    <row r="339" ht="18" customHeight="1" s="115"/>
+    <row r="340" ht="18" customHeight="1" s="115"/>
+    <row r="341" ht="18" customHeight="1" s="115"/>
+    <row r="342" ht="18" customHeight="1" s="115"/>
+    <row r="343" ht="18" customHeight="1" s="115"/>
+    <row r="344" ht="18" customHeight="1" s="115"/>
+    <row r="345" ht="18" customHeight="1" s="115"/>
+    <row r="346" ht="18" customHeight="1" s="115"/>
+    <row r="347" ht="18" customHeight="1" s="115"/>
+    <row r="348" ht="18" customHeight="1" s="115"/>
+    <row r="349" ht="18" customHeight="1" s="115"/>
+    <row r="350" ht="18" customHeight="1" s="115"/>
+    <row r="351" ht="18" customHeight="1" s="115"/>
+    <row r="352" ht="18" customHeight="1" s="115"/>
+    <row r="353" ht="18" customHeight="1" s="115"/>
+    <row r="354" ht="18" customHeight="1" s="115"/>
+    <row r="355" ht="18" customHeight="1" s="115"/>
+    <row r="356" ht="18" customHeight="1" s="115"/>
+    <row r="357" ht="18" customHeight="1" s="115"/>
+    <row r="358" ht="18" customHeight="1" s="115"/>
+    <row r="359" ht="18" customHeight="1" s="115"/>
+    <row r="360" ht="18" customHeight="1" s="115"/>
+    <row r="361" ht="18" customHeight="1" s="115"/>
+    <row r="362" ht="18" customHeight="1" s="115"/>
+    <row r="363" ht="18" customHeight="1" s="115"/>
+    <row r="364" ht="18" customHeight="1" s="115"/>
+    <row r="365" ht="18" customHeight="1" s="115"/>
+    <row r="366" ht="18" customHeight="1" s="115"/>
+    <row r="367" ht="18" customHeight="1" s="115"/>
+    <row r="368" ht="18" customHeight="1" s="115"/>
+    <row r="369" ht="18" customHeight="1" s="115"/>
+    <row r="370" ht="18" customHeight="1" s="115"/>
+    <row r="371" ht="18" customHeight="1" s="115"/>
+    <row r="372" ht="18" customHeight="1" s="115"/>
+    <row r="373" ht="18" customHeight="1" s="115"/>
+    <row r="374" ht="18" customHeight="1" s="115"/>
+    <row r="375" ht="18" customHeight="1" s="115"/>
+    <row r="376" ht="18" customHeight="1" s="115"/>
+    <row r="377" ht="18" customHeight="1" s="115"/>
+    <row r="378" ht="18" customHeight="1" s="115"/>
+    <row r="379" ht="18" customHeight="1" s="115"/>
+    <row r="380" ht="18" customHeight="1" s="115"/>
+    <row r="381" ht="18" customHeight="1" s="115"/>
+    <row r="382" ht="18" customHeight="1" s="115"/>
+    <row r="383" ht="18" customHeight="1" s="115"/>
+    <row r="384" ht="18" customHeight="1" s="115"/>
+    <row r="385" ht="18" customHeight="1" s="115"/>
+    <row r="386" ht="18" customHeight="1" s="115"/>
+    <row r="387" ht="18" customHeight="1" s="115"/>
+    <row r="388" ht="18" customHeight="1" s="115"/>
+    <row r="389" ht="18" customHeight="1" s="115"/>
+    <row r="390" ht="18" customHeight="1" s="115"/>
+    <row r="391" ht="18" customHeight="1" s="115"/>
+    <row r="392" ht="18" customHeight="1" s="115"/>
+    <row r="393" ht="18" customHeight="1" s="115"/>
+    <row r="394" ht="18" customHeight="1" s="115"/>
+    <row r="395" ht="18" customHeight="1" s="115"/>
+    <row r="396" ht="18" customHeight="1" s="115"/>
+    <row r="397" ht="18" customHeight="1" s="115"/>
+    <row r="398" ht="18" customHeight="1" s="115"/>
+    <row r="399" ht="18" customHeight="1" s="115"/>
+    <row r="400" ht="18" customHeight="1" s="115"/>
+    <row r="401" ht="18" customHeight="1" s="115"/>
+    <row r="402" ht="18" customHeight="1" s="115"/>
+    <row r="403" ht="18" customHeight="1" s="115"/>
+    <row r="404" ht="18" customHeight="1" s="115"/>
+    <row r="405" ht="18" customHeight="1" s="115"/>
+    <row r="406" ht="18" customHeight="1" s="115"/>
+    <row r="407" ht="18" customHeight="1" s="115"/>
+    <row r="408" ht="18" customHeight="1" s="115"/>
+    <row r="409" ht="18" customHeight="1" s="115"/>
+    <row r="410" ht="18" customHeight="1" s="115"/>
+    <row r="411" ht="18" customHeight="1" s="115"/>
+    <row r="412" ht="18" customHeight="1" s="115"/>
+    <row r="413" ht="18" customHeight="1" s="115"/>
+    <row r="414" ht="18" customHeight="1" s="115"/>
+    <row r="415" ht="18" customHeight="1" s="115"/>
+    <row r="416" ht="18" customHeight="1" s="115"/>
+    <row r="417" ht="18" customHeight="1" s="115"/>
+    <row r="418" ht="18" customHeight="1" s="115"/>
+    <row r="419" ht="18" customHeight="1" s="115"/>
+    <row r="420" ht="18" customHeight="1" s="115"/>
+    <row r="421" ht="18" customHeight="1" s="115"/>
+    <row r="422" ht="18" customHeight="1" s="115"/>
+    <row r="423" ht="18" customHeight="1" s="115"/>
+    <row r="424" ht="18" customHeight="1" s="115"/>
+    <row r="425" ht="18" customHeight="1" s="115"/>
+    <row r="426" ht="18" customHeight="1" s="115"/>
+    <row r="427" ht="18" customHeight="1" s="115"/>
+    <row r="428" ht="18" customHeight="1" s="115"/>
+    <row r="429" ht="18" customHeight="1" s="115"/>
+    <row r="430" ht="18" customHeight="1" s="115"/>
+    <row r="431" ht="18" customHeight="1" s="115"/>
+    <row r="432" ht="18" customHeight="1" s="115"/>
+    <row r="433" ht="18" customHeight="1" s="115"/>
+    <row r="434" ht="18" customHeight="1" s="115"/>
+    <row r="435" ht="18" customHeight="1" s="115"/>
+    <row r="436" ht="18" customHeight="1" s="115"/>
+    <row r="437" ht="18" customHeight="1" s="115"/>
+    <row r="438" ht="18" customHeight="1" s="115"/>
+    <row r="439" ht="18" customHeight="1" s="115"/>
+    <row r="440" ht="18" customHeight="1" s="115"/>
+    <row r="441" ht="18" customHeight="1" s="115"/>
+    <row r="442" ht="18" customHeight="1" s="115"/>
+    <row r="443" ht="18" customHeight="1" s="115"/>
+    <row r="444" ht="18" customHeight="1" s="115"/>
+    <row r="445" ht="18" customHeight="1" s="115"/>
+    <row r="446" ht="18" customHeight="1" s="115"/>
+    <row r="447" ht="18" customHeight="1" s="115"/>
+    <row r="448" ht="18" customHeight="1" s="115"/>
+    <row r="449" ht="18" customHeight="1" s="115"/>
+    <row r="450" ht="18" customHeight="1" s="115"/>
+    <row r="451" ht="18" customHeight="1" s="115"/>
+    <row r="452" ht="18" customHeight="1" s="115"/>
+    <row r="453" ht="18" customHeight="1" s="115"/>
+    <row r="454" ht="18" customHeight="1" s="115"/>
+    <row r="455" ht="18" customHeight="1" s="115"/>
+    <row r="456" ht="18" customHeight="1" s="115"/>
+    <row r="457" ht="18" customHeight="1" s="115"/>
+    <row r="458" ht="18" customHeight="1" s="115"/>
+    <row r="459" ht="18" customHeight="1" s="115"/>
+    <row r="460" ht="18" customHeight="1" s="115"/>
+    <row r="461" ht="18" customHeight="1" s="115"/>
+    <row r="462" ht="18" customHeight="1" s="115"/>
+    <row r="463" ht="18" customHeight="1" s="115"/>
+    <row r="464" ht="18" customHeight="1" s="115"/>
+    <row r="465" ht="18" customHeight="1" s="115"/>
+    <row r="466" ht="18" customHeight="1" s="115"/>
+    <row r="467" ht="18" customHeight="1" s="115"/>
+    <row r="468" ht="18" customHeight="1" s="115"/>
+    <row r="469" ht="18" customHeight="1" s="115"/>
+    <row r="470" ht="18" customHeight="1" s="115"/>
+    <row r="471" ht="18" customHeight="1" s="115"/>
+    <row r="472" ht="18" customHeight="1" s="115"/>
+    <row r="473" ht="18" customHeight="1" s="115"/>
+    <row r="474" ht="18" customHeight="1" s="115"/>
+    <row r="475" ht="18" customHeight="1" s="115"/>
+    <row r="476" ht="18" customHeight="1" s="115"/>
+    <row r="477" ht="18" customHeight="1" s="115"/>
+    <row r="478" ht="18" customHeight="1" s="115"/>
+    <row r="479" ht="18" customHeight="1" s="115"/>
+    <row r="480" ht="18" customHeight="1" s="115"/>
+    <row r="481" ht="18" customHeight="1" s="115"/>
+    <row r="482" ht="18" customHeight="1" s="115"/>
+    <row r="483" ht="18" customHeight="1" s="115"/>
+    <row r="484" ht="18" customHeight="1" s="115"/>
+    <row r="485" ht="18" customHeight="1" s="115"/>
+    <row r="486" ht="18" customHeight="1" s="115"/>
+    <row r="487" ht="18" customHeight="1" s="115"/>
+    <row r="488" ht="18" customHeight="1" s="115"/>
+    <row r="489" ht="18" customHeight="1" s="115"/>
+    <row r="490" ht="18" customHeight="1" s="115"/>
+    <row r="491" ht="18" customHeight="1" s="115"/>
+    <row r="492" ht="18" customHeight="1" s="115"/>
+    <row r="493" ht="18" customHeight="1" s="115"/>
+    <row r="494" ht="18" customHeight="1" s="115"/>
+    <row r="495" ht="18" customHeight="1" s="115"/>
+    <row r="496" ht="18" customHeight="1" s="115"/>
+    <row r="497" ht="18" customHeight="1" s="115"/>
+    <row r="498" ht="18" customHeight="1" s="115"/>
+    <row r="499" ht="18" customHeight="1" s="115"/>
+    <row r="500" ht="18" customHeight="1" s="115"/>
+    <row r="501" ht="18" customHeight="1" s="115"/>
+    <row r="502" ht="18" customHeight="1" s="115"/>
+    <row r="503" ht="18" customHeight="1" s="115"/>
+    <row r="504" ht="18" customHeight="1" s="115"/>
+    <row r="505" ht="18" customHeight="1" s="115"/>
+    <row r="506" ht="18" customHeight="1" s="115"/>
+    <row r="507" ht="18" customHeight="1" s="115"/>
+    <row r="508" ht="18" customHeight="1" s="115"/>
+    <row r="509" ht="18" customHeight="1" s="115"/>
+    <row r="510" ht="18" customHeight="1" s="115"/>
+    <row r="511" ht="18" customHeight="1" s="115"/>
+    <row r="512" ht="18" customHeight="1" s="115"/>
+    <row r="513" ht="18" customHeight="1" s="115"/>
+    <row r="514" ht="18" customHeight="1" s="115"/>
+    <row r="515" ht="18" customHeight="1" s="115"/>
+    <row r="516" ht="18" customHeight="1" s="115"/>
+    <row r="517" ht="18" customHeight="1" s="115"/>
+    <row r="518" ht="18" customHeight="1" s="115"/>
+    <row r="519" ht="18" customHeight="1" s="115"/>
+    <row r="520" ht="18" customHeight="1" s="115"/>
+    <row r="521" ht="18" customHeight="1" s="115"/>
+    <row r="522" ht="18" customHeight="1" s="115"/>
+    <row r="523" ht="18" customHeight="1" s="115"/>
+    <row r="524" ht="18" customHeight="1" s="115"/>
+    <row r="525" ht="18" customHeight="1" s="115"/>
+    <row r="526" ht="18" customHeight="1" s="115"/>
+    <row r="527" ht="18" customHeight="1" s="115"/>
+    <row r="528" ht="18" customHeight="1" s="115"/>
+    <row r="529" ht="18" customHeight="1" s="115"/>
+    <row r="530" ht="18" customHeight="1" s="115"/>
+    <row r="531" ht="18" customHeight="1" s="115"/>
+    <row r="532" ht="18" customHeight="1" s="115"/>
+    <row r="533" ht="18" customHeight="1" s="115"/>
+    <row r="534" ht="18" customHeight="1" s="115"/>
+    <row r="535" ht="18" customHeight="1" s="115"/>
+    <row r="536" ht="18" customHeight="1" s="115"/>
+    <row r="537" ht="18" customHeight="1" s="115"/>
+    <row r="538" ht="18" customHeight="1" s="115"/>
+    <row r="539" ht="18" customHeight="1" s="115"/>
+    <row r="540" ht="18" customHeight="1" s="115"/>
+    <row r="541" ht="18" customHeight="1" s="115"/>
+    <row r="542" ht="18" customHeight="1" s="115"/>
+    <row r="543" ht="18" customHeight="1" s="115"/>
+    <row r="544" ht="18" customHeight="1" s="115"/>
+    <row r="545" ht="18" customHeight="1" s="115"/>
+    <row r="546" ht="18" customHeight="1" s="115"/>
+    <row r="547" ht="18" customHeight="1" s="115"/>
+    <row r="548" ht="18" customHeight="1" s="115"/>
+    <row r="549" ht="18" customHeight="1" s="115"/>
+    <row r="550" ht="18" customHeight="1" s="115"/>
+    <row r="551" ht="18" customHeight="1" s="115"/>
+    <row r="552" ht="18" customHeight="1" s="115"/>
+    <row r="553" ht="18" customHeight="1" s="115"/>
+    <row r="554" ht="18" customHeight="1" s="115"/>
+    <row r="555" ht="18" customHeight="1" s="115"/>
+    <row r="556" ht="18" customHeight="1" s="115"/>
+    <row r="557" ht="18" customHeight="1" s="115"/>
+    <row r="558" ht="18" customHeight="1" s="115"/>
+    <row r="559" ht="18" customHeight="1" s="115"/>
+    <row r="560" ht="18" customHeight="1" s="115"/>
+    <row r="561" ht="18" customHeight="1" s="115"/>
+    <row r="562" ht="18" customHeight="1" s="115"/>
+    <row r="563" ht="18" customHeight="1" s="115"/>
+    <row r="564" ht="18" customHeight="1" s="115"/>
+    <row r="565" ht="18" customHeight="1" s="115"/>
+    <row r="566" ht="18" customHeight="1" s="115"/>
+    <row r="567" ht="18" customHeight="1" s="115"/>
+    <row r="568" ht="18" customHeight="1" s="115"/>
+    <row r="569" ht="18" customHeight="1" s="115"/>
+    <row r="570" ht="18" customHeight="1" s="115"/>
+    <row r="571" ht="18" customHeight="1" s="115"/>
+    <row r="572" ht="18" customHeight="1" s="115"/>
+    <row r="573" ht="18" customHeight="1" s="115"/>
+    <row r="574" ht="18" customHeight="1" s="115"/>
+    <row r="575" ht="18" customHeight="1" s="115"/>
+    <row r="576" ht="18" customHeight="1" s="115"/>
+    <row r="577" ht="18" customHeight="1" s="115"/>
+    <row r="578" ht="18" customHeight="1" s="115"/>
+    <row r="579" ht="18" customHeight="1" s="115"/>
+    <row r="580" ht="18" customHeight="1" s="115"/>
+    <row r="581" ht="18" customHeight="1" s="115"/>
+    <row r="582" ht="18" customHeight="1" s="115"/>
+    <row r="583" ht="18" customHeight="1" s="115"/>
+    <row r="584" ht="18" customHeight="1" s="115"/>
+    <row r="585" ht="18" customHeight="1" s="115"/>
+    <row r="586" ht="18" customHeight="1" s="115"/>
+    <row r="587" ht="18" customHeight="1" s="115"/>
+    <row r="588" ht="18" customHeight="1" s="115"/>
+    <row r="589" ht="18" customHeight="1" s="115"/>
+    <row r="590" ht="18" customHeight="1" s="115"/>
+    <row r="591" ht="18" customHeight="1" s="115"/>
+    <row r="592" ht="18" customHeight="1" s="115"/>
+    <row r="593" ht="18" customHeight="1" s="115"/>
+    <row r="594" ht="18" customHeight="1" s="115"/>
+    <row r="595" ht="18" customHeight="1" s="115"/>
+    <row r="596" ht="18" customHeight="1" s="115"/>
+    <row r="597" ht="18" customHeight="1" s="115"/>
+    <row r="598" ht="18" customHeight="1" s="115"/>
+    <row r="599" ht="18" customHeight="1" s="115"/>
+    <row r="600" ht="18" customHeight="1" s="115"/>
+    <row r="601" ht="18" customHeight="1" s="115"/>
+    <row r="602" ht="18" customHeight="1" s="115"/>
+    <row r="603" ht="18" customHeight="1" s="115"/>
+    <row r="604" ht="18" customHeight="1" s="115"/>
+    <row r="605" ht="18" customHeight="1" s="115"/>
+    <row r="606" ht="18" customHeight="1" s="115"/>
+    <row r="607" ht="18" customHeight="1" s="115"/>
+    <row r="608" ht="18" customHeight="1" s="115"/>
+    <row r="609" ht="18" customHeight="1" s="115"/>
+    <row r="610" ht="18" customHeight="1" s="115"/>
+    <row r="611" ht="18" customHeight="1" s="115"/>
+    <row r="612" ht="18" customHeight="1" s="115"/>
+    <row r="613" ht="18" customHeight="1" s="115"/>
+    <row r="614" ht="18" customHeight="1" s="115"/>
+    <row r="615" ht="18" customHeight="1" s="115"/>
+    <row r="616" ht="18" customHeight="1" s="115"/>
+    <row r="617" ht="18" customHeight="1" s="115"/>
+    <row r="618" ht="18" customHeight="1" s="115"/>
+    <row r="619" ht="18" customHeight="1" s="115"/>
+    <row r="620" ht="18" customHeight="1" s="115"/>
+    <row r="621" ht="18" customHeight="1" s="115"/>
+    <row r="622" ht="18" customHeight="1" s="115"/>
+    <row r="623" ht="18" customHeight="1" s="115"/>
+    <row r="624" ht="18" customHeight="1" s="115"/>
+    <row r="625" ht="18" customHeight="1" s="115"/>
+    <row r="626" ht="18" customHeight="1" s="115"/>
+    <row r="627" ht="18" customHeight="1" s="115"/>
+    <row r="628" ht="18" customHeight="1" s="115"/>
+    <row r="629" ht="18" customHeight="1" s="115"/>
+    <row r="630" ht="18" customHeight="1" s="115"/>
+    <row r="631" ht="18" customHeight="1" s="115"/>
+    <row r="632" ht="18" customHeight="1" s="115"/>
+    <row r="633" ht="18" customHeight="1" s="115"/>
+    <row r="634" ht="18" customHeight="1" s="115"/>
+    <row r="635" ht="18" customHeight="1" s="115"/>
+    <row r="636" ht="18" customHeight="1" s="115"/>
+    <row r="637" ht="18" customHeight="1" s="115"/>
+    <row r="638" ht="18" customHeight="1" s="115"/>
+    <row r="639" ht="18" customHeight="1" s="115"/>
+    <row r="640" ht="18" customHeight="1" s="115"/>
+    <row r="641" ht="18" customHeight="1" s="115"/>
+    <row r="642" ht="18" customHeight="1" s="115"/>
+    <row r="643" ht="18" customHeight="1" s="115"/>
+    <row r="644" ht="18" customHeight="1" s="115"/>
+    <row r="645" ht="18" customHeight="1" s="115"/>
+    <row r="646" ht="18" customHeight="1" s="115"/>
+    <row r="647" ht="18" customHeight="1" s="115"/>
+    <row r="648" ht="18" customHeight="1" s="115"/>
+    <row r="649" ht="18" customHeight="1" s="115"/>
+    <row r="650" ht="18" customHeight="1" s="115"/>
+    <row r="651" ht="18" customHeight="1" s="115"/>
+    <row r="652" ht="18" customHeight="1" s="115"/>
+    <row r="653" ht="18" customHeight="1" s="115"/>
+    <row r="654" ht="18" customHeight="1" s="115"/>
+    <row r="655" ht="18" customHeight="1" s="115"/>
+    <row r="656" ht="18" customHeight="1" s="115"/>
+    <row r="657" ht="18" customHeight="1" s="115"/>
+    <row r="658" ht="18" customHeight="1" s="115"/>
+    <row r="659" ht="18" customHeight="1" s="115"/>
+    <row r="660" ht="18" customHeight="1" s="115"/>
+    <row r="661" ht="18" customHeight="1" s="115"/>
+    <row r="662" ht="18" customHeight="1" s="115"/>
+    <row r="663" ht="18" customHeight="1" s="115"/>
+    <row r="664" ht="18" customHeight="1" s="115"/>
+    <row r="665" ht="18" customHeight="1" s="115"/>
+    <row r="666" ht="18" customHeight="1" s="115"/>
+    <row r="667" ht="18" customHeight="1" s="115"/>
+    <row r="668" ht="18" customHeight="1" s="115"/>
+    <row r="669" ht="18" customHeight="1" s="115"/>
+    <row r="670" ht="18" customHeight="1" s="115"/>
+    <row r="671" ht="18" customHeight="1" s="115"/>
+    <row r="672" ht="18" customHeight="1" s="115"/>
+    <row r="673" ht="18" customHeight="1" s="115"/>
+    <row r="674" ht="18" customHeight="1" s="115"/>
+    <row r="675" ht="18" customHeight="1" s="115"/>
+    <row r="676" ht="18" customHeight="1" s="115"/>
+    <row r="677" ht="18" customHeight="1" s="115"/>
+    <row r="678" ht="18" customHeight="1" s="115"/>
+    <row r="679" ht="18" customHeight="1" s="115"/>
+    <row r="680" ht="18" customHeight="1" s="115"/>
+    <row r="681" ht="18" customHeight="1" s="115"/>
+    <row r="682" ht="18" customHeight="1" s="115"/>
+    <row r="683" ht="18" customHeight="1" s="115"/>
+    <row r="684" ht="18" customHeight="1" s="115"/>
+    <row r="685" ht="18" customHeight="1" s="115"/>
+    <row r="686" ht="18" customHeight="1" s="115"/>
+    <row r="687" ht="18" customHeight="1" s="115"/>
+    <row r="688" ht="18" customHeight="1" s="115"/>
+    <row r="689" ht="18" customHeight="1" s="115"/>
+    <row r="690" ht="18" customHeight="1" s="115"/>
+    <row r="691" ht="18" customHeight="1" s="115"/>
+    <row r="692" ht="18" customHeight="1" s="115"/>
+    <row r="693" ht="18" customHeight="1" s="115"/>
+    <row r="694" ht="18" customHeight="1" s="115"/>
+    <row r="695" ht="18" customHeight="1" s="115"/>
+    <row r="696" ht="18" customHeight="1" s="115"/>
+    <row r="697" ht="18" customHeight="1" s="115"/>
+    <row r="698" ht="18" customHeight="1" s="115"/>
+    <row r="699" ht="18" customHeight="1" s="115"/>
+    <row r="700" ht="18" customHeight="1" s="115"/>
+    <row r="701" ht="18" customHeight="1" s="115"/>
+    <row r="702" ht="18" customHeight="1" s="115"/>
+    <row r="703" ht="18" customHeight="1" s="115"/>
+    <row r="704" ht="18" customHeight="1" s="115"/>
+    <row r="705" ht="18" customHeight="1" s="115"/>
+    <row r="706" ht="18" customHeight="1" s="115"/>
+    <row r="707" ht="18" customHeight="1" s="115"/>
+    <row r="708" ht="18" customHeight="1" s="115"/>
+    <row r="709" ht="18" customHeight="1" s="115"/>
+    <row r="710" ht="18" customHeight="1" s="115"/>
+    <row r="711" ht="18" customHeight="1" s="115"/>
+    <row r="712" ht="18" customHeight="1" s="115"/>
+    <row r="713" ht="18" customHeight="1" s="115"/>
+    <row r="714" ht="18" customHeight="1" s="115"/>
+    <row r="715" ht="18" customHeight="1" s="115"/>
+    <row r="716" ht="18" customHeight="1" s="115"/>
+    <row r="717" ht="18" customHeight="1" s="115"/>
+    <row r="718" ht="18" customHeight="1" s="115"/>
+    <row r="719" ht="18" customHeight="1" s="115"/>
+    <row r="720" ht="18" customHeight="1" s="115"/>
+    <row r="721" ht="18" customHeight="1" s="115"/>
+    <row r="722" ht="18" customHeight="1" s="115"/>
+    <row r="723" ht="18" customHeight="1" s="115"/>
+    <row r="724" ht="18" customHeight="1" s="115"/>
+    <row r="725" ht="18" customHeight="1" s="115"/>
+    <row r="726" ht="18" customHeight="1" s="115"/>
+    <row r="727" ht="18" customHeight="1" s="115"/>
+    <row r="728" ht="18" customHeight="1" s="115"/>
+    <row r="729" ht="18" customHeight="1" s="115"/>
+    <row r="730" ht="18" customHeight="1" s="115"/>
+    <row r="731" ht="18" customHeight="1" s="115"/>
+    <row r="732" ht="18" customHeight="1" s="115"/>
+    <row r="733" ht="18" customHeight="1" s="115"/>
+    <row r="734" ht="18" customHeight="1" s="115"/>
+    <row r="735" ht="18" customHeight="1" s="115"/>
+    <row r="736" ht="18" customHeight="1" s="115"/>
+    <row r="737" ht="18" customHeight="1" s="115"/>
+    <row r="738" ht="18" customHeight="1" s="115"/>
+    <row r="739" ht="18" customHeight="1" s="115"/>
+    <row r="740" ht="18" customHeight="1" s="115"/>
+    <row r="741" ht="18" customHeight="1" s="115"/>
+    <row r="742" ht="18" customHeight="1" s="115"/>
+    <row r="743" ht="18" customHeight="1" s="115"/>
+    <row r="744" ht="18" customHeight="1" s="115"/>
+    <row r="745" ht="18" customHeight="1" s="115"/>
+    <row r="746" ht="18" customHeight="1" s="115"/>
+    <row r="747" ht="18" customHeight="1" s="115"/>
+    <row r="748" ht="18" customHeight="1" s="115"/>
+    <row r="749" ht="18" customHeight="1" s="115"/>
+    <row r="750" ht="18" customHeight="1" s="115"/>
+    <row r="751" ht="18" customHeight="1" s="115"/>
+    <row r="752" ht="18" customHeight="1" s="115"/>
+    <row r="753" ht="18" customHeight="1" s="115"/>
+    <row r="754" ht="18" customHeight="1" s="115"/>
+    <row r="755" ht="18" customHeight="1" s="115"/>
+    <row r="756" ht="18" customHeight="1" s="115"/>
+    <row r="757" ht="18" customHeight="1" s="115"/>
+    <row r="758" ht="18" customHeight="1" s="115"/>
+    <row r="759" ht="18" customHeight="1" s="115"/>
+    <row r="760" ht="18" customHeight="1" s="115"/>
+    <row r="761" ht="18" customHeight="1" s="115"/>
+    <row r="762" ht="18" customHeight="1" s="115"/>
+    <row r="763" ht="18" customHeight="1" s="115"/>
+    <row r="764" ht="18" customHeight="1" s="115"/>
+    <row r="765" ht="18" customHeight="1" s="115"/>
+    <row r="766" ht="18" customHeight="1" s="115"/>
+    <row r="767" ht="18" customHeight="1" s="115"/>
+    <row r="768" ht="18" customHeight="1" s="115"/>
+    <row r="769" ht="18" customHeight="1" s="115"/>
+    <row r="770" ht="18" customHeight="1" s="115"/>
+    <row r="771" ht="18" customHeight="1" s="115"/>
+    <row r="772" ht="18" customHeight="1" s="115"/>
+    <row r="773" ht="18" customHeight="1" s="115"/>
+    <row r="774" ht="18" customHeight="1" s="115"/>
+    <row r="775" ht="18" customHeight="1" s="115"/>
+    <row r="776" ht="18" customHeight="1" s="115"/>
+    <row r="777" ht="18" customHeight="1" s="115"/>
+    <row r="778" ht="18" customHeight="1" s="115"/>
+    <row r="779" ht="18" customHeight="1" s="115"/>
+    <row r="780" ht="18" customHeight="1" s="115"/>
+    <row r="781" ht="18" customHeight="1" s="115"/>
+    <row r="782" ht="18" customHeight="1" s="115"/>
+    <row r="783" ht="18" customHeight="1" s="115"/>
+    <row r="784" ht="18" customHeight="1" s="115"/>
+    <row r="785" ht="18" customHeight="1" s="115"/>
+    <row r="786" ht="18" customHeight="1" s="115"/>
+    <row r="787" ht="18" customHeight="1" s="115"/>
+    <row r="788" ht="18" customHeight="1" s="115"/>
+    <row r="789" ht="18" customHeight="1" s="115"/>
+    <row r="790" ht="18" customHeight="1" s="115"/>
+    <row r="791" ht="18" customHeight="1" s="115"/>
+    <row r="792" ht="18" customHeight="1" s="115"/>
+    <row r="793" ht="18" customHeight="1" s="115"/>
+    <row r="794" ht="18" customHeight="1" s="115"/>
+    <row r="795" ht="18" customHeight="1" s="115"/>
+    <row r="796" ht="18" customHeight="1" s="115"/>
+    <row r="797" ht="18" customHeight="1" s="115"/>
+    <row r="798" ht="18" customHeight="1" s="115"/>
+    <row r="799" ht="18" customHeight="1" s="115"/>
+    <row r="800" ht="18" customHeight="1" s="115"/>
+    <row r="801" ht="18" customHeight="1" s="115"/>
+    <row r="802" ht="18" customHeight="1" s="115"/>
+    <row r="803" ht="18" customHeight="1" s="115"/>
+    <row r="804" ht="18" customHeight="1" s="115"/>
+    <row r="805" ht="18" customHeight="1" s="115"/>
+    <row r="806" ht="18" customHeight="1" s="115"/>
+    <row r="807" ht="18" customHeight="1" s="115"/>
+    <row r="808" ht="18" customHeight="1" s="115"/>
+    <row r="809" ht="18" customHeight="1" s="115"/>
+    <row r="810" ht="18" customHeight="1" s="115"/>
+    <row r="811" ht="18" customHeight="1" s="115"/>
+    <row r="812" ht="18" customHeight="1" s="115"/>
+    <row r="813" ht="18" customHeight="1" s="115"/>
+    <row r="814" ht="18" customHeight="1" s="115"/>
+    <row r="815" ht="18" customHeight="1" s="115"/>
+    <row r="816" ht="18" customHeight="1" s="115"/>
+    <row r="817" ht="18" customHeight="1" s="115"/>
+    <row r="818" ht="18" customHeight="1" s="115"/>
+    <row r="819" ht="18" customHeight="1" s="115"/>
+    <row r="820" ht="18" customHeight="1" s="115"/>
+    <row r="821" ht="18" customHeight="1" s="115"/>
+    <row r="822" ht="18" customHeight="1" s="115"/>
+    <row r="823" ht="18" customHeight="1" s="115"/>
+    <row r="824" ht="18" customHeight="1" s="115"/>
+    <row r="825" ht="18" customHeight="1" s="115"/>
+    <row r="826" ht="18" customHeight="1" s="115"/>
+    <row r="827" ht="18" customHeight="1" s="115"/>
+    <row r="828" ht="18" customHeight="1" s="115"/>
+    <row r="829" ht="18" customHeight="1" s="115"/>
+    <row r="830" ht="18" customHeight="1" s="115"/>
+    <row r="831" ht="18" customHeight="1" s="115"/>
+    <row r="832" ht="18" customHeight="1" s="115"/>
+    <row r="833" ht="18" customHeight="1" s="115"/>
+    <row r="834" ht="18" customHeight="1" s="115"/>
+    <row r="835" ht="18" customHeight="1" s="115"/>
+    <row r="836" ht="18" customHeight="1" s="115"/>
+    <row r="837" ht="18" customHeight="1" s="115"/>
+    <row r="838" ht="18" customHeight="1" s="115"/>
+    <row r="839" ht="18" customHeight="1" s="115"/>
+    <row r="840" ht="18" customHeight="1" s="115"/>
+    <row r="841" ht="18" customHeight="1" s="115"/>
+    <row r="842" ht="18" customHeight="1" s="115"/>
+    <row r="843" ht="18" customHeight="1" s="115"/>
+    <row r="844" ht="18" customHeight="1" s="115"/>
+    <row r="845" ht="18" customHeight="1" s="115"/>
+    <row r="846" ht="18" customHeight="1" s="115"/>
+    <row r="847" ht="18" customHeight="1" s="115"/>
+    <row r="848" ht="18" customHeight="1" s="115"/>
+    <row r="849" ht="18" customHeight="1" s="115"/>
+    <row r="850" ht="18" customHeight="1" s="115"/>
+    <row r="851" ht="18" customHeight="1" s="115"/>
+    <row r="852" ht="18" customHeight="1" s="115"/>
+    <row r="853" ht="18" customHeight="1" s="115"/>
+    <row r="854" ht="18" customHeight="1" s="115"/>
+    <row r="855" ht="18" customHeight="1" s="115"/>
+    <row r="856" ht="18" customHeight="1" s="115"/>
+    <row r="857" ht="18" customHeight="1" s="115"/>
+    <row r="858" ht="18" customHeight="1" s="115"/>
+    <row r="859" ht="18" customHeight="1" s="115"/>
+    <row r="860" ht="18" customHeight="1" s="115"/>
+    <row r="861" ht="18" customHeight="1" s="115"/>
+    <row r="862" ht="18" customHeight="1" s="115"/>
+    <row r="863" ht="18" customHeight="1" s="115"/>
+    <row r="864" ht="18" customHeight="1" s="115"/>
+    <row r="865" ht="18" customHeight="1" s="115"/>
+    <row r="866" ht="18" customHeight="1" s="115"/>
+    <row r="867" ht="18" customHeight="1" s="115"/>
+    <row r="868" ht="18" customHeight="1" s="115"/>
+    <row r="869" ht="18" customHeight="1" s="115"/>
+    <row r="870" ht="18" customHeight="1" s="115"/>
+    <row r="871" ht="18" customHeight="1" s="115"/>
+    <row r="872" ht="18" customHeight="1" s="115"/>
+    <row r="873" ht="18" customHeight="1" s="115"/>
+    <row r="874" ht="18" customHeight="1" s="115"/>
+    <row r="875" ht="18" customHeight="1" s="115"/>
+    <row r="876" ht="18" customHeight="1" s="115"/>
+    <row r="877" ht="18" customHeight="1" s="115"/>
+    <row r="878" ht="18" customHeight="1" s="115"/>
+    <row r="879" ht="18" customHeight="1" s="115"/>
+    <row r="880" ht="18" customHeight="1" s="115"/>
+    <row r="881" ht="18" customHeight="1" s="115"/>
+    <row r="882" ht="18" customHeight="1" s="115"/>
+    <row r="883" ht="18" customHeight="1" s="115"/>
+    <row r="884" ht="18" customHeight="1" s="115"/>
+    <row r="885" ht="18" customHeight="1" s="115"/>
+    <row r="886" ht="18" customHeight="1" s="115"/>
+    <row r="887" ht="18" customHeight="1" s="115"/>
+    <row r="888" ht="18" customHeight="1" s="115"/>
+    <row r="889" ht="18" customHeight="1" s="115"/>
+    <row r="890" ht="18" customHeight="1" s="115"/>
+    <row r="891" ht="18" customHeight="1" s="115"/>
+    <row r="892" ht="18" customHeight="1" s="115"/>
+    <row r="893" ht="18" customHeight="1" s="115"/>
+    <row r="894" ht="18" customHeight="1" s="115"/>
+    <row r="895" ht="18" customHeight="1" s="115"/>
+    <row r="896" ht="18" customHeight="1" s="115"/>
+    <row r="897" ht="18" customHeight="1" s="115"/>
+    <row r="898" ht="18" customHeight="1" s="115"/>
+    <row r="899" ht="18" customHeight="1" s="115"/>
+    <row r="900" ht="18" customHeight="1" s="115"/>
+    <row r="901" ht="18" customHeight="1" s="115"/>
+    <row r="902" ht="18" customHeight="1" s="115"/>
+    <row r="903" ht="18" customHeight="1" s="115"/>
+    <row r="904" ht="18" customHeight="1" s="115"/>
+    <row r="905" ht="18" customHeight="1" s="115"/>
+    <row r="906" ht="18" customHeight="1" s="115"/>
+    <row r="907" ht="18" customHeight="1" s="115"/>
+    <row r="908" ht="18" customHeight="1" s="115"/>
+    <row r="909" ht="18" customHeight="1" s="115"/>
+    <row r="910" ht="18" customHeight="1" s="115"/>
+    <row r="911" ht="18" customHeight="1" s="115"/>
+    <row r="912" ht="18" customHeight="1" s="115"/>
+    <row r="913" ht="18" customHeight="1" s="115"/>
+    <row r="914" ht="18" customHeight="1" s="115"/>
+    <row r="915" ht="18" customHeight="1" s="115"/>
+    <row r="916" ht="18" customHeight="1" s="115"/>
+    <row r="917" ht="18" customHeight="1" s="115"/>
+    <row r="918" ht="18" customHeight="1" s="115"/>
+    <row r="919" ht="18" customHeight="1" s="115"/>
+    <row r="920" ht="18" customHeight="1" s="115"/>
+    <row r="921" ht="18" customHeight="1" s="115"/>
+    <row r="922" ht="18" customHeight="1" s="115"/>
+    <row r="923" ht="18" customHeight="1" s="115"/>
+    <row r="924" ht="18" customHeight="1" s="115"/>
+    <row r="925" ht="18" customHeight="1" s="115"/>
+    <row r="926" ht="18" customHeight="1" s="115"/>
+    <row r="927" ht="18" customHeight="1" s="115"/>
+    <row r="928" ht="18" customHeight="1" s="115"/>
+    <row r="929" ht="18" customHeight="1" s="115"/>
+    <row r="930" ht="18" customHeight="1" s="115"/>
+    <row r="931" ht="18" customHeight="1" s="115"/>
+    <row r="932" ht="18" customHeight="1" s="115"/>
+    <row r="933" ht="18" customHeight="1" s="115"/>
+    <row r="934" ht="18" customHeight="1" s="115"/>
+    <row r="935" ht="18" customHeight="1" s="115"/>
+    <row r="936" ht="18" customHeight="1" s="115"/>
+    <row r="937" ht="18" customHeight="1" s="115"/>
+    <row r="938" ht="18" customHeight="1" s="115"/>
+    <row r="939" ht="18" customHeight="1" s="115"/>
+    <row r="940" ht="18" customHeight="1" s="115"/>
+    <row r="941" ht="18" customHeight="1" s="115"/>
+    <row r="942" ht="18" customHeight="1" s="115"/>
+    <row r="943" ht="18" customHeight="1" s="115"/>
+    <row r="944" ht="18" customHeight="1" s="115"/>
+    <row r="945" ht="18" customHeight="1" s="115"/>
+    <row r="946" ht="18" customHeight="1" s="115"/>
+    <row r="947" ht="18" customHeight="1" s="115"/>
+    <row r="948" ht="18" customHeight="1" s="115"/>
+    <row r="949" ht="18" customHeight="1" s="115"/>
+    <row r="950" ht="18" customHeight="1" s="115"/>
+    <row r="951" ht="18" customHeight="1" s="115"/>
+    <row r="952" ht="18" customHeight="1" s="115"/>
+    <row r="953" ht="18" customHeight="1" s="115"/>
+    <row r="954" ht="18" customHeight="1" s="115"/>
+    <row r="955" ht="18" customHeight="1" s="115"/>
+    <row r="956" ht="18" customHeight="1" s="115"/>
+    <row r="957" ht="18" customHeight="1" s="115"/>
+    <row r="958" ht="18" customHeight="1" s="115"/>
+    <row r="959" ht="18" customHeight="1" s="115"/>
+    <row r="960" ht="18" customHeight="1" s="115"/>
+    <row r="961" ht="18" customHeight="1" s="115"/>
+    <row r="962" ht="18" customHeight="1" s="115"/>
+    <row r="963" ht="18" customHeight="1" s="115"/>
+    <row r="964" ht="18" customHeight="1" s="115"/>
+    <row r="965" ht="18" customHeight="1" s="115"/>
+    <row r="966" ht="18" customHeight="1" s="115"/>
+    <row r="967" ht="18" customHeight="1" s="115"/>
+    <row r="968" ht="18" customHeight="1" s="115"/>
+    <row r="969" ht="18" customHeight="1" s="115"/>
+    <row r="970" ht="18" customHeight="1" s="115"/>
+    <row r="971" ht="18" customHeight="1" s="115"/>
+    <row r="972" ht="18" customHeight="1" s="115"/>
+    <row r="973" ht="18" customHeight="1" s="115"/>
+    <row r="974" ht="18" customHeight="1" s="115"/>
+    <row r="975" ht="18" customHeight="1" s="115"/>
+    <row r="976" ht="18" customHeight="1" s="115"/>
+    <row r="977" ht="18" customHeight="1" s="115"/>
+    <row r="978" ht="18" customHeight="1" s="115"/>
+    <row r="979" ht="18" customHeight="1" s="115"/>
+    <row r="980" ht="18" customHeight="1" s="115"/>
+    <row r="981" ht="18" customHeight="1" s="115"/>
+    <row r="982" ht="18" customHeight="1" s="115"/>
+    <row r="983" ht="18" customHeight="1" s="115"/>
+    <row r="984" ht="18" customHeight="1" s="115"/>
+    <row r="985" ht="18" customHeight="1" s="115"/>
+    <row r="986" ht="18" customHeight="1" s="115"/>
+    <row r="987" ht="18" customHeight="1" s="115"/>
+    <row r="988" ht="18" customHeight="1" s="115"/>
+    <row r="989" ht="18" customHeight="1" s="115"/>
+    <row r="990" ht="18" customHeight="1" s="115"/>
+    <row r="991" ht="18" customHeight="1" s="115"/>
+    <row r="992" ht="18" customHeight="1" s="115"/>
+    <row r="993" ht="18" customHeight="1" s="115"/>
+    <row r="994" ht="18" customHeight="1" s="115"/>
+    <row r="995" ht="18" customHeight="1" s="115"/>
+    <row r="996" ht="18" customHeight="1" s="115"/>
+    <row r="997" ht="18" customHeight="1" s="115"/>
+    <row r="998" ht="18" customHeight="1" s="115"/>
+    <row r="999" ht="18" customHeight="1" s="115"/>
+    <row r="1000" ht="18" customHeight="1" s="115"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:F2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.5118110236220472" right="0.1181102362204725" top="2.362204724409449" bottom="0.7480314960629921" header="0" footer="0"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col width="9" customWidth="1" style="115" min="1" max="1"/>
+    <col width="8.140000000000001" customWidth="1" style="115" min="2" max="2"/>
+    <col width="44.14" customWidth="1" style="115" min="3" max="3"/>
+    <col width="6.43" customWidth="1" style="115" min="4" max="4"/>
+    <col width="8.710000000000001" customWidth="1" style="115" min="5" max="6"/>
+    <col width="1.43" customWidth="1" style="115" min="7" max="7"/>
+    <col hidden="1" outlineLevel="1" width="7.14" customWidth="1" style="115" min="8" max="8"/>
+    <col hidden="1" outlineLevel="1" width="11.71" customWidth="1" style="115" min="9" max="9"/>
+    <col hidden="1" outlineLevel="1" width="0.86" customWidth="1" style="115" min="10" max="10"/>
+    <col hidden="1" outlineLevel="1" width="9.140000000000001" customWidth="1" style="115" min="11" max="13"/>
+    <col hidden="1" outlineLevel="1" width="10.14" customWidth="1" style="115" min="14" max="14"/>
+    <col hidden="1" outlineLevel="1" width="1.14" customWidth="1" style="115" min="15" max="15"/>
+    <col hidden="1" outlineLevel="1" width="9.140000000000001" customWidth="1" style="115" min="16" max="17"/>
+    <col hidden="1" outlineLevel="1" width="10.14" customWidth="1" style="115" min="18" max="18"/>
+    <col width="9" customWidth="1" style="115" min="19" max="19"/>
+    <col width="14.29" customWidth="1" style="115" min="20" max="20"/>
+    <col width="11.71" customWidth="1" style="115" min="21" max="24"/>
+    <col width="8.710000000000001" customWidth="1" style="115" min="25" max="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" s="115">
+      <c r="A1" s="116" t="inlineStr">
+        <is>
+          <t>2025年</t>
+        </is>
+      </c>
+      <c r="B1" s="117" t="inlineStr">
+        <is>
+          <t>1月度</t>
+        </is>
+      </c>
+      <c r="C1" s="118" t="inlineStr">
+        <is>
+          <t>経費仮払金精算</t>
+        </is>
+      </c>
+      <c r="D1" s="119" t="n"/>
+      <c r="E1" s="120" t="inlineStr">
+        <is>
+          <t>硝子設備・
+プラントプロジェクト部</t>
+        </is>
+      </c>
+      <c r="F1" s="121" t="n"/>
+      <c r="I1" s="7" t="n"/>
+      <c r="K1" s="7" t="n"/>
+      <c r="L1" s="7" t="n"/>
+      <c r="M1" s="7" t="n"/>
+      <c r="N1" s="7" t="n"/>
+      <c r="O1" s="7" t="n"/>
+      <c r="P1" s="7" t="n"/>
+      <c r="Q1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1" s="115">
+      <c r="A2" s="122" t="n"/>
+      <c r="B2" s="123" t="n"/>
+      <c r="C2" s="124" t="n"/>
+      <c r="D2" s="119" t="n"/>
+      <c r="E2" s="125" t="n"/>
+      <c r="F2" s="126" t="n"/>
+      <c r="I2" s="7" t="n"/>
+      <c r="K2" s="7" t="n"/>
+      <c r="L2" s="7" t="n"/>
+      <c r="M2" s="7" t="n"/>
+      <c r="N2" s="7" t="n"/>
+      <c r="O2" s="7" t="n"/>
+      <c r="P2" s="7" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="4.5" customHeight="1" s="115">
+      <c r="B3" s="13" t="n"/>
+      <c r="D3" s="14" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="F3" s="15" t="n"/>
+      <c r="I3" s="7" t="n"/>
+      <c r="K3" s="7" t="n"/>
+      <c r="L3" s="7" t="n"/>
+      <c r="M3" s="7" t="n"/>
+      <c r="N3" s="7" t="n"/>
+      <c r="O3" s="7" t="n"/>
+      <c r="P3" s="7" t="n"/>
+      <c r="Q3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="18" customHeight="1" s="115">
+      <c r="A4" s="90" t="inlineStr">
+        <is>
+          <t>支払日</t>
+        </is>
+      </c>
+      <c r="B4" s="91" t="inlineStr">
+        <is>
+          <t>工番</t>
+        </is>
+      </c>
+      <c r="C4" s="92" t="inlineStr">
+        <is>
+          <t>摘　　要</t>
+        </is>
+      </c>
+      <c r="D4" s="93" t="inlineStr">
+        <is>
+          <t>担当者</t>
+        </is>
+      </c>
+      <c r="E4" s="94" t="inlineStr">
+        <is>
+          <t>収入</t>
+        </is>
+      </c>
+      <c r="F4" s="95" t="inlineStr">
+        <is>
+          <t>支出</t>
+        </is>
+      </c>
+      <c r="G4" s="22" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="H4" s="23" t="inlineStr">
+        <is>
+          <t>インボイス</t>
+        </is>
+      </c>
+      <c r="I4" s="24" t="inlineStr">
+        <is>
+          <t>勘定科目</t>
+        </is>
+      </c>
+      <c r="J4" s="25" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="K4" s="26" t="inlineStr">
+        <is>
+          <t>10％税込額</t>
+        </is>
+      </c>
+      <c r="L4" s="27" t="inlineStr">
+        <is>
+          <t>8％税込額</t>
+        </is>
+      </c>
+      <c r="M4" s="28" t="inlineStr">
+        <is>
+          <t>非課税額</t>
+        </is>
+      </c>
+      <c r="N4" s="29" t="inlineStr">
+        <is>
+          <t>税込合計</t>
+        </is>
+      </c>
+      <c r="O4" s="30" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="P4" s="31" t="inlineStr">
+        <is>
+          <t>消費税10</t>
+        </is>
+      </c>
+      <c r="Q4" s="32" t="inlineStr">
+        <is>
+          <t>消費税8</t>
+        </is>
+      </c>
+      <c r="R4" s="24" t="inlineStr">
+        <is>
+          <t>消費税計</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1" s="115">
+      <c r="A5" s="33" t="n"/>
+      <c r="B5" s="34" t="n"/>
+      <c r="C5" s="96" t="inlineStr">
+        <is>
+          <t>前月より繰越</t>
+        </is>
+      </c>
+      <c r="D5" s="36" t="n"/>
+      <c r="E5" s="37" t="n">
+        <v>624668</v>
+      </c>
+      <c r="F5" s="38" t="n"/>
+      <c r="H5" s="39" t="n"/>
+      <c r="I5" s="40" t="n"/>
+      <c r="K5" s="41" t="n"/>
+      <c r="L5" s="42" t="n"/>
+      <c r="M5" s="43" t="n"/>
+      <c r="N5" s="44" t="n"/>
+      <c r="O5" s="45" t="n"/>
+      <c r="P5" s="41" t="n"/>
+      <c r="Q5" s="43" t="n"/>
+      <c r="R5" s="44" t="n"/>
+      <c r="T5" s="100" t="inlineStr">
+        <is>
+          <t>GPP</t>
+        </is>
+      </c>
+      <c r="U5" s="100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="18" customHeight="1" s="115">
+      <c r="A6" s="97" t="n">
+        <v>45664</v>
+      </c>
+      <c r="B6" s="47" t="n"/>
+      <c r="C6" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  ご祈祷 玉串代</t>
+        </is>
+      </c>
+      <c r="D6" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E6" s="50" t="n"/>
+      <c r="F6" s="99" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G6" s="51" t="n"/>
+      <c r="H6" s="52" t="inlineStr">
+        <is>
+          <t>不要</t>
+        </is>
+      </c>
+      <c r="I6" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J6" s="51" t="n"/>
+      <c r="K6" s="54" t="n"/>
+      <c r="L6" s="55" t="n"/>
+      <c r="M6" s="56" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N6" s="57">
+        <f>IF(K6+L6+M6=0,"",K6+L6+M6)</f>
+        <v/>
+      </c>
+      <c r="O6" s="58" t="n"/>
+      <c r="P6" s="59">
+        <f>ROUNDDOWN($K6/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q6" s="60">
+        <f>ROUNDDOWN($L6/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R6" s="57">
+        <f>P6+Q6</f>
+        <v/>
+      </c>
+      <c r="T6" s="100" t="inlineStr">
+        <is>
+          <t>科目</t>
+        </is>
+      </c>
+      <c r="U6" s="109" t="inlineStr">
+        <is>
+          <t>10％税込額</t>
+        </is>
+      </c>
+      <c r="V6" s="109" t="inlineStr">
+        <is>
+          <t>8％税込額</t>
+        </is>
+      </c>
+      <c r="W6" s="109" t="inlineStr">
+        <is>
+          <t>非課税額</t>
+        </is>
+      </c>
+      <c r="X6" s="109" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1" s="115">
+      <c r="A7" s="97" t="n">
+        <v>45665</v>
+      </c>
+      <c r="B7" s="47" t="n"/>
+      <c r="C7" s="98" t="inlineStr">
+        <is>
+          <t>水道光熱費・租税公課  水道料金・印紙</t>
+        </is>
+      </c>
+      <c r="D7" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E7" s="55" t="n"/>
+      <c r="F7" s="99" t="n">
+        <v>7571</v>
+      </c>
+      <c r="H7" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I7" s="53" t="inlineStr">
+        <is>
+          <t>水道光熱費</t>
+        </is>
+      </c>
+      <c r="J7" s="51" t="n"/>
+      <c r="K7" s="54" t="n">
+        <v>5571</v>
+      </c>
+      <c r="L7" s="55" t="n"/>
+      <c r="M7" s="56" t="n"/>
+      <c r="N7" s="57">
+        <f>IF(K7+L7+M7=0,"",K7+L7+M7)</f>
+        <v/>
+      </c>
+      <c r="O7" s="58" t="n"/>
+      <c r="P7" s="59">
+        <f>ROUNDDOWN($K7/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q7" s="60">
+        <f>ROUNDDOWN($L7/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R7" s="57">
+        <f>P7+Q7</f>
+        <v/>
+      </c>
+      <c r="T7" s="102" t="inlineStr">
+        <is>
+          <t>交際費</t>
+        </is>
+      </c>
+      <c r="U7" s="111" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V7" s="111" t="n"/>
+      <c r="W7" s="111" t="n"/>
+      <c r="X7" s="111" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" ht="18" customHeight="1" s="115">
+      <c r="A8" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B8" s="47" t="n"/>
+      <c r="C8" s="98" t="inlineStr">
+        <is>
+          <t>💰💰💰入金💰💰💰</t>
+        </is>
+      </c>
+      <c r="D8" s="99" t="inlineStr">
+        <is>
+          <t>田代</t>
+        </is>
+      </c>
+      <c r="E8" s="55" t="n">
+        <v>300000</v>
+      </c>
+      <c r="F8" s="99" t="n"/>
+      <c r="H8" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I8" s="53" t="inlineStr">
+        <is>
+          <t>租税公課</t>
+        </is>
+      </c>
+      <c r="J8" s="51" t="n"/>
+      <c r="K8" s="54" t="n"/>
+      <c r="L8" s="55" t="n"/>
+      <c r="M8" s="56" t="n">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="57">
+        <f>IF(K8+L8+M8=0,"",K8+L8+M8)</f>
+        <v/>
+      </c>
+      <c r="O8" s="58" t="n"/>
+      <c r="P8" s="59">
+        <f>ROUNDDOWN($K8/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q8" s="60">
+        <f>ROUNDDOWN($L8/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R8" s="57">
+        <f>P8+Q8</f>
+        <v/>
+      </c>
+      <c r="T8" s="102" t="inlineStr">
+        <is>
+          <t>仕入材料</t>
+        </is>
+      </c>
+      <c r="U8" s="111" t="n">
+        <v>4176</v>
+      </c>
+      <c r="V8" s="111" t="n"/>
+      <c r="W8" s="111" t="n"/>
+      <c r="X8" s="111" t="n">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="9" ht="18" customHeight="1" s="115">
+      <c r="A9" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B9" s="47" t="n"/>
+      <c r="C9" s="98" t="inlineStr">
+        <is>
+          <t>交際費・旅費交通費  協創会忘年会・駐車場代・PCデータ抜出</t>
+        </is>
+      </c>
+      <c r="D9" s="99" t="inlineStr">
+        <is>
+          <t>田代</t>
+        </is>
+      </c>
+      <c r="E9" s="55" t="n"/>
+      <c r="F9" s="99" t="n">
+        <v>50100</v>
+      </c>
+      <c r="H9" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I9" s="53" t="inlineStr">
+        <is>
+          <t>交際費</t>
+        </is>
+      </c>
+      <c r="J9" s="51" t="n"/>
+      <c r="K9" s="54" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L9" s="55" t="n"/>
+      <c r="M9" s="56" t="n"/>
+      <c r="N9" s="57">
+        <f>IF(K9+L9+M9=0,"",K9+L9+M9)</f>
+        <v/>
+      </c>
+      <c r="O9" s="58" t="n"/>
+      <c r="P9" s="59">
+        <f>ROUNDDOWN($K9/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q9" s="60">
+        <f>ROUNDDOWN($L9/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R9" s="57">
+        <f>P9+Q9</f>
+        <v/>
+      </c>
+      <c r="T9" s="102" t="inlineStr">
+        <is>
+          <t>事務消耗品費</t>
+        </is>
+      </c>
+      <c r="U9" s="111" t="n">
+        <v>3300</v>
+      </c>
+      <c r="V9" s="111" t="n"/>
+      <c r="W9" s="111" t="n"/>
+      <c r="X9" s="111" t="n">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="10" ht="18" customHeight="1" s="115">
+      <c r="A10" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B10" s="47" t="n"/>
+      <c r="C10" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費・仕入材料  出張経費11/28～12/27【詳細別紙】</t>
+        </is>
+      </c>
+      <c r="D10" s="99" t="inlineStr">
+        <is>
+          <t>佐藤</t>
+        </is>
+      </c>
+      <c r="E10" s="55" t="n"/>
+      <c r="F10" s="99" t="n">
+        <v>77293</v>
+      </c>
+      <c r="H10" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I10" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J10" s="51" t="n"/>
+      <c r="K10" s="54" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L10" s="55" t="n"/>
+      <c r="M10" s="56" t="n"/>
+      <c r="N10" s="57">
+        <f>IF(K10+L10+M10=0,"",K10+L10+M10)</f>
+        <v/>
+      </c>
+      <c r="O10" s="58" t="n"/>
+      <c r="P10" s="59">
+        <f>ROUNDDOWN($K10/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q10" s="60">
+        <f>ROUNDDOWN($L10/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R10" s="57">
+        <f>P10+Q10</f>
+        <v/>
+      </c>
+      <c r="T10" s="102" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="U10" s="111" t="n">
+        <v>86634</v>
+      </c>
+      <c r="V10" s="111" t="n"/>
+      <c r="W10" s="111" t="n">
+        <v>30000</v>
+      </c>
+      <c r="X10" s="111" t="n">
+        <v>116634</v>
+      </c>
+    </row>
+    <row r="11" ht="18" customHeight="1" s="115">
+      <c r="A11" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B11" s="47" t="n"/>
+      <c r="C11" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費・仕入材料  出張経費1/6～1/9【詳細別紙】</t>
+        </is>
+      </c>
+      <c r="D11" s="99" t="inlineStr">
+        <is>
+          <t>佐藤</t>
+        </is>
+      </c>
+      <c r="E11" s="55" t="n"/>
+      <c r="F11" s="99" t="n">
+        <v>14856</v>
+      </c>
+      <c r="H11" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I11" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J11" s="51" t="n"/>
+      <c r="K11" s="54" t="n">
+        <v>41800</v>
+      </c>
+      <c r="L11" s="55" t="n"/>
+      <c r="M11" s="56" t="n"/>
+      <c r="N11" s="57">
+        <f>IF(K11+L11+M11=0,"",K11+L11+M11)</f>
+        <v/>
+      </c>
+      <c r="O11" s="58" t="n"/>
+      <c r="P11" s="59">
+        <f>ROUNDDOWN($K11/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q11" s="60">
+        <f>ROUNDDOWN($L11/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R11" s="57">
+        <f>P11+Q11</f>
+        <v/>
+      </c>
+      <c r="T11" s="102" t="inlineStr">
+        <is>
+          <t>水道光熱費</t>
+        </is>
+      </c>
+      <c r="U11" s="111" t="n">
+        <v>5571</v>
+      </c>
+      <c r="V11" s="111" t="n"/>
+      <c r="W11" s="111" t="n"/>
+      <c r="X11" s="111" t="n">
+        <v>5571</v>
+      </c>
+    </row>
+    <row r="12" ht="18" customHeight="1" s="115">
+      <c r="A12" s="97" t="n">
+        <v>45667</v>
+      </c>
+      <c r="B12" s="47" t="n"/>
+      <c r="C12" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  ETC代</t>
+        </is>
+      </c>
+      <c r="D12" s="99" t="inlineStr">
+        <is>
+          <t>佐藤</t>
+        </is>
+      </c>
+      <c r="E12" s="55" t="n"/>
+      <c r="F12" s="99" t="n">
+        <v>14530</v>
+      </c>
+      <c r="H12" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I12" s="53" t="inlineStr">
+        <is>
+          <t>事務消耗品費</t>
+        </is>
+      </c>
+      <c r="J12" s="51" t="n"/>
+      <c r="K12" s="54" t="n">
+        <v>3300</v>
+      </c>
+      <c r="L12" s="55" t="n"/>
+      <c r="M12" s="56" t="n"/>
+      <c r="N12" s="57">
+        <f>IF(K12+L12+M12=0,"",K12+L12+M12)</f>
+        <v/>
+      </c>
+      <c r="O12" s="58" t="n"/>
+      <c r="P12" s="59">
+        <f>ROUNDDOWN($K12/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q12" s="60">
+        <f>ROUNDDOWN($L12/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R12" s="57">
+        <f>P12+Q12</f>
+        <v/>
+      </c>
+      <c r="T12" s="102" t="inlineStr">
+        <is>
+          <t>租税公課</t>
+        </is>
+      </c>
+      <c r="U12" s="111" t="n"/>
+      <c r="V12" s="111" t="n"/>
+      <c r="W12" s="111" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X12" s="111" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" ht="18" customHeight="1" s="115">
+      <c r="A13" s="97" t="n">
+        <v>45671</v>
+      </c>
+      <c r="B13" s="47" t="n"/>
+      <c r="C13" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  日本認証講習会交通費 横浜駅～浜松町駅(JR)往復x2日</t>
+        </is>
+      </c>
+      <c r="D13" s="99" t="inlineStr">
+        <is>
+          <t>小仁所</t>
+        </is>
+      </c>
+      <c r="E13" s="55" t="n"/>
+      <c r="F13" s="99" t="n">
+        <v>1932</v>
+      </c>
+      <c r="H13" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I13" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J13" s="51" t="n"/>
+      <c r="K13" s="54" t="n">
+        <v>14530</v>
+      </c>
+      <c r="L13" s="55" t="n"/>
+      <c r="M13" s="56" t="n"/>
+      <c r="N13" s="57">
+        <f>IF(K13+L13+M13=0,"",K13+L13+M13)</f>
+        <v/>
+      </c>
+      <c r="O13" s="58" t="n"/>
+      <c r="P13" s="59">
+        <f>ROUNDDOWN($K13/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q13" s="60">
+        <f>ROUNDDOWN($L13/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R13" s="57">
+        <f>P13+Q13</f>
+        <v/>
+      </c>
+      <c r="T13" s="102" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="U13" s="111" t="n">
+        <v>5210</v>
+      </c>
+      <c r="V13" s="111" t="n"/>
+      <c r="W13" s="111" t="n"/>
+      <c r="X13" s="111" t="n">
+        <v>5210</v>
+      </c>
+    </row>
+    <row r="14" ht="18" customHeight="1" s="115">
+      <c r="A14" s="97" t="n">
+        <v>45671</v>
+      </c>
+      <c r="B14" s="47" t="n"/>
+      <c r="C14" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  榊代</t>
+        </is>
+      </c>
+      <c r="D14" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E14" s="55" t="n"/>
+      <c r="F14" s="99" t="n">
+        <v>600</v>
+      </c>
+      <c r="H14" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I14" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J14" s="51" t="n"/>
+      <c r="K14" s="54" t="n">
+        <v>1932</v>
+      </c>
+      <c r="L14" s="55" t="n"/>
+      <c r="M14" s="56" t="n"/>
+      <c r="N14" s="57">
+        <f>IF(K14+L14+M14=0,"",K14+L14+M14)</f>
+        <v/>
+      </c>
+      <c r="O14" s="58" t="n"/>
+      <c r="P14" s="59">
+        <f>ROUNDDOWN($K14/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q14" s="60">
+        <f>ROUNDDOWN($L14/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R14" s="57">
+        <f>P14+Q14</f>
+        <v/>
+      </c>
+      <c r="T14" s="102" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="U14" s="111" t="n">
+        <v>158438</v>
+      </c>
+      <c r="V14" s="111" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W14" s="111" t="n"/>
+      <c r="X14" s="111" t="n">
+        <v>162447</v>
+      </c>
+    </row>
+    <row r="15" ht="18" customHeight="1" s="115">
+      <c r="A15" s="97" t="n">
+        <v>45672</v>
+      </c>
+      <c r="B15" s="47" t="n"/>
+      <c r="C15" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  奉献酒</t>
+        </is>
+      </c>
+      <c r="D15" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E15" s="55" t="n"/>
+      <c r="F15" s="99" t="n">
+        <v>4100</v>
+      </c>
+      <c r="H15" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I15" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J15" s="51" t="n"/>
+      <c r="K15" s="54" t="n">
+        <v>600</v>
+      </c>
+      <c r="L15" s="55" t="n"/>
+      <c r="M15" s="56" t="n"/>
+      <c r="N15" s="57">
+        <f>IF(K15+L15+M15=0,"",K15+L15+M15)</f>
+        <v/>
+      </c>
+      <c r="O15" s="58" t="n"/>
+      <c r="P15" s="59">
+        <f>ROUNDDOWN($K15/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q15" s="60">
+        <f>ROUNDDOWN($L15/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R15" s="57">
+        <f>P15+Q15</f>
+        <v/>
+      </c>
+      <c r="T15" s="102" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+      <c r="U15" s="111" t="n">
+        <v>266329</v>
+      </c>
+      <c r="V15" s="111" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W15" s="111" t="n">
+        <v>32000</v>
+      </c>
+      <c r="X15" s="111" t="n">
+        <v>302338</v>
+      </c>
+    </row>
+    <row r="16" ht="18" customHeight="1" s="115">
+      <c r="A16" s="97" t="n">
+        <v>45673</v>
+      </c>
+      <c r="B16" s="47" t="n"/>
+      <c r="C16" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  AGC鏡開き物品代</t>
+        </is>
+      </c>
+      <c r="D16" s="99" t="inlineStr">
+        <is>
+          <t>小仁所</t>
+        </is>
+      </c>
+      <c r="E16" s="55" t="n"/>
+      <c r="F16" s="99" t="n">
+        <v>6534</v>
+      </c>
+      <c r="H16" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I16" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J16" s="51" t="n"/>
+      <c r="K16" s="54" t="n">
+        <v>4100</v>
+      </c>
+      <c r="L16" s="55" t="n"/>
+      <c r="M16" s="56" t="n"/>
+      <c r="N16" s="57">
+        <f>IF(K16+L16+M16=0,"",K16+L16+M16)</f>
+        <v/>
+      </c>
+      <c r="O16" s="58" t="n"/>
+      <c r="P16" s="59">
+        <f>ROUNDDOWN($K16/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q16" s="60">
+        <f>ROUNDDOWN($L16/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R16" s="57">
+        <f>P16+Q16</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="115">
+      <c r="A17" s="97" t="n">
+        <v>45677</v>
+      </c>
+      <c r="B17" s="47" t="n"/>
+      <c r="C17" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  宿泊費</t>
+        </is>
+      </c>
+      <c r="D17" s="99" t="inlineStr">
+        <is>
+          <t>尾川</t>
+        </is>
+      </c>
+      <c r="E17" s="55" t="n"/>
+      <c r="F17" s="99" t="n">
+        <v>54600</v>
+      </c>
+      <c r="H17" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I17" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J17" s="51" t="n"/>
+      <c r="K17" s="54" t="n">
+        <v>6534</v>
+      </c>
+      <c r="L17" s="55" t="n"/>
+      <c r="M17" s="56" t="n"/>
+      <c r="N17" s="57">
+        <f>IF(K17+L17+M17=0,"",K17+L17+M17)</f>
+        <v/>
+      </c>
+      <c r="O17" s="58" t="n"/>
+      <c r="P17" s="59">
+        <f>ROUNDDOWN($K17/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q17" s="60">
+        <f>ROUNDDOWN($L17/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R17" s="57">
+        <f>P17+Q17</f>
+        <v/>
+      </c>
+      <c r="T17" s="104" t="inlineStr">
+        <is>
+          <t>GPP</t>
+        </is>
+      </c>
+      <c r="U17" s="104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="V17" s="104" t="n"/>
+      <c r="W17" s="104" t="n"/>
+      <c r="X17" s="104" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1" s="115">
+      <c r="A18" s="97" t="n">
+        <v>45680</v>
+      </c>
+      <c r="B18" s="47" t="n"/>
+      <c r="C18" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  指定ゴミ袋</t>
+        </is>
+      </c>
+      <c r="D18" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E18" s="55" t="n"/>
+      <c r="F18" s="99" t="n">
+        <v>33000</v>
+      </c>
+      <c r="H18" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I18" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J18" s="51" t="n"/>
+      <c r="K18" s="54" t="n">
+        <v>54600</v>
+      </c>
+      <c r="L18" s="55" t="n"/>
+      <c r="M18" s="56" t="n"/>
+      <c r="N18" s="57">
+        <f>IF(K18+L18+M18=0,"",K18+L18+M18)</f>
+        <v/>
+      </c>
+      <c r="O18" s="58" t="n"/>
+      <c r="P18" s="59">
+        <f>ROUNDDOWN($K18/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q18" s="60">
+        <f>ROUNDDOWN($L18/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R18" s="57">
+        <f>P18+Q18</f>
+        <v/>
+      </c>
+      <c r="T18" s="105" t="inlineStr">
+        <is>
+          <t>科目</t>
+        </is>
+      </c>
+      <c r="U18" s="106" t="inlineStr">
+        <is>
+          <t>10％税込額</t>
+        </is>
+      </c>
+      <c r="V18" s="106" t="inlineStr">
+        <is>
+          <t>8％税込額</t>
+        </is>
+      </c>
+      <c r="W18" s="106" t="inlineStr">
+        <is>
+          <t>非課税額</t>
+        </is>
+      </c>
+      <c r="X18" s="106" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="18" customHeight="1" s="115">
+      <c r="A19" s="97" t="n">
+        <v>45684</v>
+      </c>
+      <c r="B19" s="47" t="n"/>
+      <c r="C19" s="98" t="inlineStr">
+        <is>
+          <t>旅費交通費  日本認証試験交通費 鶴見駅～テレコムセンター(JR・ゆりかもめ)往復</t>
+        </is>
+      </c>
+      <c r="D19" s="99" t="inlineStr">
+        <is>
+          <t>小仁所</t>
+        </is>
+      </c>
+      <c r="E19" s="55" t="n"/>
+      <c r="F19" s="99" t="n">
+        <v>1412</v>
+      </c>
+      <c r="H19" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I19" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J19" s="51" t="n"/>
+      <c r="K19" s="54" t="n">
+        <v>33000</v>
+      </c>
+      <c r="L19" s="55" t="n"/>
+      <c r="M19" s="56" t="n"/>
+      <c r="N19" s="57">
+        <f>IF(K19+L19+M19=0,"",K19+L19+M19)</f>
+        <v/>
+      </c>
+      <c r="O19" s="58" t="n"/>
+      <c r="P19" s="59">
+        <f>ROUNDDOWN($K19/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q19" s="60">
+        <f>ROUNDDOWN($L19/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R19" s="57">
+        <f>P19+Q19</f>
+        <v/>
+      </c>
+      <c r="T19" s="102" t="inlineStr">
+        <is>
+          <t>交際費</t>
+        </is>
+      </c>
+      <c r="U19" s="111" t="n">
+        <v>3000</v>
+      </c>
+      <c r="V19" s="111" t="n"/>
+      <c r="W19" s="111" t="n"/>
+      <c r="X19" s="111" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" ht="18" customHeight="1" s="115">
+      <c r="A20" s="97" t="n">
+        <v>45685</v>
+      </c>
+      <c r="B20" s="47" t="n"/>
+      <c r="C20" s="98" t="inlineStr">
+        <is>
+          <t>通信費・租税公課  工事依頼書郵送代・印紙</t>
+        </is>
+      </c>
+      <c r="D20" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E20" s="55" t="n"/>
+      <c r="F20" s="99" t="n">
+        <v>5210</v>
+      </c>
+      <c r="H20" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I20" s="53" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="J20" s="51" t="n"/>
+      <c r="K20" s="54" t="n">
+        <v>1412</v>
+      </c>
+      <c r="L20" s="55" t="n"/>
+      <c r="M20" s="56" t="n"/>
+      <c r="N20" s="57">
+        <f>IF(K20+L20+M20=0,"",K20+L20+M20)</f>
+        <v/>
+      </c>
+      <c r="O20" s="58" t="n"/>
+      <c r="P20" s="59">
+        <f>ROUNDDOWN($K20/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q20" s="60">
+        <f>ROUNDDOWN($L20/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R20" s="57">
+        <f>P20+Q20</f>
+        <v/>
+      </c>
+      <c r="T20" s="102" t="inlineStr">
+        <is>
+          <t>仕入材料</t>
+        </is>
+      </c>
+      <c r="U20" s="111" t="n">
+        <v>4176</v>
+      </c>
+      <c r="V20" s="111" t="n"/>
+      <c r="W20" s="111" t="n"/>
+      <c r="X20" s="111" t="n">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="21" ht="18" customHeight="1" s="115">
+      <c r="A21" s="97" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B21" s="47" t="n"/>
+      <c r="C21" s="98" t="inlineStr">
+        <is>
+          <t>諸雑費  榊代</t>
+        </is>
+      </c>
+      <c r="D21" s="99" t="inlineStr">
+        <is>
+          <t>溝口</t>
+        </is>
+      </c>
+      <c r="E21" s="55" t="n"/>
+      <c r="F21" s="99" t="n">
+        <v>600</v>
+      </c>
+      <c r="H21" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I21" s="53" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="J21" s="51" t="n"/>
+      <c r="K21" s="54" t="n">
+        <v>5210</v>
+      </c>
+      <c r="L21" s="55" t="n"/>
+      <c r="M21" s="56" t="n"/>
+      <c r="N21" s="57">
+        <f>IF(K21+L21+M21=0,"",K21+L21+M21)</f>
+        <v/>
+      </c>
+      <c r="O21" s="58" t="n"/>
+      <c r="P21" s="59">
+        <f>ROUNDDOWN($K21/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q21" s="60">
+        <f>ROUNDDOWN($L21/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R21" s="57">
+        <f>P21+Q21</f>
+        <v/>
+      </c>
+      <c r="T21" s="102" t="inlineStr">
+        <is>
+          <t>事務消耗品費</t>
+        </is>
+      </c>
+      <c r="U21" s="111" t="n">
+        <v>3300</v>
+      </c>
+      <c r="V21" s="111" t="n"/>
+      <c r="W21" s="111" t="n"/>
+      <c r="X21" s="111" t="n">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="22" ht="18" customHeight="1" s="115">
+      <c r="A22" s="97" t="n"/>
+      <c r="B22" s="47" t="n"/>
+      <c r="C22" s="98" t="n"/>
+      <c r="D22" s="99" t="n"/>
+      <c r="E22" s="55" t="n"/>
+      <c r="F22" s="99" t="n"/>
+      <c r="H22" s="52" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="I22" s="53" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="J22" s="51" t="n"/>
+      <c r="K22" s="54" t="n">
+        <v>600</v>
+      </c>
+      <c r="L22" s="55" t="n"/>
+      <c r="M22" s="56" t="n"/>
+      <c r="N22" s="57">
+        <f>IF(K22+L22+M22=0,"",K22+L22+M22)</f>
+        <v/>
+      </c>
+      <c r="O22" s="58" t="n"/>
+      <c r="P22" s="59">
+        <f>ROUNDDOWN($K22/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q22" s="60">
+        <f>ROUNDDOWN($L22/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R22" s="57">
+        <f>P22+Q22</f>
+        <v/>
+      </c>
+      <c r="T22" s="102" t="inlineStr">
+        <is>
+          <t>諸雑費</t>
+        </is>
+      </c>
+      <c r="U22" s="111" t="n">
+        <v>86634</v>
+      </c>
+      <c r="V22" s="111" t="n"/>
+      <c r="W22" s="111" t="n">
+        <v>30000</v>
+      </c>
+      <c r="X22" s="111" t="n">
+        <v>116634</v>
+      </c>
+    </row>
+    <row r="23" ht="18" customHeight="1" s="115">
+      <c r="A23" s="97" t="n"/>
+      <c r="B23" s="47" t="n"/>
+      <c r="C23" s="98" t="n"/>
+      <c r="D23" s="99" t="n"/>
+      <c r="E23" s="55" t="n"/>
+      <c r="F23" s="99" t="n"/>
+      <c r="H23" s="52" t="n"/>
+      <c r="I23" s="53" t="n"/>
+      <c r="J23" s="51" t="n"/>
+      <c r="K23" s="54" t="n"/>
+      <c r="L23" s="55" t="n"/>
+      <c r="M23" s="56" t="n"/>
+      <c r="N23" s="57">
+        <f>IF(K23+L23+M23=0,"",K23+L23+M23)</f>
+        <v/>
+      </c>
+      <c r="O23" s="58" t="n"/>
+      <c r="P23" s="59">
+        <f>ROUNDDOWN($K23/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q23" s="60">
+        <f>ROUNDDOWN($L23/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R23" s="57">
+        <f>P23+Q23</f>
+        <v/>
+      </c>
+      <c r="T23" s="102" t="inlineStr">
+        <is>
+          <t>水道光熱費</t>
+        </is>
+      </c>
+      <c r="U23" s="111" t="n">
+        <v>5571</v>
+      </c>
+      <c r="V23" s="111" t="n"/>
+      <c r="W23" s="111" t="n"/>
+      <c r="X23" s="111" t="n">
+        <v>5571</v>
+      </c>
+    </row>
+    <row r="24" ht="18" customHeight="1" s="115">
+      <c r="A24" s="97" t="n"/>
+      <c r="B24" s="47" t="n"/>
+      <c r="C24" s="98" t="n"/>
+      <c r="D24" s="99" t="n"/>
+      <c r="E24" s="55" t="n"/>
+      <c r="F24" s="99" t="n"/>
+      <c r="H24" s="52" t="n"/>
+      <c r="I24" s="53" t="n"/>
+      <c r="J24" s="51" t="n"/>
+      <c r="K24" s="54" t="n"/>
+      <c r="L24" s="55" t="n"/>
+      <c r="M24" s="56" t="n"/>
+      <c r="N24" s="57">
+        <f>IF(K24+L24+M24=0,"",K24+L24+M24)</f>
+        <v/>
+      </c>
+      <c r="O24" s="58" t="n"/>
+      <c r="P24" s="59">
+        <f>ROUNDDOWN($K24/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q24" s="60">
+        <f>ROUNDDOWN($L24/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R24" s="57">
+        <f>P24+Q24</f>
+        <v/>
+      </c>
+      <c r="T24" s="102" t="inlineStr">
+        <is>
+          <t>租税公課</t>
+        </is>
+      </c>
+      <c r="U24" s="111" t="n"/>
+      <c r="V24" s="111" t="n"/>
+      <c r="W24" s="111" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X24" s="111" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" ht="18" customHeight="1" s="115">
+      <c r="A25" s="97" t="n"/>
+      <c r="B25" s="47" t="n"/>
+      <c r="C25" s="98" t="n"/>
+      <c r="D25" s="99" t="n"/>
+      <c r="E25" s="55" t="n"/>
+      <c r="F25" s="99" t="n"/>
+      <c r="H25" s="52" t="n"/>
+      <c r="I25" s="53" t="n"/>
+      <c r="J25" s="51" t="n"/>
+      <c r="K25" s="54" t="n"/>
+      <c r="L25" s="55" t="n"/>
+      <c r="M25" s="56" t="n"/>
+      <c r="N25" s="57">
+        <f>IF(K25+L25+M25=0,"",K25+L25+M25)</f>
+        <v/>
+      </c>
+      <c r="O25" s="58" t="n"/>
+      <c r="P25" s="59">
+        <f>ROUNDDOWN($K25/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q25" s="60">
+        <f>ROUNDDOWN($L25/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R25" s="57">
+        <f>P25+Q25</f>
+        <v/>
+      </c>
+      <c r="T25" s="102" t="inlineStr">
+        <is>
+          <t>通信費</t>
+        </is>
+      </c>
+      <c r="U25" s="111" t="n">
+        <v>5210</v>
+      </c>
+      <c r="V25" s="111" t="n"/>
+      <c r="W25" s="111" t="n"/>
+      <c r="X25" s="111" t="n">
+        <v>5210</v>
+      </c>
+    </row>
+    <row r="26" ht="18" customHeight="1" s="115">
+      <c r="A26" s="97" t="n"/>
+      <c r="B26" s="47" t="n"/>
+      <c r="C26" s="98" t="n"/>
+      <c r="D26" s="99" t="n"/>
+      <c r="E26" s="55" t="n"/>
+      <c r="F26" s="99" t="n"/>
+      <c r="H26" s="52" t="n"/>
+      <c r="I26" s="53" t="n"/>
+      <c r="J26" s="51" t="n"/>
+      <c r="K26" s="54" t="n"/>
+      <c r="L26" s="55" t="n"/>
+      <c r="M26" s="56" t="n"/>
+      <c r="N26" s="57">
+        <f>IF(K26+L26+M26=0,"",K26+L26+M26)</f>
+        <v/>
+      </c>
+      <c r="O26" s="58" t="n"/>
+      <c r="P26" s="59">
+        <f>ROUNDDOWN($K26/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q26" s="60">
+        <f>ROUNDDOWN($L26/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R26" s="57">
+        <f>P26+Q26</f>
+        <v/>
+      </c>
+      <c r="T26" s="102" t="inlineStr">
+        <is>
+          <t>旅費交通費</t>
+        </is>
+      </c>
+      <c r="U26" s="111" t="n">
+        <v>158438</v>
+      </c>
+      <c r="V26" s="111" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W26" s="111" t="n"/>
+      <c r="X26" s="111" t="n">
+        <v>162447</v>
+      </c>
+    </row>
+    <row r="27" ht="18" customHeight="1" s="115">
+      <c r="A27" s="97" t="n"/>
+      <c r="B27" s="47" t="n"/>
+      <c r="C27" s="98" t="n"/>
+      <c r="D27" s="99" t="n"/>
+      <c r="E27" s="55" t="n"/>
+      <c r="F27" s="99" t="n"/>
+      <c r="H27" s="52" t="n"/>
+      <c r="I27" s="53" t="n"/>
+      <c r="J27" s="51" t="n"/>
+      <c r="K27" s="54" t="n"/>
+      <c r="L27" s="55" t="n"/>
+      <c r="M27" s="56" t="n"/>
+      <c r="N27" s="57">
+        <f>IF(K27+L27+M27=0,"",K27+L27+M27)</f>
+        <v/>
+      </c>
+      <c r="O27" s="58" t="n"/>
+      <c r="P27" s="59">
+        <f>ROUNDDOWN($K27/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q27" s="60">
+        <f>ROUNDDOWN($L27/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R27" s="57">
+        <f>P27+Q27</f>
+        <v/>
+      </c>
+      <c r="T27" s="107" t="inlineStr">
+        <is>
+          <t>総計</t>
+        </is>
+      </c>
+      <c r="U27" s="108" t="n">
+        <v>266329</v>
+      </c>
+      <c r="V27" s="108" t="n">
+        <v>4009</v>
+      </c>
+      <c r="W27" s="108" t="n">
+        <v>32000</v>
+      </c>
+      <c r="X27" s="108" t="n">
+        <v>302338</v>
+      </c>
+    </row>
+    <row r="28" ht="18" customHeight="1" s="115">
+      <c r="A28" s="97" t="n"/>
+      <c r="B28" s="47" t="n"/>
+      <c r="C28" s="98" t="n"/>
+      <c r="D28" s="99" t="n"/>
+      <c r="E28" s="55" t="n"/>
+      <c r="F28" s="99" t="n"/>
+      <c r="H28" s="52" t="n"/>
+      <c r="I28" s="53" t="n"/>
+      <c r="J28" s="51" t="n"/>
+      <c r="K28" s="54" t="n"/>
+      <c r="L28" s="55" t="n"/>
+      <c r="M28" s="56" t="n"/>
+      <c r="N28" s="57">
+        <f>IF(K28+L28+M28=0,"",K28+L28+M28)</f>
+        <v/>
+      </c>
+      <c r="O28" s="58" t="n"/>
+      <c r="P28" s="59">
+        <f>ROUNDDOWN($K28/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q28" s="60">
+        <f>ROUNDDOWN($L28/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R28" s="57">
+        <f>P28+Q28</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" ht="18" customHeight="1" s="115">
+      <c r="A29" s="97" t="n"/>
+      <c r="B29" s="47" t="n"/>
+      <c r="C29" s="98" t="n"/>
+      <c r="D29" s="99" t="n"/>
+      <c r="E29" s="55" t="n"/>
+      <c r="F29" s="99" t="n"/>
+      <c r="H29" s="52" t="n"/>
+      <c r="I29" s="53" t="n"/>
+      <c r="J29" s="51" t="n"/>
+      <c r="K29" s="54" t="n"/>
+      <c r="L29" s="55" t="n"/>
+      <c r="M29" s="56" t="n"/>
+      <c r="N29" s="57">
+        <f>IF(K29+L29+M29=0,"",K29+L29+M29)</f>
+        <v/>
+      </c>
+      <c r="O29" s="58" t="n"/>
+      <c r="P29" s="59">
+        <f>ROUNDDOWN($K29/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q29" s="60">
+        <f>ROUNDDOWN($L29/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R29" s="57">
+        <f>P29+Q29</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" ht="18" customHeight="1" s="115">
+      <c r="A30" s="97" t="n"/>
+      <c r="B30" s="47" t="n"/>
+      <c r="C30" s="98" t="n"/>
+      <c r="D30" s="99" t="n"/>
+      <c r="E30" s="55" t="n"/>
+      <c r="F30" s="99" t="n"/>
+      <c r="H30" s="52" t="n"/>
+      <c r="I30" s="53" t="n"/>
+      <c r="J30" s="51" t="n"/>
+      <c r="K30" s="54" t="n"/>
+      <c r="L30" s="55" t="n"/>
+      <c r="M30" s="56" t="n"/>
+      <c r="N30" s="57">
+        <f>IF(K30+L30+M30=0,"",K30+L30+M30)</f>
+        <v/>
+      </c>
+      <c r="O30" s="58" t="n"/>
+      <c r="P30" s="59">
+        <f>ROUNDDOWN($K30/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q30" s="60">
+        <f>ROUNDDOWN($L30/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R30" s="57">
+        <f>P30+Q30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" ht="18" customHeight="1" s="115">
+      <c r="A31" s="97" t="n"/>
+      <c r="B31" s="47" t="n"/>
+      <c r="C31" s="98" t="n"/>
+      <c r="D31" s="99" t="n"/>
+      <c r="E31" s="55" t="n"/>
+      <c r="F31" s="99" t="n"/>
+      <c r="H31" s="52" t="n"/>
+      <c r="I31" s="53" t="n"/>
+      <c r="J31" s="51" t="n"/>
+      <c r="K31" s="54" t="n"/>
+      <c r="L31" s="55" t="n"/>
+      <c r="M31" s="56" t="n"/>
+      <c r="N31" s="57">
+        <f>IF(K31+L31+M31=0,"",K31+L31+M31)</f>
+        <v/>
+      </c>
+      <c r="O31" s="58" t="n"/>
+      <c r="P31" s="59">
+        <f>ROUNDDOWN($K31/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q31" s="60">
+        <f>ROUNDDOWN($L31/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R31" s="57">
+        <f>P31+Q31</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" ht="18" customHeight="1" s="115">
+      <c r="A32" s="97" t="n"/>
+      <c r="B32" s="47" t="n"/>
+      <c r="C32" s="98" t="n"/>
+      <c r="D32" s="99" t="n"/>
+      <c r="E32" s="55" t="n"/>
+      <c r="F32" s="99" t="n"/>
+      <c r="H32" s="52" t="n"/>
+      <c r="I32" s="53" t="n"/>
+      <c r="J32" s="51" t="n"/>
+      <c r="K32" s="54" t="n"/>
+      <c r="L32" s="55" t="n"/>
+      <c r="M32" s="56" t="n"/>
+      <c r="N32" s="57">
+        <f>IF(K32+L32+M32=0,"",K32+L32+M32)</f>
+        <v/>
+      </c>
+      <c r="O32" s="58" t="n"/>
+      <c r="P32" s="59">
+        <f>ROUNDDOWN($K32/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q32" s="60">
+        <f>ROUNDDOWN($L32/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R32" s="57">
+        <f>P32+Q32</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" ht="18" customHeight="1" s="115">
+      <c r="A33" s="97" t="n"/>
+      <c r="B33" s="47" t="n"/>
+      <c r="C33" s="98" t="n"/>
+      <c r="D33" s="99" t="n"/>
+      <c r="E33" s="55" t="n"/>
+      <c r="F33" s="99" t="n"/>
+      <c r="H33" s="52" t="n"/>
+      <c r="I33" s="53" t="n"/>
+      <c r="J33" s="51" t="n"/>
+      <c r="K33" s="54" t="n"/>
+      <c r="L33" s="55" t="n"/>
+      <c r="M33" s="56" t="n"/>
+      <c r="N33" s="57">
+        <f>IF(K33+L33+M33=0,"",K33+L33+M33)</f>
+        <v/>
+      </c>
+      <c r="O33" s="58" t="n"/>
+      <c r="P33" s="59">
+        <f>ROUNDDOWN($K33/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q33" s="60">
+        <f>ROUNDDOWN($L33/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R33" s="57">
+        <f>P33+Q33</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" ht="18" customHeight="1" s="115">
+      <c r="A34" s="97" t="n"/>
+      <c r="B34" s="47" t="n"/>
+      <c r="C34" s="98" t="n"/>
+      <c r="D34" s="99" t="n"/>
+      <c r="E34" s="55" t="n"/>
+      <c r="F34" s="99" t="n"/>
+      <c r="H34" s="52" t="n"/>
+      <c r="I34" s="53" t="n"/>
+      <c r="J34" s="51" t="n"/>
+      <c r="K34" s="54" t="n"/>
+      <c r="L34" s="55" t="n"/>
+      <c r="M34" s="56" t="n"/>
+      <c r="N34" s="57">
+        <f>IF(K34+L34+M34=0,"",K34+L34+M34)</f>
+        <v/>
+      </c>
+      <c r="O34" s="58" t="n"/>
+      <c r="P34" s="59">
+        <f>ROUNDDOWN($K34/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q34" s="60">
+        <f>ROUNDDOWN($L34/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R34" s="57">
+        <f>P34+Q34</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="115">
+      <c r="A35" s="97" t="n"/>
+      <c r="B35" s="47" t="n"/>
+      <c r="C35" s="98" t="n"/>
+      <c r="D35" s="99" t="n"/>
+      <c r="E35" s="55" t="n"/>
+      <c r="F35" s="99" t="n"/>
+      <c r="H35" s="52" t="n"/>
+      <c r="I35" s="53" t="n"/>
+      <c r="J35" s="51" t="n"/>
+      <c r="K35" s="54" t="n"/>
+      <c r="L35" s="55" t="n"/>
+      <c r="M35" s="56" t="n"/>
+      <c r="N35" s="57">
+        <f>IF(K35+L35+M35=0,"",K35+L35+M35)</f>
+        <v/>
+      </c>
+      <c r="O35" s="58" t="n"/>
+      <c r="P35" s="59">
+        <f>ROUNDDOWN($K35/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q35" s="60">
+        <f>ROUNDDOWN($L35/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R35" s="57">
+        <f>P35+Q35</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" ht="18" customHeight="1" s="115">
+      <c r="A36" s="97" t="n"/>
+      <c r="B36" s="47" t="n"/>
+      <c r="C36" s="98" t="n"/>
+      <c r="D36" s="99" t="n"/>
+      <c r="E36" s="55" t="n"/>
+      <c r="F36" s="99" t="n"/>
+      <c r="H36" s="52" t="n"/>
+      <c r="I36" s="53" t="n"/>
+      <c r="J36" s="51" t="n"/>
+      <c r="K36" s="54" t="n"/>
+      <c r="L36" s="55" t="n"/>
+      <c r="M36" s="56" t="n"/>
+      <c r="N36" s="57">
+        <f>IF(K36+L36+M36=0,"",K36+L36+M36)</f>
+        <v/>
+      </c>
+      <c r="O36" s="58" t="n"/>
+      <c r="P36" s="59">
+        <f>ROUNDDOWN($K36/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q36" s="60">
+        <f>ROUNDDOWN($L36/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R36" s="57">
+        <f>P36+Q36</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" ht="18" customHeight="1" s="115">
+      <c r="A37" s="97" t="n"/>
+      <c r="B37" s="47" t="n"/>
+      <c r="C37" s="98" t="n"/>
+      <c r="D37" s="99" t="n"/>
+      <c r="E37" s="55" t="n"/>
+      <c r="F37" s="99" t="n"/>
+      <c r="H37" s="52" t="n"/>
+      <c r="I37" s="53" t="n"/>
+      <c r="J37" s="51" t="n"/>
+      <c r="K37" s="54" t="n"/>
+      <c r="L37" s="55" t="n"/>
+      <c r="M37" s="56" t="n"/>
+      <c r="N37" s="57">
+        <f>IF(K37+L37+M37=0,"",K37+L37+M37)</f>
+        <v/>
+      </c>
+      <c r="O37" s="58" t="n"/>
+      <c r="P37" s="59">
+        <f>ROUNDDOWN($K37/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q37" s="60">
+        <f>ROUNDDOWN($L37/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R37" s="57">
+        <f>P37+Q37</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" ht="18" customHeight="1" s="115">
+      <c r="A38" s="61" t="n"/>
+      <c r="B38" s="62" t="n"/>
+      <c r="C38" s="63" t="n"/>
+      <c r="D38" s="64" t="n"/>
+      <c r="E38" s="65" t="n"/>
+      <c r="F38" s="64" t="n"/>
+      <c r="H38" s="66" t="n"/>
+      <c r="I38" s="67" t="n"/>
+      <c r="J38" s="51" t="n"/>
+      <c r="K38" s="68" t="n"/>
+      <c r="L38" s="65" t="n"/>
+      <c r="M38" s="69" t="n"/>
+      <c r="N38" s="70">
+        <f>IF(K38+L38+M38=0,"",K38+L38+M38)</f>
+        <v/>
+      </c>
+      <c r="O38" s="58" t="n"/>
+      <c r="P38" s="71">
+        <f>ROUNDDOWN($K38/110*10,0)</f>
+        <v/>
+      </c>
+      <c r="Q38" s="72">
+        <f>ROUNDDOWN($L38/108*8,0)</f>
+        <v/>
+      </c>
+      <c r="R38" s="70">
+        <f>P38+Q38</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" ht="18" customHeight="1" s="115">
+      <c r="A39" s="73" t="n"/>
+      <c r="B39" s="73" t="n"/>
+      <c r="C39" s="74" t="n"/>
+      <c r="D39" s="75" t="inlineStr">
+        <is>
+          <t>合計</t>
+        </is>
+      </c>
+      <c r="E39" s="76">
+        <f>SUM(E5:E38)</f>
+        <v/>
+      </c>
+      <c r="F39" s="77">
+        <f>SUM(F6:F38)</f>
+        <v/>
+      </c>
+      <c r="H39" s="73" t="n"/>
+      <c r="I39" s="73" t="n"/>
+      <c r="K39" s="78">
+        <f>SUM(K6:K38)</f>
+        <v/>
+      </c>
+      <c r="L39" s="79">
+        <f>SUM(L6:L38)</f>
+        <v/>
+      </c>
+      <c r="M39" s="80">
+        <f>SUM(M6:M38)</f>
+        <v/>
+      </c>
+      <c r="N39" s="81">
+        <f>SUM(N6:N38)</f>
+        <v/>
+      </c>
+      <c r="O39" s="58" t="n"/>
+      <c r="P39" s="82">
+        <f>SUM(P6:P38)</f>
+        <v/>
+      </c>
+      <c r="Q39" s="83">
+        <f>SUM(Q6:Q38)</f>
+        <v/>
+      </c>
+      <c r="R39" s="81">
+        <f>SUM(R6:R38)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" ht="18" customHeight="1" s="115">
+      <c r="C40" s="84" t="n"/>
+      <c r="D40" s="85" t="inlineStr">
+        <is>
+          <t>残高</t>
+        </is>
+      </c>
+      <c r="E40" s="127">
+        <f>E39-F39</f>
+        <v/>
+      </c>
+      <c r="F40" s="128" t="n"/>
+      <c r="K40" s="45" t="n"/>
+      <c r="L40" s="45" t="n"/>
+      <c r="M40" s="45" t="n"/>
+      <c r="N40" s="45" t="n"/>
+      <c r="O40" s="45" t="n"/>
+      <c r="P40" s="45" t="n"/>
+      <c r="Q40" s="45" t="n"/>
+      <c r="R40" s="45" t="n"/>
+    </row>
+    <row r="41" ht="18" customHeight="1" s="115">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-07-02</t>
+          <t>2024-12-10</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>郡山桑野食堂</t>
+          <t>Uny OiI</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Ava Thompson</t>
+          <t>Lucas Bennett</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>2848</v>
+        <v>5000</v>
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>6543456543</t>
+          <t>T2180001091960</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="L41" t="n">
         <v>0</v>
       </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="n">
-        <v>2848</v>
+        <v>5000</v>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
       <c r="R41" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" ht="18" customHeight="1" s="115"/>

</xml_diff>

<commit_message>
Big Update - Full deployment Phase 5A
</commit_message>
<xml_diff>
--- a/app/Data/accumulation/Aichi_Accumulated.xlsx
+++ b/app/Data/accumulation/Aichi_Accumulated.xlsx
@@ -1,34 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="記入例" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="English ver 記入例" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年1月" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="追加1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年2月" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年3月" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年4月" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年5月" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年6月" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年7月" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年8月" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年9月" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年10月" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年11月" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年12月" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="集計ﾃｰﾌﾞﾙ" sheetId="16" state="hidden" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024年11月" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025年07月" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024年12月" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="記入例" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="English ver 記入例" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2025年1月" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="追加1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2025年2月" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2025年3月" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="2025年4月" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2025年5月" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="2025年6月" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2025年7月" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2025年8月" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="2025年9月" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="2025年10月" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="2025年11月" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="2025年12月" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="集計ﾃｰﾌﾞﾙ" sheetId="16" state="hidden" r:id="rId16"/>
+    <sheet name="2024年11月" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="2025年07月" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="2024年12月" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_4" localSheetId="3">'追加1'!$A$1:$H$39</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="0" r:id="rId20"/>
+    <pivotCache cacheId="0" r:id="rId20"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -18515,7 +18515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X45"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18728,7 +18728,7 @@
       </c>
       <c r="U5" s="100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -19525,7 +19525,7 @@
       </c>
       <c r="U17" s="104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="V17" s="104" t="n"/>
@@ -20739,8 +20739,106 @@
         <v>250</v>
       </c>
     </row>
-    <row r="46" ht="18" customHeight="1" s="115"/>
-    <row r="47" ht="18" customHeight="1" s="115"/>
+    <row r="46" ht="18" customHeight="1" s="115">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>2024-11-20</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr"/>
+      <c r="C46" s="0" t="inlineStr">
+        <is>
+          <t>Test Vendor 株式会社</t>
+        </is>
+      </c>
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>Ethan Cole</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr"/>
+      <c r="F46" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G46" s="0" t="inlineStr"/>
+      <c r="H46" s="0" t="inlineStr">
+        <is>
+          <t>TEST-INVOICE-1768717972</t>
+        </is>
+      </c>
+      <c r="I46" s="0" t="inlineStr"/>
+      <c r="J46" s="0" t="inlineStr"/>
+      <c r="K46" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="L46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" s="0" t="inlineStr"/>
+      <c r="N46" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="O46" s="0" t="inlineStr"/>
+      <c r="P46" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="Q46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R46" s="0" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="47" ht="18" customHeight="1" s="115">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-11-20</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Test Vendor 株式会社</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Ethan Cole</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>TEST-INVOICE-1768717972</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="n">
+        <v>1234</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="n">
+        <v>12345</v>
+      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="n">
+        <v>1234</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0</v>
+      </c>
+      <c r="R47" t="n">
+        <v>1234</v>
+      </c>
+    </row>
     <row r="48" ht="18" customHeight="1" s="115"/>
     <row r="49" ht="18" customHeight="1" s="115"/>
     <row r="50" ht="18" customHeight="1" s="115"/>
@@ -21927,7 +22025,7 @@
       </c>
       <c r="U5" s="100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -22724,7 +22822,7 @@
       </c>
       <c r="U17" s="104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="V17" s="104" t="n"/>
@@ -24942,7 +25040,7 @@
       </c>
       <c r="U5" s="100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -25739,7 +25837,7 @@
       </c>
       <c r="U17" s="104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="V17" s="104" t="n"/>
@@ -26716,52 +26814,52 @@
       <c r="R40" s="45" t="n"/>
     </row>
     <row r="41" ht="18" customHeight="1" s="115">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="0" t="inlineStr">
         <is>
           <t>2024-12-10</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr"/>
+      <c r="C41" s="0" t="inlineStr">
         <is>
           <t>Uny OiI</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D41" s="0" t="inlineStr">
         <is>
           <t>Lucas Bennett</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="n">
+      <c r="E41" s="0" t="inlineStr"/>
+      <c r="F41" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr">
+      <c r="G41" s="0" t="inlineStr"/>
+      <c r="H41" s="0" t="inlineStr">
         <is>
           <t>T2180001091960</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="n">
+      <c r="I41" s="0" t="inlineStr"/>
+      <c r="J41" s="0" t="inlineStr"/>
+      <c r="K41" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="L41" t="n">
+      <c r="L41" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="n">
+      <c r="M41" s="0" t="inlineStr"/>
+      <c r="N41" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="n">
+      <c r="O41" s="0" t="inlineStr"/>
+      <c r="P41" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="Q41" t="n">
+      <c r="Q41" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R41" t="n">
+      <c r="R41" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -30311,7 +30409,7 @@
       </c>
       <c r="U5" s="100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -31108,7 +31206,7 @@
       </c>
       <c r="U17" s="104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t> </t>
         </is>
       </c>
       <c r="V17" s="104" t="n"/>

</xml_diff>